<commit_message>
Adding depends_on to necessary resources for order
</commit_message>
<xml_diff>
--- a/deploy-fabric-Input-Spreadsheet.xlsx
+++ b/deploy-fabric-Input-Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\tyscott\terraform-aci-fabric-deploy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19403AC3-7ED5-4036-8822-6EFA92819F76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9134FD90-DD6A-4B09-8B06-C6493386A1C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2010,103 +2010,103 @@
     <xf numFmtId="164" fontId="19" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="17" fillId="33" borderId="8" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="25" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="26" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="20" fillId="34" borderId="22" xfId="43" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="34" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="34" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="34" borderId="22" xfId="43" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="34" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="33" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="34" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="34" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="34" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="18" fillId="34" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="23" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="24" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="34" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="34" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="28" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="34" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="18" fillId="34" borderId="29" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="33" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="34" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="23" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="24" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="33" borderId="8" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="28" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="17" fillId="36" borderId="8" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="19" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="19" fillId="34" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="19" fillId="34" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="25" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="26" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="20" fillId="34" borderId="22" xfId="43" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="19" fillId="34" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="19" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="19" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="34" borderId="22" xfId="43" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2494,21 +2494,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
     </row>
     <row r="2" spans="1:16" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -2549,41 +2549,41 @@
       <c r="M3" s="13"/>
     </row>
     <row r="5" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="42" t="s">
         <v>202</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
-      <c r="M5" s="31"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="42"/>
+      <c r="L5" s="42"/>
+      <c r="M5" s="42"/>
       <c r="N5" s="22"/>
       <c r="O5" s="22"/>
       <c r="P5" s="22"/>
     </row>
     <row r="6" spans="1:16" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="20"/>
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="58" t="s">
         <v>238</v>
       </c>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
-      <c r="J6" s="40"/>
-      <c r="K6" s="40"/>
-      <c r="L6" s="40"/>
-      <c r="M6" s="40"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="58"/>
+      <c r="K6" s="58"/>
+      <c r="L6" s="58"/>
+      <c r="M6" s="58"/>
       <c r="N6" s="20"/>
       <c r="O6" s="20"/>
       <c r="P6" s="20"/>
@@ -2628,11 +2628,11 @@
       <c r="M7" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="N7" s="33" t="s">
+      <c r="N7" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="O7" s="34"/>
-      <c r="P7" s="35"/>
+      <c r="O7" s="54"/>
+      <c r="P7" s="55"/>
     </row>
     <row r="8" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
@@ -2672,43 +2672,43 @@
         <v>48</v>
       </c>
       <c r="M8" s="27"/>
-      <c r="N8" s="36"/>
-      <c r="O8" s="37"/>
-      <c r="P8" s="38"/>
+      <c r="N8" s="56"/>
+      <c r="O8" s="57"/>
+      <c r="P8" s="41"/>
     </row>
     <row r="10" spans="1:16" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="B10" s="39"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="39"/>
-      <c r="K10" s="39"/>
-      <c r="L10" s="39"/>
-      <c r="M10" s="39"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
     </row>
     <row r="11" spans="1:16" s="6" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="21"/>
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="51" t="s">
         <v>225</v>
       </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
-      <c r="J11" s="41"/>
-      <c r="K11" s="41"/>
-      <c r="L11" s="41"/>
-      <c r="M11" s="41"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="51"/>
+      <c r="K11" s="51"/>
+      <c r="L11" s="51"/>
+      <c r="M11" s="51"/>
     </row>
     <row r="12" spans="1:16" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
@@ -3032,38 +3032,38 @@
       <c r="M26" s="11"/>
     </row>
     <row r="28" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="39" t="s">
+      <c r="A28" s="29" t="s">
         <v>243</v>
       </c>
-      <c r="B28" s="39"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="39"/>
-      <c r="J28" s="39"/>
-      <c r="K28" s="39"/>
-      <c r="L28" s="39"/>
-      <c r="M28" s="39"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
+      <c r="K28" s="29"/>
+      <c r="L28" s="29"/>
+      <c r="M28" s="29"/>
     </row>
     <row r="29" spans="1:13" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="21"/>
-      <c r="B29" s="41" t="s">
+      <c r="B29" s="51" t="s">
         <v>244</v>
       </c>
-      <c r="C29" s="41"/>
-      <c r="D29" s="41"/>
-      <c r="E29" s="41"/>
-      <c r="F29" s="41"/>
-      <c r="G29" s="41"/>
-      <c r="H29" s="41"/>
-      <c r="I29" s="41"/>
-      <c r="J29" s="41"/>
-      <c r="K29" s="41"/>
-      <c r="L29" s="41"/>
-      <c r="M29" s="41"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="51"/>
+      <c r="G29" s="51"/>
+      <c r="H29" s="51"/>
+      <c r="I29" s="51"/>
+      <c r="J29" s="51"/>
+      <c r="K29" s="51"/>
+      <c r="L29" s="51"/>
+      <c r="M29" s="51"/>
     </row>
     <row r="30" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
@@ -3206,38 +3206,38 @@
       <c r="M37" s="13"/>
     </row>
     <row r="39" spans="1:13" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="39" t="s">
+      <c r="A39" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="B39" s="39"/>
-      <c r="C39" s="39"/>
-      <c r="D39" s="39"/>
-      <c r="E39" s="39"/>
-      <c r="F39" s="39"/>
-      <c r="G39" s="39"/>
-      <c r="H39" s="39"/>
-      <c r="I39" s="39"/>
-      <c r="J39" s="39"/>
-      <c r="K39" s="39"/>
-      <c r="L39" s="39"/>
-      <c r="M39" s="39"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="29"/>
+      <c r="E39" s="29"/>
+      <c r="F39" s="29"/>
+      <c r="G39" s="29"/>
+      <c r="H39" s="29"/>
+      <c r="I39" s="29"/>
+      <c r="J39" s="29"/>
+      <c r="K39" s="29"/>
+      <c r="L39" s="29"/>
+      <c r="M39" s="29"/>
     </row>
     <row r="40" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="23"/>
-      <c r="B40" s="29" t="s">
+      <c r="B40" s="52" t="s">
         <v>226</v>
       </c>
-      <c r="C40" s="29"/>
-      <c r="D40" s="29"/>
-      <c r="E40" s="29"/>
-      <c r="F40" s="29"/>
-      <c r="G40" s="29"/>
-      <c r="H40" s="29"/>
-      <c r="I40" s="29"/>
-      <c r="J40" s="29"/>
-      <c r="K40" s="29"/>
-      <c r="L40" s="29"/>
-      <c r="M40" s="29"/>
+      <c r="C40" s="52"/>
+      <c r="D40" s="52"/>
+      <c r="E40" s="52"/>
+      <c r="F40" s="52"/>
+      <c r="G40" s="52"/>
+      <c r="H40" s="52"/>
+      <c r="I40" s="52"/>
+      <c r="J40" s="52"/>
+      <c r="K40" s="52"/>
+      <c r="L40" s="52"/>
+      <c r="M40" s="52"/>
     </row>
     <row r="41" spans="1:13" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="8" t="s">
@@ -3400,21 +3400,21 @@
       <c r="M48" s="13"/>
     </row>
     <row r="50" spans="1:13" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="39" t="s">
+      <c r="A50" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="B50" s="39"/>
-      <c r="C50" s="39"/>
-      <c r="D50" s="39"/>
-      <c r="E50" s="39"/>
-      <c r="F50" s="39"/>
-      <c r="G50" s="39"/>
-      <c r="H50" s="39"/>
-      <c r="I50" s="39"/>
-      <c r="J50" s="39"/>
-      <c r="K50" s="39"/>
-      <c r="L50" s="39"/>
-      <c r="M50" s="39"/>
+      <c r="B50" s="29"/>
+      <c r="C50" s="29"/>
+      <c r="D50" s="29"/>
+      <c r="E50" s="29"/>
+      <c r="F50" s="29"/>
+      <c r="G50" s="29"/>
+      <c r="H50" s="29"/>
+      <c r="I50" s="29"/>
+      <c r="J50" s="29"/>
+      <c r="K50" s="29"/>
+      <c r="L50" s="29"/>
+      <c r="M50" s="29"/>
     </row>
     <row r="51" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="8" t="s">
@@ -3455,38 +3455,38 @@
       <c r="M52" s="13"/>
     </row>
     <row r="54" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="39" t="s">
+      <c r="A54" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="B54" s="39"/>
-      <c r="C54" s="39"/>
-      <c r="D54" s="39"/>
-      <c r="E54" s="39"/>
-      <c r="F54" s="39"/>
-      <c r="G54" s="39"/>
-      <c r="H54" s="39"/>
-      <c r="I54" s="39"/>
-      <c r="J54" s="39"/>
-      <c r="K54" s="39"/>
-      <c r="L54" s="39"/>
-      <c r="M54" s="39"/>
+      <c r="B54" s="29"/>
+      <c r="C54" s="29"/>
+      <c r="D54" s="29"/>
+      <c r="E54" s="29"/>
+      <c r="F54" s="29"/>
+      <c r="G54" s="29"/>
+      <c r="H54" s="29"/>
+      <c r="I54" s="29"/>
+      <c r="J54" s="29"/>
+      <c r="K54" s="29"/>
+      <c r="L54" s="29"/>
+      <c r="M54" s="29"/>
     </row>
     <row r="55" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="23"/>
-      <c r="B55" s="29" t="s">
+      <c r="B55" s="52" t="s">
         <v>227</v>
       </c>
-      <c r="C55" s="29"/>
-      <c r="D55" s="29"/>
-      <c r="E55" s="29"/>
-      <c r="F55" s="29"/>
-      <c r="G55" s="29"/>
-      <c r="H55" s="29"/>
-      <c r="I55" s="29"/>
-      <c r="J55" s="29"/>
-      <c r="K55" s="29"/>
-      <c r="L55" s="29"/>
-      <c r="M55" s="29"/>
+      <c r="C55" s="52"/>
+      <c r="D55" s="52"/>
+      <c r="E55" s="52"/>
+      <c r="F55" s="52"/>
+      <c r="G55" s="52"/>
+      <c r="H55" s="52"/>
+      <c r="I55" s="52"/>
+      <c r="J55" s="52"/>
+      <c r="K55" s="52"/>
+      <c r="L55" s="52"/>
+      <c r="M55" s="52"/>
     </row>
     <row r="56" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="8" t="s">
@@ -3546,21 +3546,21 @@
       <c r="M58" s="11"/>
     </row>
     <row r="60" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="39" t="s">
+      <c r="A60" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="B60" s="39"/>
-      <c r="C60" s="39"/>
-      <c r="D60" s="39"/>
-      <c r="E60" s="39"/>
-      <c r="F60" s="39"/>
-      <c r="G60" s="39"/>
-      <c r="H60" s="39"/>
-      <c r="I60" s="39"/>
-      <c r="J60" s="39"/>
-      <c r="K60" s="39"/>
-      <c r="L60" s="39"/>
-      <c r="M60" s="39"/>
+      <c r="B60" s="29"/>
+      <c r="C60" s="29"/>
+      <c r="D60" s="29"/>
+      <c r="E60" s="29"/>
+      <c r="F60" s="29"/>
+      <c r="G60" s="29"/>
+      <c r="H60" s="29"/>
+      <c r="I60" s="29"/>
+      <c r="J60" s="29"/>
+      <c r="K60" s="29"/>
+      <c r="L60" s="29"/>
+      <c r="M60" s="29"/>
     </row>
     <row r="61" spans="1:13" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="8" t="s">
@@ -3601,38 +3601,38 @@
       <c r="M62" s="13"/>
     </row>
     <row r="64" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="39" t="s">
+      <c r="A64" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="B64" s="39"/>
-      <c r="C64" s="39"/>
-      <c r="D64" s="39"/>
-      <c r="E64" s="39"/>
-      <c r="F64" s="39"/>
-      <c r="G64" s="39"/>
-      <c r="H64" s="39"/>
-      <c r="I64" s="39"/>
-      <c r="J64" s="39"/>
-      <c r="K64" s="39"/>
-      <c r="L64" s="39"/>
-      <c r="M64" s="39"/>
+      <c r="B64" s="29"/>
+      <c r="C64" s="29"/>
+      <c r="D64" s="29"/>
+      <c r="E64" s="29"/>
+      <c r="F64" s="29"/>
+      <c r="G64" s="29"/>
+      <c r="H64" s="29"/>
+      <c r="I64" s="29"/>
+      <c r="J64" s="29"/>
+      <c r="K64" s="29"/>
+      <c r="L64" s="29"/>
+      <c r="M64" s="29"/>
     </row>
     <row r="65" spans="1:16" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="23"/>
-      <c r="B65" s="29" t="s">
+      <c r="B65" s="52" t="s">
         <v>228</v>
       </c>
-      <c r="C65" s="29"/>
-      <c r="D65" s="29"/>
-      <c r="E65" s="29"/>
-      <c r="F65" s="29"/>
-      <c r="G65" s="29"/>
-      <c r="H65" s="29"/>
-      <c r="I65" s="29"/>
-      <c r="J65" s="29"/>
-      <c r="K65" s="29"/>
-      <c r="L65" s="29"/>
-      <c r="M65" s="29"/>
+      <c r="C65" s="52"/>
+      <c r="D65" s="52"/>
+      <c r="E65" s="52"/>
+      <c r="F65" s="52"/>
+      <c r="G65" s="52"/>
+      <c r="H65" s="52"/>
+      <c r="I65" s="52"/>
+      <c r="J65" s="52"/>
+      <c r="K65" s="52"/>
+      <c r="L65" s="52"/>
+      <c r="M65" s="52"/>
     </row>
     <row r="66" spans="1:16" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="8" t="s">
@@ -3698,41 +3698,41 @@
       <c r="M68" s="11"/>
     </row>
     <row r="70" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="31" t="s">
+      <c r="A70" s="42" t="s">
         <v>120</v>
       </c>
-      <c r="B70" s="31"/>
-      <c r="C70" s="31"/>
-      <c r="D70" s="31"/>
-      <c r="E70" s="31"/>
-      <c r="F70" s="31"/>
-      <c r="G70" s="31"/>
-      <c r="H70" s="31"/>
-      <c r="I70" s="31"/>
-      <c r="J70" s="31"/>
-      <c r="K70" s="31"/>
-      <c r="L70" s="31"/>
-      <c r="M70" s="31"/>
+      <c r="B70" s="42"/>
+      <c r="C70" s="42"/>
+      <c r="D70" s="42"/>
+      <c r="E70" s="42"/>
+      <c r="F70" s="42"/>
+      <c r="G70" s="42"/>
+      <c r="H70" s="42"/>
+      <c r="I70" s="42"/>
+      <c r="J70" s="42"/>
+      <c r="K70" s="42"/>
+      <c r="L70" s="42"/>
+      <c r="M70" s="42"/>
       <c r="N70" s="24"/>
       <c r="O70" s="24"/>
       <c r="P70" s="24"/>
     </row>
     <row r="71" spans="1:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="25"/>
-      <c r="B71" s="32" t="s">
+      <c r="B71" s="59" t="s">
         <v>229</v>
       </c>
-      <c r="C71" s="32"/>
-      <c r="D71" s="32"/>
-      <c r="E71" s="32"/>
-      <c r="F71" s="32"/>
-      <c r="G71" s="32"/>
-      <c r="H71" s="32"/>
-      <c r="I71" s="32"/>
-      <c r="J71" s="32"/>
-      <c r="K71" s="32"/>
-      <c r="L71" s="32"/>
-      <c r="M71" s="32"/>
+      <c r="C71" s="59"/>
+      <c r="D71" s="59"/>
+      <c r="E71" s="59"/>
+      <c r="F71" s="59"/>
+      <c r="G71" s="59"/>
+      <c r="H71" s="59"/>
+      <c r="I71" s="59"/>
+      <c r="J71" s="59"/>
+      <c r="K71" s="59"/>
+      <c r="L71" s="59"/>
+      <c r="M71" s="59"/>
       <c r="N71" s="25"/>
       <c r="O71" s="25"/>
       <c r="P71" s="25"/>
@@ -3750,18 +3750,18 @@
       <c r="D72" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="E72" s="52" t="s">
+      <c r="E72" s="32" t="s">
         <v>131</v>
       </c>
-      <c r="F72" s="53"/>
-      <c r="G72" s="52" t="s">
+      <c r="F72" s="33"/>
+      <c r="G72" s="32" t="s">
         <v>132</v>
       </c>
-      <c r="H72" s="53"/>
-      <c r="I72" s="52" t="s">
+      <c r="H72" s="33"/>
+      <c r="I72" s="32" t="s">
         <v>133</v>
       </c>
-      <c r="J72" s="53"/>
+      <c r="J72" s="33"/>
       <c r="K72" s="8" t="s">
         <v>134</v>
       </c>
@@ -3794,18 +3794,18 @@
       <c r="D73" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E73" s="61" t="s">
+      <c r="E73" s="40" t="s">
         <v>183</v>
       </c>
-      <c r="F73" s="38"/>
-      <c r="G73" s="54" t="s">
+      <c r="F73" s="41"/>
+      <c r="G73" s="34" t="s">
         <v>184</v>
       </c>
-      <c r="H73" s="55"/>
-      <c r="I73" s="54" t="s">
+      <c r="H73" s="35"/>
+      <c r="I73" s="34" t="s">
         <v>184</v>
       </c>
-      <c r="J73" s="55"/>
+      <c r="J73" s="35"/>
       <c r="K73" s="13" t="s">
         <v>185</v>
       </c>
@@ -3827,21 +3827,21 @@
     </row>
     <row r="74" spans="1:16" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="75" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="39" t="s">
+      <c r="A75" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="B75" s="39"/>
-      <c r="C75" s="39"/>
-      <c r="D75" s="39"/>
-      <c r="E75" s="39"/>
-      <c r="F75" s="39"/>
-      <c r="G75" s="39"/>
-      <c r="H75" s="39"/>
-      <c r="I75" s="39"/>
-      <c r="J75" s="39"/>
-      <c r="K75" s="39"/>
-      <c r="L75" s="39"/>
-      <c r="M75" s="39"/>
+      <c r="B75" s="29"/>
+      <c r="C75" s="29"/>
+      <c r="D75" s="29"/>
+      <c r="E75" s="29"/>
+      <c r="F75" s="29"/>
+      <c r="G75" s="29"/>
+      <c r="H75" s="29"/>
+      <c r="I75" s="29"/>
+      <c r="J75" s="29"/>
+      <c r="K75" s="29"/>
+      <c r="L75" s="29"/>
+      <c r="M75" s="29"/>
     </row>
     <row r="76" spans="1:16" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="8" t="s">
@@ -3913,34 +3913,34 @@
       <c r="M78" s="11"/>
     </row>
     <row r="80" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="39" t="s">
+      <c r="A80" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="B80" s="39"/>
-      <c r="C80" s="39"/>
-      <c r="D80" s="39"/>
-      <c r="E80" s="39"/>
-      <c r="F80" s="39"/>
-      <c r="G80" s="39"/>
-      <c r="H80" s="39"/>
-      <c r="I80" s="39"/>
-      <c r="J80" s="39"/>
-      <c r="K80" s="39"/>
-      <c r="L80" s="39"/>
-      <c r="M80" s="39"/>
+      <c r="B80" s="29"/>
+      <c r="C80" s="29"/>
+      <c r="D80" s="29"/>
+      <c r="E80" s="29"/>
+      <c r="F80" s="29"/>
+      <c r="G80" s="29"/>
+      <c r="H80" s="29"/>
+      <c r="I80" s="29"/>
+      <c r="J80" s="29"/>
+      <c r="K80" s="29"/>
+      <c r="L80" s="29"/>
+      <c r="M80" s="29"/>
     </row>
     <row r="81" spans="1:13" s="3" customFormat="1" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B81" s="42" t="s">
+      <c r="B81" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="C81" s="43"/>
-      <c r="D81" s="42" t="s">
+      <c r="C81" s="45"/>
+      <c r="D81" s="43" t="s">
         <v>125</v>
       </c>
-      <c r="E81" s="43"/>
+      <c r="E81" s="45"/>
       <c r="F81" s="8"/>
       <c r="G81" s="8"/>
       <c r="H81" s="8"/>
@@ -3954,14 +3954,14 @@
       <c r="A82" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B82" s="44" t="s">
+      <c r="B82" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="C82" s="45"/>
-      <c r="D82" s="48" t="s">
+      <c r="C82" s="49"/>
+      <c r="D82" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="E82" s="50"/>
+      <c r="E82" s="37"/>
       <c r="F82" s="13"/>
       <c r="G82" s="14"/>
       <c r="H82" s="14"/>
@@ -3975,14 +3975,14 @@
       <c r="A83" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B83" s="56" t="s">
+      <c r="B83" s="30" t="s">
         <v>128</v>
       </c>
-      <c r="C83" s="58"/>
-      <c r="D83" s="59" t="s">
+      <c r="C83" s="31"/>
+      <c r="D83" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="E83" s="60"/>
+      <c r="E83" s="39"/>
       <c r="F83" s="11"/>
       <c r="G83" s="12"/>
       <c r="H83" s="12"/>
@@ -3993,21 +3993,21 @@
       <c r="M83" s="11"/>
     </row>
     <row r="85" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="39" t="s">
+      <c r="A85" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B85" s="39"/>
-      <c r="C85" s="39"/>
-      <c r="D85" s="39"/>
-      <c r="E85" s="39"/>
-      <c r="F85" s="39"/>
-      <c r="G85" s="39"/>
-      <c r="H85" s="39"/>
-      <c r="I85" s="39"/>
-      <c r="J85" s="39"/>
-      <c r="K85" s="39"/>
-      <c r="L85" s="39"/>
-      <c r="M85" s="39"/>
+      <c r="B85" s="29"/>
+      <c r="C85" s="29"/>
+      <c r="D85" s="29"/>
+      <c r="E85" s="29"/>
+      <c r="F85" s="29"/>
+      <c r="G85" s="29"/>
+      <c r="H85" s="29"/>
+      <c r="I85" s="29"/>
+      <c r="J85" s="29"/>
+      <c r="K85" s="29"/>
+      <c r="L85" s="29"/>
+      <c r="M85" s="29"/>
     </row>
     <row r="86" spans="1:13" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="8" t="s">
@@ -4079,35 +4079,35 @@
       <c r="M88" s="11"/>
     </row>
     <row r="90" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="39" t="s">
+      <c r="A90" s="29" t="s">
         <v>147</v>
       </c>
-      <c r="B90" s="39"/>
-      <c r="C90" s="39"/>
-      <c r="D90" s="39"/>
-      <c r="E90" s="39"/>
-      <c r="F90" s="39"/>
-      <c r="G90" s="39"/>
-      <c r="H90" s="39"/>
-      <c r="I90" s="39"/>
-      <c r="J90" s="39"/>
-      <c r="K90" s="39"/>
-      <c r="L90" s="39"/>
-      <c r="M90" s="39"/>
+      <c r="B90" s="29"/>
+      <c r="C90" s="29"/>
+      <c r="D90" s="29"/>
+      <c r="E90" s="29"/>
+      <c r="F90" s="29"/>
+      <c r="G90" s="29"/>
+      <c r="H90" s="29"/>
+      <c r="I90" s="29"/>
+      <c r="J90" s="29"/>
+      <c r="K90" s="29"/>
+      <c r="L90" s="29"/>
+      <c r="M90" s="29"/>
     </row>
     <row r="91" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B91" s="47" t="s">
+      <c r="B91" s="44" t="s">
         <v>145</v>
       </c>
-      <c r="C91" s="47"/>
-      <c r="D91" s="42" t="s">
+      <c r="C91" s="44"/>
+      <c r="D91" s="43" t="s">
         <v>146</v>
       </c>
-      <c r="E91" s="47"/>
-      <c r="F91" s="43"/>
+      <c r="E91" s="44"/>
+      <c r="F91" s="45"/>
       <c r="G91" s="8"/>
       <c r="H91" s="8"/>
       <c r="I91" s="8"/>
@@ -4120,15 +4120,15 @@
       <c r="A92" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B92" s="44" t="s">
+      <c r="B92" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="C92" s="45"/>
-      <c r="D92" s="48" t="s">
+      <c r="C92" s="49"/>
+      <c r="D92" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="E92" s="49"/>
-      <c r="F92" s="50"/>
+      <c r="E92" s="46"/>
+      <c r="F92" s="37"/>
       <c r="G92" s="14"/>
       <c r="H92" s="14"/>
       <c r="I92" s="13"/>
@@ -4141,38 +4141,38 @@
       <c r="B93" s="7"/>
     </row>
     <row r="94" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="39" t="s">
+      <c r="A94" s="29" t="s">
         <v>140</v>
       </c>
-      <c r="B94" s="39"/>
-      <c r="C94" s="39"/>
-      <c r="D94" s="39"/>
-      <c r="E94" s="39"/>
-      <c r="F94" s="39"/>
-      <c r="G94" s="39"/>
-      <c r="H94" s="39"/>
-      <c r="I94" s="39"/>
-      <c r="J94" s="39"/>
-      <c r="K94" s="39"/>
-      <c r="L94" s="39"/>
-      <c r="M94" s="39"/>
+      <c r="B94" s="29"/>
+      <c r="C94" s="29"/>
+      <c r="D94" s="29"/>
+      <c r="E94" s="29"/>
+      <c r="F94" s="29"/>
+      <c r="G94" s="29"/>
+      <c r="H94" s="29"/>
+      <c r="I94" s="29"/>
+      <c r="J94" s="29"/>
+      <c r="K94" s="29"/>
+      <c r="L94" s="29"/>
+      <c r="M94" s="29"/>
     </row>
     <row r="95" spans="1:13" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="23"/>
-      <c r="B95" s="29" t="s">
+      <c r="B95" s="52" t="s">
         <v>235</v>
       </c>
-      <c r="C95" s="29"/>
-      <c r="D95" s="29"/>
-      <c r="E95" s="29"/>
-      <c r="F95" s="29"/>
-      <c r="G95" s="29"/>
-      <c r="H95" s="29"/>
-      <c r="I95" s="29"/>
-      <c r="J95" s="29"/>
-      <c r="K95" s="29"/>
-      <c r="L95" s="29"/>
-      <c r="M95" s="29"/>
+      <c r="C95" s="52"/>
+      <c r="D95" s="52"/>
+      <c r="E95" s="52"/>
+      <c r="F95" s="52"/>
+      <c r="G95" s="52"/>
+      <c r="H95" s="52"/>
+      <c r="I95" s="52"/>
+      <c r="J95" s="52"/>
+      <c r="K95" s="52"/>
+      <c r="L95" s="52"/>
+      <c r="M95" s="52"/>
     </row>
     <row r="96" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="8" t="s">
@@ -4181,11 +4181,11 @@
       <c r="B96" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="C96" s="42" t="s">
+      <c r="C96" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="D96" s="47"/>
-      <c r="E96" s="43"/>
+      <c r="D96" s="44"/>
+      <c r="E96" s="45"/>
       <c r="F96" s="8"/>
       <c r="G96" s="8"/>
       <c r="H96" s="8"/>
@@ -4202,11 +4202,11 @@
       <c r="B97" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="C97" s="44" t="s">
+      <c r="C97" s="47" t="s">
         <v>223</v>
       </c>
-      <c r="D97" s="51"/>
-      <c r="E97" s="45"/>
+      <c r="D97" s="48"/>
+      <c r="E97" s="49"/>
       <c r="F97" s="13"/>
       <c r="G97" s="14"/>
       <c r="H97" s="14"/>
@@ -4223,11 +4223,11 @@
       <c r="B98" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="C98" s="56" t="s">
+      <c r="C98" s="30" t="s">
         <v>224</v>
       </c>
-      <c r="D98" s="57"/>
-      <c r="E98" s="58"/>
+      <c r="D98" s="50"/>
+      <c r="E98" s="31"/>
       <c r="F98" s="11"/>
       <c r="G98" s="12"/>
       <c r="H98" s="12"/>
@@ -4239,38 +4239,38 @@
     </row>
     <row r="99" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="100" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="31" t="s">
+      <c r="A100" s="42" t="s">
         <v>148</v>
       </c>
-      <c r="B100" s="31"/>
-      <c r="C100" s="31"/>
-      <c r="D100" s="31"/>
-      <c r="E100" s="31"/>
-      <c r="F100" s="31"/>
-      <c r="G100" s="31"/>
-      <c r="H100" s="31"/>
-      <c r="I100" s="31"/>
-      <c r="J100" s="31"/>
-      <c r="K100" s="31"/>
-      <c r="L100" s="31"/>
-      <c r="M100" s="31"/>
+      <c r="B100" s="42"/>
+      <c r="C100" s="42"/>
+      <c r="D100" s="42"/>
+      <c r="E100" s="42"/>
+      <c r="F100" s="42"/>
+      <c r="G100" s="42"/>
+      <c r="H100" s="42"/>
+      <c r="I100" s="42"/>
+      <c r="J100" s="42"/>
+      <c r="K100" s="42"/>
+      <c r="L100" s="42"/>
+      <c r="M100" s="42"/>
     </row>
     <row r="101" spans="1:13" ht="35.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="23"/>
-      <c r="B101" s="29" t="s">
+      <c r="B101" s="52" t="s">
         <v>236</v>
       </c>
-      <c r="C101" s="29"/>
-      <c r="D101" s="29"/>
-      <c r="E101" s="29"/>
-      <c r="F101" s="29"/>
-      <c r="G101" s="29"/>
-      <c r="H101" s="29"/>
-      <c r="I101" s="29"/>
-      <c r="J101" s="29"/>
-      <c r="K101" s="29"/>
-      <c r="L101" s="29"/>
-      <c r="M101" s="29"/>
+      <c r="C101" s="52"/>
+      <c r="D101" s="52"/>
+      <c r="E101" s="52"/>
+      <c r="F101" s="52"/>
+      <c r="G101" s="52"/>
+      <c r="H101" s="52"/>
+      <c r="I101" s="52"/>
+      <c r="J101" s="52"/>
+      <c r="K101" s="52"/>
+      <c r="L101" s="52"/>
+      <c r="M101" s="52"/>
     </row>
     <row r="102" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="8" t="s">
@@ -4361,38 +4361,38 @@
     </row>
     <row r="105" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="106" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="39" t="s">
+      <c r="A106" s="29" t="s">
         <v>149</v>
       </c>
-      <c r="B106" s="39"/>
-      <c r="C106" s="39"/>
-      <c r="D106" s="39"/>
-      <c r="E106" s="39"/>
-      <c r="F106" s="39"/>
-      <c r="G106" s="39"/>
-      <c r="H106" s="39"/>
-      <c r="I106" s="39"/>
-      <c r="J106" s="39"/>
-      <c r="K106" s="39"/>
-      <c r="L106" s="39"/>
-      <c r="M106" s="39"/>
+      <c r="B106" s="29"/>
+      <c r="C106" s="29"/>
+      <c r="D106" s="29"/>
+      <c r="E106" s="29"/>
+      <c r="F106" s="29"/>
+      <c r="G106" s="29"/>
+      <c r="H106" s="29"/>
+      <c r="I106" s="29"/>
+      <c r="J106" s="29"/>
+      <c r="K106" s="29"/>
+      <c r="L106" s="29"/>
+      <c r="M106" s="29"/>
     </row>
     <row r="107" spans="1:13" s="3" customFormat="1" ht="36.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="23"/>
-      <c r="B107" s="29" t="s">
+      <c r="B107" s="52" t="s">
         <v>237</v>
       </c>
-      <c r="C107" s="29"/>
-      <c r="D107" s="29"/>
-      <c r="E107" s="29"/>
-      <c r="F107" s="29"/>
-      <c r="G107" s="29"/>
-      <c r="H107" s="29"/>
-      <c r="I107" s="29"/>
-      <c r="J107" s="29"/>
-      <c r="K107" s="29"/>
-      <c r="L107" s="29"/>
-      <c r="M107" s="29"/>
+      <c r="C107" s="52"/>
+      <c r="D107" s="52"/>
+      <c r="E107" s="52"/>
+      <c r="F107" s="52"/>
+      <c r="G107" s="52"/>
+      <c r="H107" s="52"/>
+      <c r="I107" s="52"/>
+      <c r="J107" s="52"/>
+      <c r="K107" s="52"/>
+      <c r="L107" s="52"/>
+      <c r="M107" s="52"/>
     </row>
     <row r="108" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="8" t="s">
@@ -4502,21 +4502,21 @@
     </row>
     <row r="112" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="113" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="39" t="s">
+      <c r="A113" s="29" t="s">
         <v>151</v>
       </c>
-      <c r="B113" s="39"/>
-      <c r="C113" s="39"/>
-      <c r="D113" s="39"/>
-      <c r="E113" s="39"/>
-      <c r="F113" s="39"/>
-      <c r="G113" s="39"/>
-      <c r="H113" s="39"/>
-      <c r="I113" s="39"/>
-      <c r="J113" s="39"/>
-      <c r="K113" s="39"/>
-      <c r="L113" s="39"/>
-      <c r="M113" s="39"/>
+      <c r="B113" s="29"/>
+      <c r="C113" s="29"/>
+      <c r="D113" s="29"/>
+      <c r="E113" s="29"/>
+      <c r="F113" s="29"/>
+      <c r="G113" s="29"/>
+      <c r="H113" s="29"/>
+      <c r="I113" s="29"/>
+      <c r="J113" s="29"/>
+      <c r="K113" s="29"/>
+      <c r="L113" s="29"/>
+      <c r="M113" s="29"/>
     </row>
     <row r="114" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="8" t="s">
@@ -4590,38 +4590,38 @@
     </row>
     <row r="116" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="117" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="39" t="s">
+      <c r="A117" s="29" t="s">
         <v>159</v>
       </c>
-      <c r="B117" s="39"/>
-      <c r="C117" s="39"/>
-      <c r="D117" s="39"/>
-      <c r="E117" s="39"/>
-      <c r="F117" s="39"/>
-      <c r="G117" s="39"/>
-      <c r="H117" s="39"/>
-      <c r="I117" s="39"/>
-      <c r="J117" s="39"/>
-      <c r="K117" s="39"/>
-      <c r="L117" s="39"/>
-      <c r="M117" s="39"/>
+      <c r="B117" s="29"/>
+      <c r="C117" s="29"/>
+      <c r="D117" s="29"/>
+      <c r="E117" s="29"/>
+      <c r="F117" s="29"/>
+      <c r="G117" s="29"/>
+      <c r="H117" s="29"/>
+      <c r="I117" s="29"/>
+      <c r="J117" s="29"/>
+      <c r="K117" s="29"/>
+      <c r="L117" s="29"/>
+      <c r="M117" s="29"/>
     </row>
     <row r="118" spans="1:13" ht="63.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="26"/>
-      <c r="B118" s="30" t="s">
+      <c r="B118" s="60" t="s">
         <v>241</v>
       </c>
-      <c r="C118" s="30"/>
-      <c r="D118" s="30"/>
-      <c r="E118" s="30"/>
-      <c r="F118" s="30"/>
-      <c r="G118" s="30"/>
-      <c r="H118" s="30"/>
-      <c r="I118" s="30"/>
-      <c r="J118" s="30"/>
-      <c r="K118" s="30"/>
-      <c r="L118" s="30"/>
-      <c r="M118" s="30"/>
+      <c r="C118" s="60"/>
+      <c r="D118" s="60"/>
+      <c r="E118" s="60"/>
+      <c r="F118" s="60"/>
+      <c r="G118" s="60"/>
+      <c r="H118" s="60"/>
+      <c r="I118" s="60"/>
+      <c r="J118" s="60"/>
+      <c r="K118" s="60"/>
+      <c r="L118" s="60"/>
+      <c r="M118" s="60"/>
     </row>
     <row r="119" spans="1:13" s="4" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="8" t="s">
@@ -4724,38 +4724,38 @@
     </row>
     <row r="122" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="123" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="39" t="s">
+      <c r="A123" s="29" t="s">
         <v>172</v>
       </c>
-      <c r="B123" s="39"/>
-      <c r="C123" s="39"/>
-      <c r="D123" s="39"/>
-      <c r="E123" s="39"/>
-      <c r="F123" s="39"/>
-      <c r="G123" s="39"/>
-      <c r="H123" s="39"/>
-      <c r="I123" s="39"/>
-      <c r="J123" s="39"/>
-      <c r="K123" s="39"/>
-      <c r="L123" s="39"/>
-      <c r="M123" s="39"/>
+      <c r="B123" s="29"/>
+      <c r="C123" s="29"/>
+      <c r="D123" s="29"/>
+      <c r="E123" s="29"/>
+      <c r="F123" s="29"/>
+      <c r="G123" s="29"/>
+      <c r="H123" s="29"/>
+      <c r="I123" s="29"/>
+      <c r="J123" s="29"/>
+      <c r="K123" s="29"/>
+      <c r="L123" s="29"/>
+      <c r="M123" s="29"/>
     </row>
     <row r="124" spans="1:13" ht="69.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="26"/>
-      <c r="B124" s="30" t="s">
+      <c r="B124" s="60" t="s">
         <v>242</v>
       </c>
-      <c r="C124" s="30"/>
-      <c r="D124" s="30"/>
-      <c r="E124" s="30"/>
-      <c r="F124" s="30"/>
-      <c r="G124" s="30"/>
-      <c r="H124" s="30"/>
-      <c r="I124" s="30"/>
-      <c r="J124" s="30"/>
-      <c r="K124" s="30"/>
-      <c r="L124" s="30"/>
-      <c r="M124" s="30"/>
+      <c r="C124" s="60"/>
+      <c r="D124" s="60"/>
+      <c r="E124" s="60"/>
+      <c r="F124" s="60"/>
+      <c r="G124" s="60"/>
+      <c r="H124" s="60"/>
+      <c r="I124" s="60"/>
+      <c r="J124" s="60"/>
+      <c r="K124" s="60"/>
+      <c r="L124" s="60"/>
+      <c r="M124" s="60"/>
     </row>
     <row r="125" spans="1:13" s="4" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="10" t="s">
@@ -4857,38 +4857,38 @@
       <c r="M127" s="11"/>
     </row>
     <row r="129" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="46" t="s">
+      <c r="A129" s="61" t="s">
         <v>239</v>
       </c>
-      <c r="B129" s="46"/>
-      <c r="C129" s="46"/>
-      <c r="D129" s="46"/>
-      <c r="E129" s="46"/>
-      <c r="F129" s="46"/>
-      <c r="G129" s="46"/>
-      <c r="H129" s="46"/>
-      <c r="I129" s="46"/>
-      <c r="J129" s="46"/>
-      <c r="K129" s="46"/>
-      <c r="L129" s="46"/>
-      <c r="M129" s="46"/>
+      <c r="B129" s="61"/>
+      <c r="C129" s="61"/>
+      <c r="D129" s="61"/>
+      <c r="E129" s="61"/>
+      <c r="F129" s="61"/>
+      <c r="G129" s="61"/>
+      <c r="H129" s="61"/>
+      <c r="I129" s="61"/>
+      <c r="J129" s="61"/>
+      <c r="K129" s="61"/>
+      <c r="L129" s="61"/>
+      <c r="M129" s="61"/>
     </row>
     <row r="130" spans="1:13" s="3" customFormat="1" ht="51.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="26"/>
-      <c r="B130" s="30" t="s">
+      <c r="B130" s="60" t="s">
         <v>240</v>
       </c>
-      <c r="C130" s="30"/>
-      <c r="D130" s="30"/>
-      <c r="E130" s="30"/>
-      <c r="F130" s="30"/>
-      <c r="G130" s="30"/>
-      <c r="H130" s="30"/>
-      <c r="I130" s="30"/>
-      <c r="J130" s="30"/>
-      <c r="K130" s="30"/>
-      <c r="L130" s="30"/>
-      <c r="M130" s="30"/>
+      <c r="C130" s="60"/>
+      <c r="D130" s="60"/>
+      <c r="E130" s="60"/>
+      <c r="F130" s="60"/>
+      <c r="G130" s="60"/>
+      <c r="H130" s="60"/>
+      <c r="I130" s="60"/>
+      <c r="J130" s="60"/>
+      <c r="K130" s="60"/>
+      <c r="L130" s="60"/>
+      <c r="M130" s="60"/>
     </row>
     <row r="131" spans="1:13" s="4" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="8" t="s">
@@ -4959,36 +4959,14 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="A75:M75"/>
-    <mergeCell ref="A80:M80"/>
-    <mergeCell ref="A85:M85"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="G72:H72"/>
-    <mergeCell ref="G73:H73"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="E72:F72"/>
-    <mergeCell ref="E73:F73"/>
-    <mergeCell ref="A100:M100"/>
-    <mergeCell ref="A106:M106"/>
-    <mergeCell ref="D91:F91"/>
-    <mergeCell ref="D92:F92"/>
-    <mergeCell ref="C97:E97"/>
-    <mergeCell ref="C96:E96"/>
-    <mergeCell ref="C98:E98"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A39:M39"/>
-    <mergeCell ref="A50:M50"/>
-    <mergeCell ref="A54:M54"/>
-    <mergeCell ref="A28:M28"/>
-    <mergeCell ref="B11:M11"/>
-    <mergeCell ref="B40:M40"/>
-    <mergeCell ref="B29:M29"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="N8:P8"/>
-    <mergeCell ref="A10:M10"/>
-    <mergeCell ref="B6:M6"/>
-    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="B107:M107"/>
+    <mergeCell ref="B118:M118"/>
+    <mergeCell ref="B130:M130"/>
+    <mergeCell ref="B124:M124"/>
+    <mergeCell ref="A123:M123"/>
+    <mergeCell ref="A113:M113"/>
+    <mergeCell ref="A117:M117"/>
+    <mergeCell ref="A129:M129"/>
     <mergeCell ref="B55:M55"/>
     <mergeCell ref="B65:M65"/>
     <mergeCell ref="A70:M70"/>
@@ -5005,15 +4983,37 @@
     <mergeCell ref="I72:J72"/>
     <mergeCell ref="I73:J73"/>
     <mergeCell ref="A90:M90"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="N8:P8"/>
+    <mergeCell ref="A10:M10"/>
+    <mergeCell ref="B6:M6"/>
+    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A39:M39"/>
+    <mergeCell ref="A50:M50"/>
+    <mergeCell ref="A54:M54"/>
+    <mergeCell ref="A28:M28"/>
+    <mergeCell ref="B11:M11"/>
+    <mergeCell ref="B40:M40"/>
+    <mergeCell ref="B29:M29"/>
+    <mergeCell ref="A100:M100"/>
+    <mergeCell ref="A106:M106"/>
+    <mergeCell ref="D91:F91"/>
+    <mergeCell ref="D92:F92"/>
+    <mergeCell ref="C97:E97"/>
+    <mergeCell ref="C96:E96"/>
+    <mergeCell ref="C98:E98"/>
     <mergeCell ref="B101:M101"/>
-    <mergeCell ref="B107:M107"/>
-    <mergeCell ref="B118:M118"/>
-    <mergeCell ref="B130:M130"/>
-    <mergeCell ref="B124:M124"/>
-    <mergeCell ref="A123:M123"/>
-    <mergeCell ref="A113:M113"/>
-    <mergeCell ref="A117:M117"/>
-    <mergeCell ref="A129:M129"/>
+    <mergeCell ref="A75:M75"/>
+    <mergeCell ref="A80:M80"/>
+    <mergeCell ref="A85:M85"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="G72:H72"/>
+    <mergeCell ref="G73:H73"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="E72:F72"/>
+    <mergeCell ref="E73:F73"/>
   </mergeCells>
   <dataValidations count="59">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3" xr:uid="{00000000-0002-0000-0000-000000000000}">

</xml_diff>

<commit_message>
added bds, epgs, static ports to tenant config
</commit_message>
<xml_diff>
--- a/deploy-fabric-Input-Spreadsheet.xlsx
+++ b/deploy-fabric-Input-Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\tyscott\terraform-aci-fabric-deploy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9134FD90-DD6A-4B09-8B06-C6493386A1C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1EE10C4-C961-46E4-ABD7-72D432E5A848}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2010,33 +2010,96 @@
     <xf numFmtId="164" fontId="19" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="18" fillId="34" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="34" borderId="29" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="17" fillId="33" borderId="8" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="17" fillId="36" borderId="8" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="33" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="34" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="34" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="25" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="26" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="20" fillId="34" borderId="22" xfId="43" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="34" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="23" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="24" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="34" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="34" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="34" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="28" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="34" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="34" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="34" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="25" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="26" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="20" fillId="34" borderId="22" xfId="43" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="19" fillId="34" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="19" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="19" fillId="34" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="19" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2044,69 +2107,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="20" fillId="34" borderId="22" xfId="43" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="33" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="19" fillId="34" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="34" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="23" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="24" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="28" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="34" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="34" borderId="29" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="36" borderId="8" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2469,7 +2469,7 @@
   <dimension ref="A1:P133"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2494,21 +2494,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
     </row>
     <row r="2" spans="1:16" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -2549,41 +2549,41 @@
       <c r="M3" s="13"/>
     </row>
     <row r="5" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="33" t="s">
         <v>202</v>
       </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="42"/>
-      <c r="K5" s="42"/>
-      <c r="L5" s="42"/>
-      <c r="M5" s="42"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="33"/>
       <c r="N5" s="22"/>
       <c r="O5" s="22"/>
       <c r="P5" s="22"/>
     </row>
     <row r="6" spans="1:16" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="20"/>
-      <c r="B6" s="58" t="s">
+      <c r="B6" s="50" t="s">
         <v>238</v>
       </c>
-      <c r="C6" s="58"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="58"/>
-      <c r="G6" s="58"/>
-      <c r="H6" s="58"/>
-      <c r="I6" s="58"/>
-      <c r="J6" s="58"/>
-      <c r="K6" s="58"/>
-      <c r="L6" s="58"/>
-      <c r="M6" s="58"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="50"/>
+      <c r="K6" s="50"/>
+      <c r="L6" s="50"/>
+      <c r="M6" s="50"/>
       <c r="N6" s="20"/>
       <c r="O6" s="20"/>
       <c r="P6" s="20"/>
@@ -2628,11 +2628,11 @@
       <c r="M7" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="N7" s="53" t="s">
+      <c r="N7" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="O7" s="54"/>
-      <c r="P7" s="55"/>
+      <c r="O7" s="45"/>
+      <c r="P7" s="46"/>
     </row>
     <row r="8" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
@@ -2672,26 +2672,26 @@
         <v>48</v>
       </c>
       <c r="M8" s="27"/>
-      <c r="N8" s="56"/>
-      <c r="O8" s="57"/>
-      <c r="P8" s="41"/>
+      <c r="N8" s="47"/>
+      <c r="O8" s="48"/>
+      <c r="P8" s="49"/>
     </row>
     <row r="10" spans="1:16" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="29"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
     </row>
     <row r="11" spans="1:16" s="6" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="21"/>
@@ -3032,21 +3032,21 @@
       <c r="M26" s="11"/>
     </row>
     <row r="28" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="31" t="s">
         <v>243</v>
       </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
-      <c r="K28" s="29"/>
-      <c r="L28" s="29"/>
-      <c r="M28" s="29"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="31"/>
+      <c r="I28" s="31"/>
+      <c r="J28" s="31"/>
+      <c r="K28" s="31"/>
+      <c r="L28" s="31"/>
+      <c r="M28" s="31"/>
     </row>
     <row r="29" spans="1:13" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="21"/>
@@ -3206,38 +3206,38 @@
       <c r="M37" s="13"/>
     </row>
     <row r="39" spans="1:13" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="29" t="s">
+      <c r="A39" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="B39" s="29"/>
-      <c r="C39" s="29"/>
-      <c r="D39" s="29"/>
-      <c r="E39" s="29"/>
-      <c r="F39" s="29"/>
-      <c r="G39" s="29"/>
-      <c r="H39" s="29"/>
-      <c r="I39" s="29"/>
-      <c r="J39" s="29"/>
-      <c r="K39" s="29"/>
-      <c r="L39" s="29"/>
-      <c r="M39" s="29"/>
+      <c r="B39" s="31"/>
+      <c r="C39" s="31"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="31"/>
+      <c r="G39" s="31"/>
+      <c r="H39" s="31"/>
+      <c r="I39" s="31"/>
+      <c r="J39" s="31"/>
+      <c r="K39" s="31"/>
+      <c r="L39" s="31"/>
+      <c r="M39" s="31"/>
     </row>
     <row r="40" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="23"/>
-      <c r="B40" s="52" t="s">
+      <c r="B40" s="29" t="s">
         <v>226</v>
       </c>
-      <c r="C40" s="52"/>
-      <c r="D40" s="52"/>
-      <c r="E40" s="52"/>
-      <c r="F40" s="52"/>
-      <c r="G40" s="52"/>
-      <c r="H40" s="52"/>
-      <c r="I40" s="52"/>
-      <c r="J40" s="52"/>
-      <c r="K40" s="52"/>
-      <c r="L40" s="52"/>
-      <c r="M40" s="52"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="29"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="29"/>
+      <c r="G40" s="29"/>
+      <c r="H40" s="29"/>
+      <c r="I40" s="29"/>
+      <c r="J40" s="29"/>
+      <c r="K40" s="29"/>
+      <c r="L40" s="29"/>
+      <c r="M40" s="29"/>
     </row>
     <row r="41" spans="1:13" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="8" t="s">
@@ -3400,21 +3400,21 @@
       <c r="M48" s="13"/>
     </row>
     <row r="50" spans="1:13" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="29" t="s">
+      <c r="A50" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="B50" s="29"/>
-      <c r="C50" s="29"/>
-      <c r="D50" s="29"/>
-      <c r="E50" s="29"/>
-      <c r="F50" s="29"/>
-      <c r="G50" s="29"/>
-      <c r="H50" s="29"/>
-      <c r="I50" s="29"/>
-      <c r="J50" s="29"/>
-      <c r="K50" s="29"/>
-      <c r="L50" s="29"/>
-      <c r="M50" s="29"/>
+      <c r="B50" s="31"/>
+      <c r="C50" s="31"/>
+      <c r="D50" s="31"/>
+      <c r="E50" s="31"/>
+      <c r="F50" s="31"/>
+      <c r="G50" s="31"/>
+      <c r="H50" s="31"/>
+      <c r="I50" s="31"/>
+      <c r="J50" s="31"/>
+      <c r="K50" s="31"/>
+      <c r="L50" s="31"/>
+      <c r="M50" s="31"/>
     </row>
     <row r="51" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="8" t="s">
@@ -3455,38 +3455,38 @@
       <c r="M52" s="13"/>
     </row>
     <row r="54" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="29" t="s">
+      <c r="A54" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="B54" s="29"/>
-      <c r="C54" s="29"/>
-      <c r="D54" s="29"/>
-      <c r="E54" s="29"/>
-      <c r="F54" s="29"/>
-      <c r="G54" s="29"/>
-      <c r="H54" s="29"/>
-      <c r="I54" s="29"/>
-      <c r="J54" s="29"/>
-      <c r="K54" s="29"/>
-      <c r="L54" s="29"/>
-      <c r="M54" s="29"/>
+      <c r="B54" s="31"/>
+      <c r="C54" s="31"/>
+      <c r="D54" s="31"/>
+      <c r="E54" s="31"/>
+      <c r="F54" s="31"/>
+      <c r="G54" s="31"/>
+      <c r="H54" s="31"/>
+      <c r="I54" s="31"/>
+      <c r="J54" s="31"/>
+      <c r="K54" s="31"/>
+      <c r="L54" s="31"/>
+      <c r="M54" s="31"/>
     </row>
     <row r="55" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="23"/>
-      <c r="B55" s="52" t="s">
+      <c r="B55" s="29" t="s">
         <v>227</v>
       </c>
-      <c r="C55" s="52"/>
-      <c r="D55" s="52"/>
-      <c r="E55" s="52"/>
-      <c r="F55" s="52"/>
-      <c r="G55" s="52"/>
-      <c r="H55" s="52"/>
-      <c r="I55" s="52"/>
-      <c r="J55" s="52"/>
-      <c r="K55" s="52"/>
-      <c r="L55" s="52"/>
-      <c r="M55" s="52"/>
+      <c r="C55" s="29"/>
+      <c r="D55" s="29"/>
+      <c r="E55" s="29"/>
+      <c r="F55" s="29"/>
+      <c r="G55" s="29"/>
+      <c r="H55" s="29"/>
+      <c r="I55" s="29"/>
+      <c r="J55" s="29"/>
+      <c r="K55" s="29"/>
+      <c r="L55" s="29"/>
+      <c r="M55" s="29"/>
     </row>
     <row r="56" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="8" t="s">
@@ -3546,21 +3546,21 @@
       <c r="M58" s="11"/>
     </row>
     <row r="60" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="29" t="s">
+      <c r="A60" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="B60" s="29"/>
-      <c r="C60" s="29"/>
-      <c r="D60" s="29"/>
-      <c r="E60" s="29"/>
-      <c r="F60" s="29"/>
-      <c r="G60" s="29"/>
-      <c r="H60" s="29"/>
-      <c r="I60" s="29"/>
-      <c r="J60" s="29"/>
-      <c r="K60" s="29"/>
-      <c r="L60" s="29"/>
-      <c r="M60" s="29"/>
+      <c r="B60" s="31"/>
+      <c r="C60" s="31"/>
+      <c r="D60" s="31"/>
+      <c r="E60" s="31"/>
+      <c r="F60" s="31"/>
+      <c r="G60" s="31"/>
+      <c r="H60" s="31"/>
+      <c r="I60" s="31"/>
+      <c r="J60" s="31"/>
+      <c r="K60" s="31"/>
+      <c r="L60" s="31"/>
+      <c r="M60" s="31"/>
     </row>
     <row r="61" spans="1:13" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="8" t="s">
@@ -3601,38 +3601,38 @@
       <c r="M62" s="13"/>
     </row>
     <row r="64" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="29" t="s">
+      <c r="A64" s="31" t="s">
         <v>119</v>
       </c>
-      <c r="B64" s="29"/>
-      <c r="C64" s="29"/>
-      <c r="D64" s="29"/>
-      <c r="E64" s="29"/>
-      <c r="F64" s="29"/>
-      <c r="G64" s="29"/>
-      <c r="H64" s="29"/>
-      <c r="I64" s="29"/>
-      <c r="J64" s="29"/>
-      <c r="K64" s="29"/>
-      <c r="L64" s="29"/>
-      <c r="M64" s="29"/>
+      <c r="B64" s="31"/>
+      <c r="C64" s="31"/>
+      <c r="D64" s="31"/>
+      <c r="E64" s="31"/>
+      <c r="F64" s="31"/>
+      <c r="G64" s="31"/>
+      <c r="H64" s="31"/>
+      <c r="I64" s="31"/>
+      <c r="J64" s="31"/>
+      <c r="K64" s="31"/>
+      <c r="L64" s="31"/>
+      <c r="M64" s="31"/>
     </row>
     <row r="65" spans="1:16" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="23"/>
-      <c r="B65" s="52" t="s">
+      <c r="B65" s="29" t="s">
         <v>228</v>
       </c>
-      <c r="C65" s="52"/>
-      <c r="D65" s="52"/>
-      <c r="E65" s="52"/>
-      <c r="F65" s="52"/>
-      <c r="G65" s="52"/>
-      <c r="H65" s="52"/>
-      <c r="I65" s="52"/>
-      <c r="J65" s="52"/>
-      <c r="K65" s="52"/>
-      <c r="L65" s="52"/>
-      <c r="M65" s="52"/>
+      <c r="C65" s="29"/>
+      <c r="D65" s="29"/>
+      <c r="E65" s="29"/>
+      <c r="F65" s="29"/>
+      <c r="G65" s="29"/>
+      <c r="H65" s="29"/>
+      <c r="I65" s="29"/>
+      <c r="J65" s="29"/>
+      <c r="K65" s="29"/>
+      <c r="L65" s="29"/>
+      <c r="M65" s="29"/>
     </row>
     <row r="66" spans="1:16" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="8" t="s">
@@ -3698,41 +3698,41 @@
       <c r="M68" s="11"/>
     </row>
     <row r="70" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="42" t="s">
+      <c r="A70" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="B70" s="42"/>
-      <c r="C70" s="42"/>
-      <c r="D70" s="42"/>
-      <c r="E70" s="42"/>
-      <c r="F70" s="42"/>
-      <c r="G70" s="42"/>
-      <c r="H70" s="42"/>
-      <c r="I70" s="42"/>
-      <c r="J70" s="42"/>
-      <c r="K70" s="42"/>
-      <c r="L70" s="42"/>
-      <c r="M70" s="42"/>
+      <c r="B70" s="33"/>
+      <c r="C70" s="33"/>
+      <c r="D70" s="33"/>
+      <c r="E70" s="33"/>
+      <c r="F70" s="33"/>
+      <c r="G70" s="33"/>
+      <c r="H70" s="33"/>
+      <c r="I70" s="33"/>
+      <c r="J70" s="33"/>
+      <c r="K70" s="33"/>
+      <c r="L70" s="33"/>
+      <c r="M70" s="33"/>
       <c r="N70" s="24"/>
       <c r="O70" s="24"/>
       <c r="P70" s="24"/>
     </row>
     <row r="71" spans="1:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="25"/>
-      <c r="B71" s="59" t="s">
+      <c r="B71" s="34" t="s">
         <v>229</v>
       </c>
-      <c r="C71" s="59"/>
-      <c r="D71" s="59"/>
-      <c r="E71" s="59"/>
-      <c r="F71" s="59"/>
-      <c r="G71" s="59"/>
-      <c r="H71" s="59"/>
-      <c r="I71" s="59"/>
-      <c r="J71" s="59"/>
-      <c r="K71" s="59"/>
-      <c r="L71" s="59"/>
-      <c r="M71" s="59"/>
+      <c r="C71" s="34"/>
+      <c r="D71" s="34"/>
+      <c r="E71" s="34"/>
+      <c r="F71" s="34"/>
+      <c r="G71" s="34"/>
+      <c r="H71" s="34"/>
+      <c r="I71" s="34"/>
+      <c r="J71" s="34"/>
+      <c r="K71" s="34"/>
+      <c r="L71" s="34"/>
+      <c r="M71" s="34"/>
       <c r="N71" s="25"/>
       <c r="O71" s="25"/>
       <c r="P71" s="25"/>
@@ -3750,18 +3750,18 @@
       <c r="D72" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="E72" s="32" t="s">
+      <c r="E72" s="40" t="s">
         <v>131</v>
       </c>
-      <c r="F72" s="33"/>
-      <c r="G72" s="32" t="s">
+      <c r="F72" s="41"/>
+      <c r="G72" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="H72" s="33"/>
-      <c r="I72" s="32" t="s">
+      <c r="H72" s="41"/>
+      <c r="I72" s="40" t="s">
         <v>133</v>
       </c>
-      <c r="J72" s="33"/>
+      <c r="J72" s="41"/>
       <c r="K72" s="8" t="s">
         <v>134</v>
       </c>
@@ -3794,18 +3794,18 @@
       <c r="D73" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E73" s="40" t="s">
+      <c r="E73" s="61" t="s">
         <v>183</v>
       </c>
-      <c r="F73" s="41"/>
-      <c r="G73" s="34" t="s">
+      <c r="F73" s="49"/>
+      <c r="G73" s="42" t="s">
         <v>184</v>
       </c>
-      <c r="H73" s="35"/>
-      <c r="I73" s="34" t="s">
+      <c r="H73" s="43"/>
+      <c r="I73" s="42" t="s">
         <v>184</v>
       </c>
-      <c r="J73" s="35"/>
+      <c r="J73" s="43"/>
       <c r="K73" s="13" t="s">
         <v>185</v>
       </c>
@@ -3827,21 +3827,21 @@
     </row>
     <row r="74" spans="1:16" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="75" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="29" t="s">
+      <c r="A75" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="B75" s="29"/>
-      <c r="C75" s="29"/>
-      <c r="D75" s="29"/>
-      <c r="E75" s="29"/>
-      <c r="F75" s="29"/>
-      <c r="G75" s="29"/>
-      <c r="H75" s="29"/>
-      <c r="I75" s="29"/>
-      <c r="J75" s="29"/>
-      <c r="K75" s="29"/>
-      <c r="L75" s="29"/>
-      <c r="M75" s="29"/>
+      <c r="B75" s="31"/>
+      <c r="C75" s="31"/>
+      <c r="D75" s="31"/>
+      <c r="E75" s="31"/>
+      <c r="F75" s="31"/>
+      <c r="G75" s="31"/>
+      <c r="H75" s="31"/>
+      <c r="I75" s="31"/>
+      <c r="J75" s="31"/>
+      <c r="K75" s="31"/>
+      <c r="L75" s="31"/>
+      <c r="M75" s="31"/>
     </row>
     <row r="76" spans="1:16" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="8" t="s">
@@ -3913,34 +3913,34 @@
       <c r="M78" s="11"/>
     </row>
     <row r="80" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="29" t="s">
+      <c r="A80" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="B80" s="29"/>
-      <c r="C80" s="29"/>
-      <c r="D80" s="29"/>
-      <c r="E80" s="29"/>
-      <c r="F80" s="29"/>
-      <c r="G80" s="29"/>
-      <c r="H80" s="29"/>
-      <c r="I80" s="29"/>
-      <c r="J80" s="29"/>
-      <c r="K80" s="29"/>
-      <c r="L80" s="29"/>
-      <c r="M80" s="29"/>
+      <c r="B80" s="31"/>
+      <c r="C80" s="31"/>
+      <c r="D80" s="31"/>
+      <c r="E80" s="31"/>
+      <c r="F80" s="31"/>
+      <c r="G80" s="31"/>
+      <c r="H80" s="31"/>
+      <c r="I80" s="31"/>
+      <c r="J80" s="31"/>
+      <c r="K80" s="31"/>
+      <c r="L80" s="31"/>
+      <c r="M80" s="31"/>
     </row>
     <row r="81" spans="1:13" s="3" customFormat="1" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B81" s="43" t="s">
+      <c r="B81" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C81" s="45"/>
-      <c r="D81" s="43" t="s">
+      <c r="C81" s="36"/>
+      <c r="D81" s="35" t="s">
         <v>125</v>
       </c>
-      <c r="E81" s="45"/>
+      <c r="E81" s="36"/>
       <c r="F81" s="8"/>
       <c r="G81" s="8"/>
       <c r="H81" s="8"/>
@@ -3954,14 +3954,14 @@
       <c r="A82" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B82" s="47" t="s">
+      <c r="B82" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="C82" s="49"/>
-      <c r="D82" s="36" t="s">
+      <c r="C82" s="38"/>
+      <c r="D82" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="E82" s="37"/>
+      <c r="E82" s="54"/>
       <c r="F82" s="13"/>
       <c r="G82" s="14"/>
       <c r="H82" s="14"/>
@@ -3975,14 +3975,14 @@
       <c r="A83" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B83" s="30" t="s">
+      <c r="B83" s="56" t="s">
         <v>128</v>
       </c>
-      <c r="C83" s="31"/>
-      <c r="D83" s="38" t="s">
+      <c r="C83" s="58"/>
+      <c r="D83" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="E83" s="39"/>
+      <c r="E83" s="60"/>
       <c r="F83" s="11"/>
       <c r="G83" s="12"/>
       <c r="H83" s="12"/>
@@ -3993,21 +3993,21 @@
       <c r="M83" s="11"/>
     </row>
     <row r="85" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="29" t="s">
+      <c r="A85" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="B85" s="29"/>
-      <c r="C85" s="29"/>
-      <c r="D85" s="29"/>
-      <c r="E85" s="29"/>
-      <c r="F85" s="29"/>
-      <c r="G85" s="29"/>
-      <c r="H85" s="29"/>
-      <c r="I85" s="29"/>
-      <c r="J85" s="29"/>
-      <c r="K85" s="29"/>
-      <c r="L85" s="29"/>
-      <c r="M85" s="29"/>
+      <c r="B85" s="31"/>
+      <c r="C85" s="31"/>
+      <c r="D85" s="31"/>
+      <c r="E85" s="31"/>
+      <c r="F85" s="31"/>
+      <c r="G85" s="31"/>
+      <c r="H85" s="31"/>
+      <c r="I85" s="31"/>
+      <c r="J85" s="31"/>
+      <c r="K85" s="31"/>
+      <c r="L85" s="31"/>
+      <c r="M85" s="31"/>
     </row>
     <row r="86" spans="1:13" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="8" t="s">
@@ -4079,35 +4079,35 @@
       <c r="M88" s="11"/>
     </row>
     <row r="90" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="29" t="s">
+      <c r="A90" s="31" t="s">
         <v>147</v>
       </c>
-      <c r="B90" s="29"/>
-      <c r="C90" s="29"/>
-      <c r="D90" s="29"/>
-      <c r="E90" s="29"/>
-      <c r="F90" s="29"/>
-      <c r="G90" s="29"/>
-      <c r="H90" s="29"/>
-      <c r="I90" s="29"/>
-      <c r="J90" s="29"/>
-      <c r="K90" s="29"/>
-      <c r="L90" s="29"/>
-      <c r="M90" s="29"/>
+      <c r="B90" s="31"/>
+      <c r="C90" s="31"/>
+      <c r="D90" s="31"/>
+      <c r="E90" s="31"/>
+      <c r="F90" s="31"/>
+      <c r="G90" s="31"/>
+      <c r="H90" s="31"/>
+      <c r="I90" s="31"/>
+      <c r="J90" s="31"/>
+      <c r="K90" s="31"/>
+      <c r="L90" s="31"/>
+      <c r="M90" s="31"/>
     </row>
     <row r="91" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B91" s="44" t="s">
+      <c r="B91" s="39" t="s">
         <v>145</v>
       </c>
-      <c r="C91" s="44"/>
-      <c r="D91" s="43" t="s">
+      <c r="C91" s="39"/>
+      <c r="D91" s="35" t="s">
         <v>146</v>
       </c>
-      <c r="E91" s="44"/>
-      <c r="F91" s="45"/>
+      <c r="E91" s="39"/>
+      <c r="F91" s="36"/>
       <c r="G91" s="8"/>
       <c r="H91" s="8"/>
       <c r="I91" s="8"/>
@@ -4120,15 +4120,15 @@
       <c r="A92" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B92" s="47" t="s">
+      <c r="B92" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="C92" s="49"/>
-      <c r="D92" s="36" t="s">
+      <c r="C92" s="38"/>
+      <c r="D92" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="E92" s="46"/>
-      <c r="F92" s="37"/>
+      <c r="E92" s="53"/>
+      <c r="F92" s="54"/>
       <c r="G92" s="14"/>
       <c r="H92" s="14"/>
       <c r="I92" s="13"/>
@@ -4141,38 +4141,38 @@
       <c r="B93" s="7"/>
     </row>
     <row r="94" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="29" t="s">
+      <c r="A94" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="B94" s="29"/>
-      <c r="C94" s="29"/>
-      <c r="D94" s="29"/>
-      <c r="E94" s="29"/>
-      <c r="F94" s="29"/>
-      <c r="G94" s="29"/>
-      <c r="H94" s="29"/>
-      <c r="I94" s="29"/>
-      <c r="J94" s="29"/>
-      <c r="K94" s="29"/>
-      <c r="L94" s="29"/>
-      <c r="M94" s="29"/>
+      <c r="B94" s="31"/>
+      <c r="C94" s="31"/>
+      <c r="D94" s="31"/>
+      <c r="E94" s="31"/>
+      <c r="F94" s="31"/>
+      <c r="G94" s="31"/>
+      <c r="H94" s="31"/>
+      <c r="I94" s="31"/>
+      <c r="J94" s="31"/>
+      <c r="K94" s="31"/>
+      <c r="L94" s="31"/>
+      <c r="M94" s="31"/>
     </row>
     <row r="95" spans="1:13" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="23"/>
-      <c r="B95" s="52" t="s">
+      <c r="B95" s="29" t="s">
         <v>235</v>
       </c>
-      <c r="C95" s="52"/>
-      <c r="D95" s="52"/>
-      <c r="E95" s="52"/>
-      <c r="F95" s="52"/>
-      <c r="G95" s="52"/>
-      <c r="H95" s="52"/>
-      <c r="I95" s="52"/>
-      <c r="J95" s="52"/>
-      <c r="K95" s="52"/>
-      <c r="L95" s="52"/>
-      <c r="M95" s="52"/>
+      <c r="C95" s="29"/>
+      <c r="D95" s="29"/>
+      <c r="E95" s="29"/>
+      <c r="F95" s="29"/>
+      <c r="G95" s="29"/>
+      <c r="H95" s="29"/>
+      <c r="I95" s="29"/>
+      <c r="J95" s="29"/>
+      <c r="K95" s="29"/>
+      <c r="L95" s="29"/>
+      <c r="M95" s="29"/>
     </row>
     <row r="96" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="8" t="s">
@@ -4181,11 +4181,11 @@
       <c r="B96" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="C96" s="43" t="s">
+      <c r="C96" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="D96" s="44"/>
-      <c r="E96" s="45"/>
+      <c r="D96" s="39"/>
+      <c r="E96" s="36"/>
       <c r="F96" s="8"/>
       <c r="G96" s="8"/>
       <c r="H96" s="8"/>
@@ -4202,11 +4202,11 @@
       <c r="B97" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="C97" s="47" t="s">
+      <c r="C97" s="37" t="s">
         <v>223</v>
       </c>
-      <c r="D97" s="48"/>
-      <c r="E97" s="49"/>
+      <c r="D97" s="55"/>
+      <c r="E97" s="38"/>
       <c r="F97" s="13"/>
       <c r="G97" s="14"/>
       <c r="H97" s="14"/>
@@ -4223,11 +4223,11 @@
       <c r="B98" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="C98" s="30" t="s">
+      <c r="C98" s="56" t="s">
         <v>224</v>
       </c>
-      <c r="D98" s="50"/>
-      <c r="E98" s="31"/>
+      <c r="D98" s="57"/>
+      <c r="E98" s="58"/>
       <c r="F98" s="11"/>
       <c r="G98" s="12"/>
       <c r="H98" s="12"/>
@@ -4239,38 +4239,38 @@
     </row>
     <row r="99" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="100" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="42" t="s">
+      <c r="A100" s="33" t="s">
         <v>148</v>
       </c>
-      <c r="B100" s="42"/>
-      <c r="C100" s="42"/>
-      <c r="D100" s="42"/>
-      <c r="E100" s="42"/>
-      <c r="F100" s="42"/>
-      <c r="G100" s="42"/>
-      <c r="H100" s="42"/>
-      <c r="I100" s="42"/>
-      <c r="J100" s="42"/>
-      <c r="K100" s="42"/>
-      <c r="L100" s="42"/>
-      <c r="M100" s="42"/>
+      <c r="B100" s="33"/>
+      <c r="C100" s="33"/>
+      <c r="D100" s="33"/>
+      <c r="E100" s="33"/>
+      <c r="F100" s="33"/>
+      <c r="G100" s="33"/>
+      <c r="H100" s="33"/>
+      <c r="I100" s="33"/>
+      <c r="J100" s="33"/>
+      <c r="K100" s="33"/>
+      <c r="L100" s="33"/>
+      <c r="M100" s="33"/>
     </row>
     <row r="101" spans="1:13" ht="35.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="23"/>
-      <c r="B101" s="52" t="s">
+      <c r="B101" s="29" t="s">
         <v>236</v>
       </c>
-      <c r="C101" s="52"/>
-      <c r="D101" s="52"/>
-      <c r="E101" s="52"/>
-      <c r="F101" s="52"/>
-      <c r="G101" s="52"/>
-      <c r="H101" s="52"/>
-      <c r="I101" s="52"/>
-      <c r="J101" s="52"/>
-      <c r="K101" s="52"/>
-      <c r="L101" s="52"/>
-      <c r="M101" s="52"/>
+      <c r="C101" s="29"/>
+      <c r="D101" s="29"/>
+      <c r="E101" s="29"/>
+      <c r="F101" s="29"/>
+      <c r="G101" s="29"/>
+      <c r="H101" s="29"/>
+      <c r="I101" s="29"/>
+      <c r="J101" s="29"/>
+      <c r="K101" s="29"/>
+      <c r="L101" s="29"/>
+      <c r="M101" s="29"/>
     </row>
     <row r="102" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="8" t="s">
@@ -4361,38 +4361,38 @@
     </row>
     <row r="105" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="106" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="29" t="s">
+      <c r="A106" s="31" t="s">
         <v>149</v>
       </c>
-      <c r="B106" s="29"/>
-      <c r="C106" s="29"/>
-      <c r="D106" s="29"/>
-      <c r="E106" s="29"/>
-      <c r="F106" s="29"/>
-      <c r="G106" s="29"/>
-      <c r="H106" s="29"/>
-      <c r="I106" s="29"/>
-      <c r="J106" s="29"/>
-      <c r="K106" s="29"/>
-      <c r="L106" s="29"/>
-      <c r="M106" s="29"/>
+      <c r="B106" s="31"/>
+      <c r="C106" s="31"/>
+      <c r="D106" s="31"/>
+      <c r="E106" s="31"/>
+      <c r="F106" s="31"/>
+      <c r="G106" s="31"/>
+      <c r="H106" s="31"/>
+      <c r="I106" s="31"/>
+      <c r="J106" s="31"/>
+      <c r="K106" s="31"/>
+      <c r="L106" s="31"/>
+      <c r="M106" s="31"/>
     </row>
     <row r="107" spans="1:13" s="3" customFormat="1" ht="36.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="23"/>
-      <c r="B107" s="52" t="s">
+      <c r="B107" s="29" t="s">
         <v>237</v>
       </c>
-      <c r="C107" s="52"/>
-      <c r="D107" s="52"/>
-      <c r="E107" s="52"/>
-      <c r="F107" s="52"/>
-      <c r="G107" s="52"/>
-      <c r="H107" s="52"/>
-      <c r="I107" s="52"/>
-      <c r="J107" s="52"/>
-      <c r="K107" s="52"/>
-      <c r="L107" s="52"/>
-      <c r="M107" s="52"/>
+      <c r="C107" s="29"/>
+      <c r="D107" s="29"/>
+      <c r="E107" s="29"/>
+      <c r="F107" s="29"/>
+      <c r="G107" s="29"/>
+      <c r="H107" s="29"/>
+      <c r="I107" s="29"/>
+      <c r="J107" s="29"/>
+      <c r="K107" s="29"/>
+      <c r="L107" s="29"/>
+      <c r="M107" s="29"/>
     </row>
     <row r="108" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="8" t="s">
@@ -4502,21 +4502,21 @@
     </row>
     <row r="112" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="113" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="29" t="s">
+      <c r="A113" s="31" t="s">
         <v>151</v>
       </c>
-      <c r="B113" s="29"/>
-      <c r="C113" s="29"/>
-      <c r="D113" s="29"/>
-      <c r="E113" s="29"/>
-      <c r="F113" s="29"/>
-      <c r="G113" s="29"/>
-      <c r="H113" s="29"/>
-      <c r="I113" s="29"/>
-      <c r="J113" s="29"/>
-      <c r="K113" s="29"/>
-      <c r="L113" s="29"/>
-      <c r="M113" s="29"/>
+      <c r="B113" s="31"/>
+      <c r="C113" s="31"/>
+      <c r="D113" s="31"/>
+      <c r="E113" s="31"/>
+      <c r="F113" s="31"/>
+      <c r="G113" s="31"/>
+      <c r="H113" s="31"/>
+      <c r="I113" s="31"/>
+      <c r="J113" s="31"/>
+      <c r="K113" s="31"/>
+      <c r="L113" s="31"/>
+      <c r="M113" s="31"/>
     </row>
     <row r="114" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="8" t="s">
@@ -4590,38 +4590,38 @@
     </row>
     <row r="116" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="117" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="29" t="s">
+      <c r="A117" s="31" t="s">
         <v>159</v>
       </c>
-      <c r="B117" s="29"/>
-      <c r="C117" s="29"/>
-      <c r="D117" s="29"/>
-      <c r="E117" s="29"/>
-      <c r="F117" s="29"/>
-      <c r="G117" s="29"/>
-      <c r="H117" s="29"/>
-      <c r="I117" s="29"/>
-      <c r="J117" s="29"/>
-      <c r="K117" s="29"/>
-      <c r="L117" s="29"/>
-      <c r="M117" s="29"/>
+      <c r="B117" s="31"/>
+      <c r="C117" s="31"/>
+      <c r="D117" s="31"/>
+      <c r="E117" s="31"/>
+      <c r="F117" s="31"/>
+      <c r="G117" s="31"/>
+      <c r="H117" s="31"/>
+      <c r="I117" s="31"/>
+      <c r="J117" s="31"/>
+      <c r="K117" s="31"/>
+      <c r="L117" s="31"/>
+      <c r="M117" s="31"/>
     </row>
     <row r="118" spans="1:13" ht="63.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="26"/>
-      <c r="B118" s="60" t="s">
+      <c r="B118" s="30" t="s">
         <v>241</v>
       </c>
-      <c r="C118" s="60"/>
-      <c r="D118" s="60"/>
-      <c r="E118" s="60"/>
-      <c r="F118" s="60"/>
-      <c r="G118" s="60"/>
-      <c r="H118" s="60"/>
-      <c r="I118" s="60"/>
-      <c r="J118" s="60"/>
-      <c r="K118" s="60"/>
-      <c r="L118" s="60"/>
-      <c r="M118" s="60"/>
+      <c r="C118" s="30"/>
+      <c r="D118" s="30"/>
+      <c r="E118" s="30"/>
+      <c r="F118" s="30"/>
+      <c r="G118" s="30"/>
+      <c r="H118" s="30"/>
+      <c r="I118" s="30"/>
+      <c r="J118" s="30"/>
+      <c r="K118" s="30"/>
+      <c r="L118" s="30"/>
+      <c r="M118" s="30"/>
     </row>
     <row r="119" spans="1:13" s="4" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="8" t="s">
@@ -4724,38 +4724,38 @@
     </row>
     <row r="122" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="123" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="29" t="s">
+      <c r="A123" s="31" t="s">
         <v>172</v>
       </c>
-      <c r="B123" s="29"/>
-      <c r="C123" s="29"/>
-      <c r="D123" s="29"/>
-      <c r="E123" s="29"/>
-      <c r="F123" s="29"/>
-      <c r="G123" s="29"/>
-      <c r="H123" s="29"/>
-      <c r="I123" s="29"/>
-      <c r="J123" s="29"/>
-      <c r="K123" s="29"/>
-      <c r="L123" s="29"/>
-      <c r="M123" s="29"/>
+      <c r="B123" s="31"/>
+      <c r="C123" s="31"/>
+      <c r="D123" s="31"/>
+      <c r="E123" s="31"/>
+      <c r="F123" s="31"/>
+      <c r="G123" s="31"/>
+      <c r="H123" s="31"/>
+      <c r="I123" s="31"/>
+      <c r="J123" s="31"/>
+      <c r="K123" s="31"/>
+      <c r="L123" s="31"/>
+      <c r="M123" s="31"/>
     </row>
     <row r="124" spans="1:13" ht="69.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="26"/>
-      <c r="B124" s="60" t="s">
+      <c r="B124" s="30" t="s">
         <v>242</v>
       </c>
-      <c r="C124" s="60"/>
-      <c r="D124" s="60"/>
-      <c r="E124" s="60"/>
-      <c r="F124" s="60"/>
-      <c r="G124" s="60"/>
-      <c r="H124" s="60"/>
-      <c r="I124" s="60"/>
-      <c r="J124" s="60"/>
-      <c r="K124" s="60"/>
-      <c r="L124" s="60"/>
-      <c r="M124" s="60"/>
+      <c r="C124" s="30"/>
+      <c r="D124" s="30"/>
+      <c r="E124" s="30"/>
+      <c r="F124" s="30"/>
+      <c r="G124" s="30"/>
+      <c r="H124" s="30"/>
+      <c r="I124" s="30"/>
+      <c r="J124" s="30"/>
+      <c r="K124" s="30"/>
+      <c r="L124" s="30"/>
+      <c r="M124" s="30"/>
     </row>
     <row r="125" spans="1:13" s="4" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="10" t="s">
@@ -4857,38 +4857,38 @@
       <c r="M127" s="11"/>
     </row>
     <row r="129" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="61" t="s">
+      <c r="A129" s="32" t="s">
         <v>239</v>
       </c>
-      <c r="B129" s="61"/>
-      <c r="C129" s="61"/>
-      <c r="D129" s="61"/>
-      <c r="E129" s="61"/>
-      <c r="F129" s="61"/>
-      <c r="G129" s="61"/>
-      <c r="H129" s="61"/>
-      <c r="I129" s="61"/>
-      <c r="J129" s="61"/>
-      <c r="K129" s="61"/>
-      <c r="L129" s="61"/>
-      <c r="M129" s="61"/>
+      <c r="B129" s="32"/>
+      <c r="C129" s="32"/>
+      <c r="D129" s="32"/>
+      <c r="E129" s="32"/>
+      <c r="F129" s="32"/>
+      <c r="G129" s="32"/>
+      <c r="H129" s="32"/>
+      <c r="I129" s="32"/>
+      <c r="J129" s="32"/>
+      <c r="K129" s="32"/>
+      <c r="L129" s="32"/>
+      <c r="M129" s="32"/>
     </row>
     <row r="130" spans="1:13" s="3" customFormat="1" ht="51.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="26"/>
-      <c r="B130" s="60" t="s">
+      <c r="B130" s="30" t="s">
         <v>240</v>
       </c>
-      <c r="C130" s="60"/>
-      <c r="D130" s="60"/>
-      <c r="E130" s="60"/>
-      <c r="F130" s="60"/>
-      <c r="G130" s="60"/>
-      <c r="H130" s="60"/>
-      <c r="I130" s="60"/>
-      <c r="J130" s="60"/>
-      <c r="K130" s="60"/>
-      <c r="L130" s="60"/>
-      <c r="M130" s="60"/>
+      <c r="C130" s="30"/>
+      <c r="D130" s="30"/>
+      <c r="E130" s="30"/>
+      <c r="F130" s="30"/>
+      <c r="G130" s="30"/>
+      <c r="H130" s="30"/>
+      <c r="I130" s="30"/>
+      <c r="J130" s="30"/>
+      <c r="K130" s="30"/>
+      <c r="L130" s="30"/>
+      <c r="M130" s="30"/>
     </row>
     <row r="131" spans="1:13" s="4" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="8" t="s">
@@ -4959,14 +4959,37 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="B107:M107"/>
-    <mergeCell ref="B118:M118"/>
-    <mergeCell ref="B130:M130"/>
-    <mergeCell ref="B124:M124"/>
-    <mergeCell ref="A123:M123"/>
-    <mergeCell ref="A113:M113"/>
-    <mergeCell ref="A117:M117"/>
-    <mergeCell ref="A129:M129"/>
+    <mergeCell ref="A75:M75"/>
+    <mergeCell ref="A80:M80"/>
+    <mergeCell ref="A85:M85"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="G72:H72"/>
+    <mergeCell ref="G73:H73"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="E72:F72"/>
+    <mergeCell ref="E73:F73"/>
+    <mergeCell ref="A100:M100"/>
+    <mergeCell ref="A106:M106"/>
+    <mergeCell ref="D91:F91"/>
+    <mergeCell ref="D92:F92"/>
+    <mergeCell ref="C97:E97"/>
+    <mergeCell ref="C96:E96"/>
+    <mergeCell ref="C98:E98"/>
+    <mergeCell ref="B101:M101"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A39:M39"/>
+    <mergeCell ref="A50:M50"/>
+    <mergeCell ref="A54:M54"/>
+    <mergeCell ref="A28:M28"/>
+    <mergeCell ref="B11:M11"/>
+    <mergeCell ref="B40:M40"/>
+    <mergeCell ref="B29:M29"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="N8:P8"/>
+    <mergeCell ref="A10:M10"/>
+    <mergeCell ref="B6:M6"/>
+    <mergeCell ref="A5:M5"/>
     <mergeCell ref="B55:M55"/>
     <mergeCell ref="B65:M65"/>
     <mergeCell ref="A70:M70"/>
@@ -4983,37 +5006,14 @@
     <mergeCell ref="I72:J72"/>
     <mergeCell ref="I73:J73"/>
     <mergeCell ref="A90:M90"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="N8:P8"/>
-    <mergeCell ref="A10:M10"/>
-    <mergeCell ref="B6:M6"/>
-    <mergeCell ref="A5:M5"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A39:M39"/>
-    <mergeCell ref="A50:M50"/>
-    <mergeCell ref="A54:M54"/>
-    <mergeCell ref="A28:M28"/>
-    <mergeCell ref="B11:M11"/>
-    <mergeCell ref="B40:M40"/>
-    <mergeCell ref="B29:M29"/>
-    <mergeCell ref="A100:M100"/>
-    <mergeCell ref="A106:M106"/>
-    <mergeCell ref="D91:F91"/>
-    <mergeCell ref="D92:F92"/>
-    <mergeCell ref="C97:E97"/>
-    <mergeCell ref="C96:E96"/>
-    <mergeCell ref="C98:E98"/>
-    <mergeCell ref="B101:M101"/>
-    <mergeCell ref="A75:M75"/>
-    <mergeCell ref="A80:M80"/>
-    <mergeCell ref="A85:M85"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="G72:H72"/>
-    <mergeCell ref="G73:H73"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="E72:F72"/>
-    <mergeCell ref="E73:F73"/>
+    <mergeCell ref="B107:M107"/>
+    <mergeCell ref="B118:M118"/>
+    <mergeCell ref="B130:M130"/>
+    <mergeCell ref="B124:M124"/>
+    <mergeCell ref="A123:M123"/>
+    <mergeCell ref="A113:M113"/>
+    <mergeCell ref="A117:M117"/>
+    <mergeCell ref="A129:M129"/>
   </mergeCells>
   <dataValidations count="59">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3" xr:uid="{00000000-0002-0000-0000-000000000000}">

</xml_diff>

<commit_message>
access port configuration complete.  applying
</commit_message>
<xml_diff>
--- a/deploy-fabric-Input-Spreadsheet.xlsx
+++ b/deploy-fabric-Input-Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\tyscott\terraform-aci-fabric-deploy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1EE10C4-C961-46E4-ABD7-72D432E5A848}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7139621-DB50-4E4B-9291-E5DAB86C51A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="leaf">formulas!$B$2:$B$18</definedName>
-    <definedName name="spine">formulas!$C$2:$C$11</definedName>
+    <definedName name="spine">formulas!$C$2:$C$12</definedName>
     <definedName name="switch_role">formulas!$A$2:$A$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="246">
   <si>
     <t>Type</t>
   </si>
@@ -1125,6 +1125,9 @@
       </rPr>
       <t xml:space="preserve"> It is Recommended to use the 1st Node Id for the VPC ID unless you are using Node ID's &gt; 1000.  Make sure each VPC Domain is unique in the Fabric.</t>
     </r>
+  </si>
+  <si>
+    <t>9336PQ</t>
   </si>
 </sst>
 </file>
@@ -2010,103 +2013,103 @@
     <xf numFmtId="164" fontId="19" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="17" fillId="33" borderId="8" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="25" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="26" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="20" fillId="34" borderId="22" xfId="43" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="34" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="34" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="34" borderId="22" xfId="43" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="34" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="33" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="34" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="34" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="34" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="18" fillId="34" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="23" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="24" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="34" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="34" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="28" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="34" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="18" fillId="34" borderId="29" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="33" borderId="8" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="17" fillId="36" borderId="8" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="33" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="34" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="25" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="26" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="20" fillId="34" borderId="22" xfId="43" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="19" fillId="34" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="23" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="24" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="28" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="19" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="19" fillId="34" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="19" fillId="34" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="19" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="19" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="34" borderId="22" xfId="43" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2469,7 +2472,7 @@
   <dimension ref="A1:P133"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="D14" sqref="D14:D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2494,21 +2497,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
     </row>
     <row r="2" spans="1:16" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -2549,41 +2552,41 @@
       <c r="M3" s="13"/>
     </row>
     <row r="5" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="42" t="s">
         <v>202</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="33"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="42"/>
+      <c r="L5" s="42"/>
+      <c r="M5" s="42"/>
       <c r="N5" s="22"/>
       <c r="O5" s="22"/>
       <c r="P5" s="22"/>
     </row>
     <row r="6" spans="1:16" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="20"/>
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="58" t="s">
         <v>238</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="50"/>
-      <c r="I6" s="50"/>
-      <c r="J6" s="50"/>
-      <c r="K6" s="50"/>
-      <c r="L6" s="50"/>
-      <c r="M6" s="50"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="58"/>
+      <c r="K6" s="58"/>
+      <c r="L6" s="58"/>
+      <c r="M6" s="58"/>
       <c r="N6" s="20"/>
       <c r="O6" s="20"/>
       <c r="P6" s="20"/>
@@ -2628,11 +2631,11 @@
       <c r="M7" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="N7" s="44" t="s">
+      <c r="N7" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="O7" s="45"/>
-      <c r="P7" s="46"/>
+      <c r="O7" s="54"/>
+      <c r="P7" s="55"/>
     </row>
     <row r="8" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
@@ -2672,43 +2675,43 @@
         <v>48</v>
       </c>
       <c r="M8" s="27"/>
-      <c r="N8" s="47"/>
-      <c r="O8" s="48"/>
-      <c r="P8" s="49"/>
+      <c r="N8" s="56"/>
+      <c r="O8" s="57"/>
+      <c r="P8" s="41"/>
     </row>
     <row r="10" spans="1:16" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="31"/>
-      <c r="L10" s="31"/>
-      <c r="M10" s="31"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
     </row>
     <row r="11" spans="1:16" s="6" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="21"/>
-      <c r="B11" s="51" t="s">
+      <c r="B11" s="52" t="s">
         <v>225</v>
       </c>
-      <c r="C11" s="51"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="51"/>
-      <c r="G11" s="51"/>
-      <c r="H11" s="51"/>
-      <c r="I11" s="51"/>
-      <c r="J11" s="51"/>
-      <c r="K11" s="51"/>
-      <c r="L11" s="51"/>
-      <c r="M11" s="51"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="52"/>
+      <c r="K11" s="52"/>
+      <c r="L11" s="52"/>
+      <c r="M11" s="52"/>
     </row>
     <row r="12" spans="1:16" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
@@ -3032,38 +3035,38 @@
       <c r="M26" s="11"/>
     </row>
     <row r="28" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="29" t="s">
         <v>243</v>
       </c>
-      <c r="B28" s="31"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
-      <c r="I28" s="31"/>
-      <c r="J28" s="31"/>
-      <c r="K28" s="31"/>
-      <c r="L28" s="31"/>
-      <c r="M28" s="31"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
+      <c r="K28" s="29"/>
+      <c r="L28" s="29"/>
+      <c r="M28" s="29"/>
     </row>
     <row r="29" spans="1:13" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="21"/>
-      <c r="B29" s="51" t="s">
+      <c r="B29" s="52" t="s">
         <v>244</v>
       </c>
-      <c r="C29" s="51"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="51"/>
-      <c r="G29" s="51"/>
-      <c r="H29" s="51"/>
-      <c r="I29" s="51"/>
-      <c r="J29" s="51"/>
-      <c r="K29" s="51"/>
-      <c r="L29" s="51"/>
-      <c r="M29" s="51"/>
+      <c r="C29" s="52"/>
+      <c r="D29" s="52"/>
+      <c r="E29" s="52"/>
+      <c r="F29" s="52"/>
+      <c r="G29" s="52"/>
+      <c r="H29" s="52"/>
+      <c r="I29" s="52"/>
+      <c r="J29" s="52"/>
+      <c r="K29" s="52"/>
+      <c r="L29" s="52"/>
+      <c r="M29" s="52"/>
     </row>
     <row r="30" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
@@ -3206,38 +3209,38 @@
       <c r="M37" s="13"/>
     </row>
     <row r="39" spans="1:13" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="31" t="s">
+      <c r="A39" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="B39" s="31"/>
-      <c r="C39" s="31"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="31"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="31"/>
-      <c r="H39" s="31"/>
-      <c r="I39" s="31"/>
-      <c r="J39" s="31"/>
-      <c r="K39" s="31"/>
-      <c r="L39" s="31"/>
-      <c r="M39" s="31"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="29"/>
+      <c r="E39" s="29"/>
+      <c r="F39" s="29"/>
+      <c r="G39" s="29"/>
+      <c r="H39" s="29"/>
+      <c r="I39" s="29"/>
+      <c r="J39" s="29"/>
+      <c r="K39" s="29"/>
+      <c r="L39" s="29"/>
+      <c r="M39" s="29"/>
     </row>
     <row r="40" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="23"/>
-      <c r="B40" s="29" t="s">
+      <c r="B40" s="51" t="s">
         <v>226</v>
       </c>
-      <c r="C40" s="29"/>
-      <c r="D40" s="29"/>
-      <c r="E40" s="29"/>
-      <c r="F40" s="29"/>
-      <c r="G40" s="29"/>
-      <c r="H40" s="29"/>
-      <c r="I40" s="29"/>
-      <c r="J40" s="29"/>
-      <c r="K40" s="29"/>
-      <c r="L40" s="29"/>
-      <c r="M40" s="29"/>
+      <c r="C40" s="51"/>
+      <c r="D40" s="51"/>
+      <c r="E40" s="51"/>
+      <c r="F40" s="51"/>
+      <c r="G40" s="51"/>
+      <c r="H40" s="51"/>
+      <c r="I40" s="51"/>
+      <c r="J40" s="51"/>
+      <c r="K40" s="51"/>
+      <c r="L40" s="51"/>
+      <c r="M40" s="51"/>
     </row>
     <row r="41" spans="1:13" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="8" t="s">
@@ -3400,21 +3403,21 @@
       <c r="M48" s="13"/>
     </row>
     <row r="50" spans="1:13" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="31" t="s">
+      <c r="A50" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="B50" s="31"/>
-      <c r="C50" s="31"/>
-      <c r="D50" s="31"/>
-      <c r="E50" s="31"/>
-      <c r="F50" s="31"/>
-      <c r="G50" s="31"/>
-      <c r="H50" s="31"/>
-      <c r="I50" s="31"/>
-      <c r="J50" s="31"/>
-      <c r="K50" s="31"/>
-      <c r="L50" s="31"/>
-      <c r="M50" s="31"/>
+      <c r="B50" s="29"/>
+      <c r="C50" s="29"/>
+      <c r="D50" s="29"/>
+      <c r="E50" s="29"/>
+      <c r="F50" s="29"/>
+      <c r="G50" s="29"/>
+      <c r="H50" s="29"/>
+      <c r="I50" s="29"/>
+      <c r="J50" s="29"/>
+      <c r="K50" s="29"/>
+      <c r="L50" s="29"/>
+      <c r="M50" s="29"/>
     </row>
     <row r="51" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="8" t="s">
@@ -3455,38 +3458,38 @@
       <c r="M52" s="13"/>
     </row>
     <row r="54" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="31" t="s">
+      <c r="A54" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="B54" s="31"/>
-      <c r="C54" s="31"/>
-      <c r="D54" s="31"/>
-      <c r="E54" s="31"/>
-      <c r="F54" s="31"/>
-      <c r="G54" s="31"/>
-      <c r="H54" s="31"/>
-      <c r="I54" s="31"/>
-      <c r="J54" s="31"/>
-      <c r="K54" s="31"/>
-      <c r="L54" s="31"/>
-      <c r="M54" s="31"/>
+      <c r="B54" s="29"/>
+      <c r="C54" s="29"/>
+      <c r="D54" s="29"/>
+      <c r="E54" s="29"/>
+      <c r="F54" s="29"/>
+      <c r="G54" s="29"/>
+      <c r="H54" s="29"/>
+      <c r="I54" s="29"/>
+      <c r="J54" s="29"/>
+      <c r="K54" s="29"/>
+      <c r="L54" s="29"/>
+      <c r="M54" s="29"/>
     </row>
     <row r="55" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="23"/>
-      <c r="B55" s="29" t="s">
+      <c r="B55" s="51" t="s">
         <v>227</v>
       </c>
-      <c r="C55" s="29"/>
-      <c r="D55" s="29"/>
-      <c r="E55" s="29"/>
-      <c r="F55" s="29"/>
-      <c r="G55" s="29"/>
-      <c r="H55" s="29"/>
-      <c r="I55" s="29"/>
-      <c r="J55" s="29"/>
-      <c r="K55" s="29"/>
-      <c r="L55" s="29"/>
-      <c r="M55" s="29"/>
+      <c r="C55" s="51"/>
+      <c r="D55" s="51"/>
+      <c r="E55" s="51"/>
+      <c r="F55" s="51"/>
+      <c r="G55" s="51"/>
+      <c r="H55" s="51"/>
+      <c r="I55" s="51"/>
+      <c r="J55" s="51"/>
+      <c r="K55" s="51"/>
+      <c r="L55" s="51"/>
+      <c r="M55" s="51"/>
     </row>
     <row r="56" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="8" t="s">
@@ -3546,21 +3549,21 @@
       <c r="M58" s="11"/>
     </row>
     <row r="60" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="31" t="s">
+      <c r="A60" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="B60" s="31"/>
-      <c r="C60" s="31"/>
-      <c r="D60" s="31"/>
-      <c r="E60" s="31"/>
-      <c r="F60" s="31"/>
-      <c r="G60" s="31"/>
-      <c r="H60" s="31"/>
-      <c r="I60" s="31"/>
-      <c r="J60" s="31"/>
-      <c r="K60" s="31"/>
-      <c r="L60" s="31"/>
-      <c r="M60" s="31"/>
+      <c r="B60" s="29"/>
+      <c r="C60" s="29"/>
+      <c r="D60" s="29"/>
+      <c r="E60" s="29"/>
+      <c r="F60" s="29"/>
+      <c r="G60" s="29"/>
+      <c r="H60" s="29"/>
+      <c r="I60" s="29"/>
+      <c r="J60" s="29"/>
+      <c r="K60" s="29"/>
+      <c r="L60" s="29"/>
+      <c r="M60" s="29"/>
     </row>
     <row r="61" spans="1:13" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="8" t="s">
@@ -3601,38 +3604,38 @@
       <c r="M62" s="13"/>
     </row>
     <row r="64" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="31" t="s">
+      <c r="A64" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="B64" s="31"/>
-      <c r="C64" s="31"/>
-      <c r="D64" s="31"/>
-      <c r="E64" s="31"/>
-      <c r="F64" s="31"/>
-      <c r="G64" s="31"/>
-      <c r="H64" s="31"/>
-      <c r="I64" s="31"/>
-      <c r="J64" s="31"/>
-      <c r="K64" s="31"/>
-      <c r="L64" s="31"/>
-      <c r="M64" s="31"/>
+      <c r="B64" s="29"/>
+      <c r="C64" s="29"/>
+      <c r="D64" s="29"/>
+      <c r="E64" s="29"/>
+      <c r="F64" s="29"/>
+      <c r="G64" s="29"/>
+      <c r="H64" s="29"/>
+      <c r="I64" s="29"/>
+      <c r="J64" s="29"/>
+      <c r="K64" s="29"/>
+      <c r="L64" s="29"/>
+      <c r="M64" s="29"/>
     </row>
     <row r="65" spans="1:16" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="23"/>
-      <c r="B65" s="29" t="s">
+      <c r="B65" s="51" t="s">
         <v>228</v>
       </c>
-      <c r="C65" s="29"/>
-      <c r="D65" s="29"/>
-      <c r="E65" s="29"/>
-      <c r="F65" s="29"/>
-      <c r="G65" s="29"/>
-      <c r="H65" s="29"/>
-      <c r="I65" s="29"/>
-      <c r="J65" s="29"/>
-      <c r="K65" s="29"/>
-      <c r="L65" s="29"/>
-      <c r="M65" s="29"/>
+      <c r="C65" s="51"/>
+      <c r="D65" s="51"/>
+      <c r="E65" s="51"/>
+      <c r="F65" s="51"/>
+      <c r="G65" s="51"/>
+      <c r="H65" s="51"/>
+      <c r="I65" s="51"/>
+      <c r="J65" s="51"/>
+      <c r="K65" s="51"/>
+      <c r="L65" s="51"/>
+      <c r="M65" s="51"/>
     </row>
     <row r="66" spans="1:16" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="8" t="s">
@@ -3698,41 +3701,41 @@
       <c r="M68" s="11"/>
     </row>
     <row r="70" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="33" t="s">
+      <c r="A70" s="42" t="s">
         <v>120</v>
       </c>
-      <c r="B70" s="33"/>
-      <c r="C70" s="33"/>
-      <c r="D70" s="33"/>
-      <c r="E70" s="33"/>
-      <c r="F70" s="33"/>
-      <c r="G70" s="33"/>
-      <c r="H70" s="33"/>
-      <c r="I70" s="33"/>
-      <c r="J70" s="33"/>
-      <c r="K70" s="33"/>
-      <c r="L70" s="33"/>
-      <c r="M70" s="33"/>
+      <c r="B70" s="42"/>
+      <c r="C70" s="42"/>
+      <c r="D70" s="42"/>
+      <c r="E70" s="42"/>
+      <c r="F70" s="42"/>
+      <c r="G70" s="42"/>
+      <c r="H70" s="42"/>
+      <c r="I70" s="42"/>
+      <c r="J70" s="42"/>
+      <c r="K70" s="42"/>
+      <c r="L70" s="42"/>
+      <c r="M70" s="42"/>
       <c r="N70" s="24"/>
       <c r="O70" s="24"/>
       <c r="P70" s="24"/>
     </row>
     <row r="71" spans="1:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="25"/>
-      <c r="B71" s="34" t="s">
+      <c r="B71" s="59" t="s">
         <v>229</v>
       </c>
-      <c r="C71" s="34"/>
-      <c r="D71" s="34"/>
-      <c r="E71" s="34"/>
-      <c r="F71" s="34"/>
-      <c r="G71" s="34"/>
-      <c r="H71" s="34"/>
-      <c r="I71" s="34"/>
-      <c r="J71" s="34"/>
-      <c r="K71" s="34"/>
-      <c r="L71" s="34"/>
-      <c r="M71" s="34"/>
+      <c r="C71" s="59"/>
+      <c r="D71" s="59"/>
+      <c r="E71" s="59"/>
+      <c r="F71" s="59"/>
+      <c r="G71" s="59"/>
+      <c r="H71" s="59"/>
+      <c r="I71" s="59"/>
+      <c r="J71" s="59"/>
+      <c r="K71" s="59"/>
+      <c r="L71" s="59"/>
+      <c r="M71" s="59"/>
       <c r="N71" s="25"/>
       <c r="O71" s="25"/>
       <c r="P71" s="25"/>
@@ -3750,18 +3753,18 @@
       <c r="D72" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="E72" s="40" t="s">
+      <c r="E72" s="32" t="s">
         <v>131</v>
       </c>
-      <c r="F72" s="41"/>
-      <c r="G72" s="40" t="s">
+      <c r="F72" s="33"/>
+      <c r="G72" s="32" t="s">
         <v>132</v>
       </c>
-      <c r="H72" s="41"/>
-      <c r="I72" s="40" t="s">
+      <c r="H72" s="33"/>
+      <c r="I72" s="32" t="s">
         <v>133</v>
       </c>
-      <c r="J72" s="41"/>
+      <c r="J72" s="33"/>
       <c r="K72" s="8" t="s">
         <v>134</v>
       </c>
@@ -3794,18 +3797,18 @@
       <c r="D73" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E73" s="61" t="s">
+      <c r="E73" s="40" t="s">
         <v>183</v>
       </c>
-      <c r="F73" s="49"/>
-      <c r="G73" s="42" t="s">
+      <c r="F73" s="41"/>
+      <c r="G73" s="34" t="s">
         <v>184</v>
       </c>
-      <c r="H73" s="43"/>
-      <c r="I73" s="42" t="s">
+      <c r="H73" s="35"/>
+      <c r="I73" s="34" t="s">
         <v>184</v>
       </c>
-      <c r="J73" s="43"/>
+      <c r="J73" s="35"/>
       <c r="K73" s="13" t="s">
         <v>185</v>
       </c>
@@ -3827,21 +3830,21 @@
     </row>
     <row r="74" spans="1:16" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="75" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="31" t="s">
+      <c r="A75" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="B75" s="31"/>
-      <c r="C75" s="31"/>
-      <c r="D75" s="31"/>
-      <c r="E75" s="31"/>
-      <c r="F75" s="31"/>
-      <c r="G75" s="31"/>
-      <c r="H75" s="31"/>
-      <c r="I75" s="31"/>
-      <c r="J75" s="31"/>
-      <c r="K75" s="31"/>
-      <c r="L75" s="31"/>
-      <c r="M75" s="31"/>
+      <c r="B75" s="29"/>
+      <c r="C75" s="29"/>
+      <c r="D75" s="29"/>
+      <c r="E75" s="29"/>
+      <c r="F75" s="29"/>
+      <c r="G75" s="29"/>
+      <c r="H75" s="29"/>
+      <c r="I75" s="29"/>
+      <c r="J75" s="29"/>
+      <c r="K75" s="29"/>
+      <c r="L75" s="29"/>
+      <c r="M75" s="29"/>
     </row>
     <row r="76" spans="1:16" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="8" t="s">
@@ -3913,34 +3916,34 @@
       <c r="M78" s="11"/>
     </row>
     <row r="80" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="31" t="s">
+      <c r="A80" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="B80" s="31"/>
-      <c r="C80" s="31"/>
-      <c r="D80" s="31"/>
-      <c r="E80" s="31"/>
-      <c r="F80" s="31"/>
-      <c r="G80" s="31"/>
-      <c r="H80" s="31"/>
-      <c r="I80" s="31"/>
-      <c r="J80" s="31"/>
-      <c r="K80" s="31"/>
-      <c r="L80" s="31"/>
-      <c r="M80" s="31"/>
+      <c r="B80" s="29"/>
+      <c r="C80" s="29"/>
+      <c r="D80" s="29"/>
+      <c r="E80" s="29"/>
+      <c r="F80" s="29"/>
+      <c r="G80" s="29"/>
+      <c r="H80" s="29"/>
+      <c r="I80" s="29"/>
+      <c r="J80" s="29"/>
+      <c r="K80" s="29"/>
+      <c r="L80" s="29"/>
+      <c r="M80" s="29"/>
     </row>
     <row r="81" spans="1:13" s="3" customFormat="1" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B81" s="35" t="s">
+      <c r="B81" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="C81" s="36"/>
-      <c r="D81" s="35" t="s">
+      <c r="C81" s="45"/>
+      <c r="D81" s="43" t="s">
         <v>125</v>
       </c>
-      <c r="E81" s="36"/>
+      <c r="E81" s="45"/>
       <c r="F81" s="8"/>
       <c r="G81" s="8"/>
       <c r="H81" s="8"/>
@@ -3954,14 +3957,14 @@
       <c r="A82" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B82" s="37" t="s">
+      <c r="B82" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="C82" s="38"/>
-      <c r="D82" s="52" t="s">
+      <c r="C82" s="49"/>
+      <c r="D82" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="E82" s="54"/>
+      <c r="E82" s="37"/>
       <c r="F82" s="13"/>
       <c r="G82" s="14"/>
       <c r="H82" s="14"/>
@@ -3975,14 +3978,14 @@
       <c r="A83" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B83" s="56" t="s">
+      <c r="B83" s="30" t="s">
         <v>128</v>
       </c>
-      <c r="C83" s="58"/>
-      <c r="D83" s="59" t="s">
+      <c r="C83" s="31"/>
+      <c r="D83" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="E83" s="60"/>
+      <c r="E83" s="39"/>
       <c r="F83" s="11"/>
       <c r="G83" s="12"/>
       <c r="H83" s="12"/>
@@ -3993,21 +3996,21 @@
       <c r="M83" s="11"/>
     </row>
     <row r="85" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="31" t="s">
+      <c r="A85" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B85" s="31"/>
-      <c r="C85" s="31"/>
-      <c r="D85" s="31"/>
-      <c r="E85" s="31"/>
-      <c r="F85" s="31"/>
-      <c r="G85" s="31"/>
-      <c r="H85" s="31"/>
-      <c r="I85" s="31"/>
-      <c r="J85" s="31"/>
-      <c r="K85" s="31"/>
-      <c r="L85" s="31"/>
-      <c r="M85" s="31"/>
+      <c r="B85" s="29"/>
+      <c r="C85" s="29"/>
+      <c r="D85" s="29"/>
+      <c r="E85" s="29"/>
+      <c r="F85" s="29"/>
+      <c r="G85" s="29"/>
+      <c r="H85" s="29"/>
+      <c r="I85" s="29"/>
+      <c r="J85" s="29"/>
+      <c r="K85" s="29"/>
+      <c r="L85" s="29"/>
+      <c r="M85" s="29"/>
     </row>
     <row r="86" spans="1:13" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="8" t="s">
@@ -4079,35 +4082,35 @@
       <c r="M88" s="11"/>
     </row>
     <row r="90" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="31" t="s">
+      <c r="A90" s="29" t="s">
         <v>147</v>
       </c>
-      <c r="B90" s="31"/>
-      <c r="C90" s="31"/>
-      <c r="D90" s="31"/>
-      <c r="E90" s="31"/>
-      <c r="F90" s="31"/>
-      <c r="G90" s="31"/>
-      <c r="H90" s="31"/>
-      <c r="I90" s="31"/>
-      <c r="J90" s="31"/>
-      <c r="K90" s="31"/>
-      <c r="L90" s="31"/>
-      <c r="M90" s="31"/>
+      <c r="B90" s="29"/>
+      <c r="C90" s="29"/>
+      <c r="D90" s="29"/>
+      <c r="E90" s="29"/>
+      <c r="F90" s="29"/>
+      <c r="G90" s="29"/>
+      <c r="H90" s="29"/>
+      <c r="I90" s="29"/>
+      <c r="J90" s="29"/>
+      <c r="K90" s="29"/>
+      <c r="L90" s="29"/>
+      <c r="M90" s="29"/>
     </row>
     <row r="91" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B91" s="39" t="s">
+      <c r="B91" s="44" t="s">
         <v>145</v>
       </c>
-      <c r="C91" s="39"/>
-      <c r="D91" s="35" t="s">
+      <c r="C91" s="44"/>
+      <c r="D91" s="43" t="s">
         <v>146</v>
       </c>
-      <c r="E91" s="39"/>
-      <c r="F91" s="36"/>
+      <c r="E91" s="44"/>
+      <c r="F91" s="45"/>
       <c r="G91" s="8"/>
       <c r="H91" s="8"/>
       <c r="I91" s="8"/>
@@ -4120,15 +4123,15 @@
       <c r="A92" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B92" s="37" t="s">
+      <c r="B92" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="C92" s="38"/>
-      <c r="D92" s="52" t="s">
+      <c r="C92" s="49"/>
+      <c r="D92" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="E92" s="53"/>
-      <c r="F92" s="54"/>
+      <c r="E92" s="46"/>
+      <c r="F92" s="37"/>
       <c r="G92" s="14"/>
       <c r="H92" s="14"/>
       <c r="I92" s="13"/>
@@ -4141,38 +4144,38 @@
       <c r="B93" s="7"/>
     </row>
     <row r="94" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="31" t="s">
+      <c r="A94" s="29" t="s">
         <v>140</v>
       </c>
-      <c r="B94" s="31"/>
-      <c r="C94" s="31"/>
-      <c r="D94" s="31"/>
-      <c r="E94" s="31"/>
-      <c r="F94" s="31"/>
-      <c r="G94" s="31"/>
-      <c r="H94" s="31"/>
-      <c r="I94" s="31"/>
-      <c r="J94" s="31"/>
-      <c r="K94" s="31"/>
-      <c r="L94" s="31"/>
-      <c r="M94" s="31"/>
+      <c r="B94" s="29"/>
+      <c r="C94" s="29"/>
+      <c r="D94" s="29"/>
+      <c r="E94" s="29"/>
+      <c r="F94" s="29"/>
+      <c r="G94" s="29"/>
+      <c r="H94" s="29"/>
+      <c r="I94" s="29"/>
+      <c r="J94" s="29"/>
+      <c r="K94" s="29"/>
+      <c r="L94" s="29"/>
+      <c r="M94" s="29"/>
     </row>
     <row r="95" spans="1:13" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="23"/>
-      <c r="B95" s="29" t="s">
+      <c r="B95" s="51" t="s">
         <v>235</v>
       </c>
-      <c r="C95" s="29"/>
-      <c r="D95" s="29"/>
-      <c r="E95" s="29"/>
-      <c r="F95" s="29"/>
-      <c r="G95" s="29"/>
-      <c r="H95" s="29"/>
-      <c r="I95" s="29"/>
-      <c r="J95" s="29"/>
-      <c r="K95" s="29"/>
-      <c r="L95" s="29"/>
-      <c r="M95" s="29"/>
+      <c r="C95" s="51"/>
+      <c r="D95" s="51"/>
+      <c r="E95" s="51"/>
+      <c r="F95" s="51"/>
+      <c r="G95" s="51"/>
+      <c r="H95" s="51"/>
+      <c r="I95" s="51"/>
+      <c r="J95" s="51"/>
+      <c r="K95" s="51"/>
+      <c r="L95" s="51"/>
+      <c r="M95" s="51"/>
     </row>
     <row r="96" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="8" t="s">
@@ -4181,11 +4184,11 @@
       <c r="B96" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="C96" s="35" t="s">
+      <c r="C96" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="D96" s="39"/>
-      <c r="E96" s="36"/>
+      <c r="D96" s="44"/>
+      <c r="E96" s="45"/>
       <c r="F96" s="8"/>
       <c r="G96" s="8"/>
       <c r="H96" s="8"/>
@@ -4202,11 +4205,11 @@
       <c r="B97" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="C97" s="37" t="s">
+      <c r="C97" s="47" t="s">
         <v>223</v>
       </c>
-      <c r="D97" s="55"/>
-      <c r="E97" s="38"/>
+      <c r="D97" s="48"/>
+      <c r="E97" s="49"/>
       <c r="F97" s="13"/>
       <c r="G97" s="14"/>
       <c r="H97" s="14"/>
@@ -4223,11 +4226,11 @@
       <c r="B98" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="C98" s="56" t="s">
+      <c r="C98" s="30" t="s">
         <v>224</v>
       </c>
-      <c r="D98" s="57"/>
-      <c r="E98" s="58"/>
+      <c r="D98" s="50"/>
+      <c r="E98" s="31"/>
       <c r="F98" s="11"/>
       <c r="G98" s="12"/>
       <c r="H98" s="12"/>
@@ -4239,38 +4242,38 @@
     </row>
     <row r="99" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="100" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="33" t="s">
+      <c r="A100" s="42" t="s">
         <v>148</v>
       </c>
-      <c r="B100" s="33"/>
-      <c r="C100" s="33"/>
-      <c r="D100" s="33"/>
-      <c r="E100" s="33"/>
-      <c r="F100" s="33"/>
-      <c r="G100" s="33"/>
-      <c r="H100" s="33"/>
-      <c r="I100" s="33"/>
-      <c r="J100" s="33"/>
-      <c r="K100" s="33"/>
-      <c r="L100" s="33"/>
-      <c r="M100" s="33"/>
+      <c r="B100" s="42"/>
+      <c r="C100" s="42"/>
+      <c r="D100" s="42"/>
+      <c r="E100" s="42"/>
+      <c r="F100" s="42"/>
+      <c r="G100" s="42"/>
+      <c r="H100" s="42"/>
+      <c r="I100" s="42"/>
+      <c r="J100" s="42"/>
+      <c r="K100" s="42"/>
+      <c r="L100" s="42"/>
+      <c r="M100" s="42"/>
     </row>
     <row r="101" spans="1:13" ht="35.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="23"/>
-      <c r="B101" s="29" t="s">
+      <c r="B101" s="51" t="s">
         <v>236</v>
       </c>
-      <c r="C101" s="29"/>
-      <c r="D101" s="29"/>
-      <c r="E101" s="29"/>
-      <c r="F101" s="29"/>
-      <c r="G101" s="29"/>
-      <c r="H101" s="29"/>
-      <c r="I101" s="29"/>
-      <c r="J101" s="29"/>
-      <c r="K101" s="29"/>
-      <c r="L101" s="29"/>
-      <c r="M101" s="29"/>
+      <c r="C101" s="51"/>
+      <c r="D101" s="51"/>
+      <c r="E101" s="51"/>
+      <c r="F101" s="51"/>
+      <c r="G101" s="51"/>
+      <c r="H101" s="51"/>
+      <c r="I101" s="51"/>
+      <c r="J101" s="51"/>
+      <c r="K101" s="51"/>
+      <c r="L101" s="51"/>
+      <c r="M101" s="51"/>
     </row>
     <row r="102" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="8" t="s">
@@ -4361,38 +4364,38 @@
     </row>
     <row r="105" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="106" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="31" t="s">
+      <c r="A106" s="29" t="s">
         <v>149</v>
       </c>
-      <c r="B106" s="31"/>
-      <c r="C106" s="31"/>
-      <c r="D106" s="31"/>
-      <c r="E106" s="31"/>
-      <c r="F106" s="31"/>
-      <c r="G106" s="31"/>
-      <c r="H106" s="31"/>
-      <c r="I106" s="31"/>
-      <c r="J106" s="31"/>
-      <c r="K106" s="31"/>
-      <c r="L106" s="31"/>
-      <c r="M106" s="31"/>
+      <c r="B106" s="29"/>
+      <c r="C106" s="29"/>
+      <c r="D106" s="29"/>
+      <c r="E106" s="29"/>
+      <c r="F106" s="29"/>
+      <c r="G106" s="29"/>
+      <c r="H106" s="29"/>
+      <c r="I106" s="29"/>
+      <c r="J106" s="29"/>
+      <c r="K106" s="29"/>
+      <c r="L106" s="29"/>
+      <c r="M106" s="29"/>
     </row>
     <row r="107" spans="1:13" s="3" customFormat="1" ht="36.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="23"/>
-      <c r="B107" s="29" t="s">
+      <c r="B107" s="51" t="s">
         <v>237</v>
       </c>
-      <c r="C107" s="29"/>
-      <c r="D107" s="29"/>
-      <c r="E107" s="29"/>
-      <c r="F107" s="29"/>
-      <c r="G107" s="29"/>
-      <c r="H107" s="29"/>
-      <c r="I107" s="29"/>
-      <c r="J107" s="29"/>
-      <c r="K107" s="29"/>
-      <c r="L107" s="29"/>
-      <c r="M107" s="29"/>
+      <c r="C107" s="51"/>
+      <c r="D107" s="51"/>
+      <c r="E107" s="51"/>
+      <c r="F107" s="51"/>
+      <c r="G107" s="51"/>
+      <c r="H107" s="51"/>
+      <c r="I107" s="51"/>
+      <c r="J107" s="51"/>
+      <c r="K107" s="51"/>
+      <c r="L107" s="51"/>
+      <c r="M107" s="51"/>
     </row>
     <row r="108" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="8" t="s">
@@ -4502,21 +4505,21 @@
     </row>
     <row r="112" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="113" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="31" t="s">
+      <c r="A113" s="29" t="s">
         <v>151</v>
       </c>
-      <c r="B113" s="31"/>
-      <c r="C113" s="31"/>
-      <c r="D113" s="31"/>
-      <c r="E113" s="31"/>
-      <c r="F113" s="31"/>
-      <c r="G113" s="31"/>
-      <c r="H113" s="31"/>
-      <c r="I113" s="31"/>
-      <c r="J113" s="31"/>
-      <c r="K113" s="31"/>
-      <c r="L113" s="31"/>
-      <c r="M113" s="31"/>
+      <c r="B113" s="29"/>
+      <c r="C113" s="29"/>
+      <c r="D113" s="29"/>
+      <c r="E113" s="29"/>
+      <c r="F113" s="29"/>
+      <c r="G113" s="29"/>
+      <c r="H113" s="29"/>
+      <c r="I113" s="29"/>
+      <c r="J113" s="29"/>
+      <c r="K113" s="29"/>
+      <c r="L113" s="29"/>
+      <c r="M113" s="29"/>
     </row>
     <row r="114" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="8" t="s">
@@ -4590,38 +4593,38 @@
     </row>
     <row r="116" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="117" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="31" t="s">
+      <c r="A117" s="29" t="s">
         <v>159</v>
       </c>
-      <c r="B117" s="31"/>
-      <c r="C117" s="31"/>
-      <c r="D117" s="31"/>
-      <c r="E117" s="31"/>
-      <c r="F117" s="31"/>
-      <c r="G117" s="31"/>
-      <c r="H117" s="31"/>
-      <c r="I117" s="31"/>
-      <c r="J117" s="31"/>
-      <c r="K117" s="31"/>
-      <c r="L117" s="31"/>
-      <c r="M117" s="31"/>
+      <c r="B117" s="29"/>
+      <c r="C117" s="29"/>
+      <c r="D117" s="29"/>
+      <c r="E117" s="29"/>
+      <c r="F117" s="29"/>
+      <c r="G117" s="29"/>
+      <c r="H117" s="29"/>
+      <c r="I117" s="29"/>
+      <c r="J117" s="29"/>
+      <c r="K117" s="29"/>
+      <c r="L117" s="29"/>
+      <c r="M117" s="29"/>
     </row>
     <row r="118" spans="1:13" ht="63.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="26"/>
-      <c r="B118" s="30" t="s">
+      <c r="B118" s="60" t="s">
         <v>241</v>
       </c>
-      <c r="C118" s="30"/>
-      <c r="D118" s="30"/>
-      <c r="E118" s="30"/>
-      <c r="F118" s="30"/>
-      <c r="G118" s="30"/>
-      <c r="H118" s="30"/>
-      <c r="I118" s="30"/>
-      <c r="J118" s="30"/>
-      <c r="K118" s="30"/>
-      <c r="L118" s="30"/>
-      <c r="M118" s="30"/>
+      <c r="C118" s="60"/>
+      <c r="D118" s="60"/>
+      <c r="E118" s="60"/>
+      <c r="F118" s="60"/>
+      <c r="G118" s="60"/>
+      <c r="H118" s="60"/>
+      <c r="I118" s="60"/>
+      <c r="J118" s="60"/>
+      <c r="K118" s="60"/>
+      <c r="L118" s="60"/>
+      <c r="M118" s="60"/>
     </row>
     <row r="119" spans="1:13" s="4" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="8" t="s">
@@ -4724,38 +4727,38 @@
     </row>
     <row r="122" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="123" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="31" t="s">
+      <c r="A123" s="29" t="s">
         <v>172</v>
       </c>
-      <c r="B123" s="31"/>
-      <c r="C123" s="31"/>
-      <c r="D123" s="31"/>
-      <c r="E123" s="31"/>
-      <c r="F123" s="31"/>
-      <c r="G123" s="31"/>
-      <c r="H123" s="31"/>
-      <c r="I123" s="31"/>
-      <c r="J123" s="31"/>
-      <c r="K123" s="31"/>
-      <c r="L123" s="31"/>
-      <c r="M123" s="31"/>
+      <c r="B123" s="29"/>
+      <c r="C123" s="29"/>
+      <c r="D123" s="29"/>
+      <c r="E123" s="29"/>
+      <c r="F123" s="29"/>
+      <c r="G123" s="29"/>
+      <c r="H123" s="29"/>
+      <c r="I123" s="29"/>
+      <c r="J123" s="29"/>
+      <c r="K123" s="29"/>
+      <c r="L123" s="29"/>
+      <c r="M123" s="29"/>
     </row>
     <row r="124" spans="1:13" ht="69.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="26"/>
-      <c r="B124" s="30" t="s">
+      <c r="B124" s="60" t="s">
         <v>242</v>
       </c>
-      <c r="C124" s="30"/>
-      <c r="D124" s="30"/>
-      <c r="E124" s="30"/>
-      <c r="F124" s="30"/>
-      <c r="G124" s="30"/>
-      <c r="H124" s="30"/>
-      <c r="I124" s="30"/>
-      <c r="J124" s="30"/>
-      <c r="K124" s="30"/>
-      <c r="L124" s="30"/>
-      <c r="M124" s="30"/>
+      <c r="C124" s="60"/>
+      <c r="D124" s="60"/>
+      <c r="E124" s="60"/>
+      <c r="F124" s="60"/>
+      <c r="G124" s="60"/>
+      <c r="H124" s="60"/>
+      <c r="I124" s="60"/>
+      <c r="J124" s="60"/>
+      <c r="K124" s="60"/>
+      <c r="L124" s="60"/>
+      <c r="M124" s="60"/>
     </row>
     <row r="125" spans="1:13" s="4" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="10" t="s">
@@ -4857,38 +4860,38 @@
       <c r="M127" s="11"/>
     </row>
     <row r="129" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="32" t="s">
+      <c r="A129" s="61" t="s">
         <v>239</v>
       </c>
-      <c r="B129" s="32"/>
-      <c r="C129" s="32"/>
-      <c r="D129" s="32"/>
-      <c r="E129" s="32"/>
-      <c r="F129" s="32"/>
-      <c r="G129" s="32"/>
-      <c r="H129" s="32"/>
-      <c r="I129" s="32"/>
-      <c r="J129" s="32"/>
-      <c r="K129" s="32"/>
-      <c r="L129" s="32"/>
-      <c r="M129" s="32"/>
+      <c r="B129" s="61"/>
+      <c r="C129" s="61"/>
+      <c r="D129" s="61"/>
+      <c r="E129" s="61"/>
+      <c r="F129" s="61"/>
+      <c r="G129" s="61"/>
+      <c r="H129" s="61"/>
+      <c r="I129" s="61"/>
+      <c r="J129" s="61"/>
+      <c r="K129" s="61"/>
+      <c r="L129" s="61"/>
+      <c r="M129" s="61"/>
     </row>
     <row r="130" spans="1:13" s="3" customFormat="1" ht="51.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="26"/>
-      <c r="B130" s="30" t="s">
+      <c r="B130" s="60" t="s">
         <v>240</v>
       </c>
-      <c r="C130" s="30"/>
-      <c r="D130" s="30"/>
-      <c r="E130" s="30"/>
-      <c r="F130" s="30"/>
-      <c r="G130" s="30"/>
-      <c r="H130" s="30"/>
-      <c r="I130" s="30"/>
-      <c r="J130" s="30"/>
-      <c r="K130" s="30"/>
-      <c r="L130" s="30"/>
-      <c r="M130" s="30"/>
+      <c r="C130" s="60"/>
+      <c r="D130" s="60"/>
+      <c r="E130" s="60"/>
+      <c r="F130" s="60"/>
+      <c r="G130" s="60"/>
+      <c r="H130" s="60"/>
+      <c r="I130" s="60"/>
+      <c r="J130" s="60"/>
+      <c r="K130" s="60"/>
+      <c r="L130" s="60"/>
+      <c r="M130" s="60"/>
     </row>
     <row r="131" spans="1:13" s="4" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="8" t="s">
@@ -4959,37 +4962,14 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="A75:M75"/>
-    <mergeCell ref="A80:M80"/>
-    <mergeCell ref="A85:M85"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="G72:H72"/>
-    <mergeCell ref="G73:H73"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="E72:F72"/>
-    <mergeCell ref="E73:F73"/>
-    <mergeCell ref="A100:M100"/>
-    <mergeCell ref="A106:M106"/>
-    <mergeCell ref="D91:F91"/>
-    <mergeCell ref="D92:F92"/>
-    <mergeCell ref="C97:E97"/>
-    <mergeCell ref="C96:E96"/>
-    <mergeCell ref="C98:E98"/>
-    <mergeCell ref="B101:M101"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A39:M39"/>
-    <mergeCell ref="A50:M50"/>
-    <mergeCell ref="A54:M54"/>
-    <mergeCell ref="A28:M28"/>
-    <mergeCell ref="B11:M11"/>
-    <mergeCell ref="B40:M40"/>
-    <mergeCell ref="B29:M29"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="N8:P8"/>
-    <mergeCell ref="A10:M10"/>
-    <mergeCell ref="B6:M6"/>
-    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="B107:M107"/>
+    <mergeCell ref="B118:M118"/>
+    <mergeCell ref="B130:M130"/>
+    <mergeCell ref="B124:M124"/>
+    <mergeCell ref="A123:M123"/>
+    <mergeCell ref="A113:M113"/>
+    <mergeCell ref="A117:M117"/>
+    <mergeCell ref="A129:M129"/>
     <mergeCell ref="B55:M55"/>
     <mergeCell ref="B65:M65"/>
     <mergeCell ref="A70:M70"/>
@@ -5006,14 +4986,37 @@
     <mergeCell ref="I72:J72"/>
     <mergeCell ref="I73:J73"/>
     <mergeCell ref="A90:M90"/>
-    <mergeCell ref="B107:M107"/>
-    <mergeCell ref="B118:M118"/>
-    <mergeCell ref="B130:M130"/>
-    <mergeCell ref="B124:M124"/>
-    <mergeCell ref="A123:M123"/>
-    <mergeCell ref="A113:M113"/>
-    <mergeCell ref="A117:M117"/>
-    <mergeCell ref="A129:M129"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="N8:P8"/>
+    <mergeCell ref="A10:M10"/>
+    <mergeCell ref="B6:M6"/>
+    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A39:M39"/>
+    <mergeCell ref="A50:M50"/>
+    <mergeCell ref="A54:M54"/>
+    <mergeCell ref="A28:M28"/>
+    <mergeCell ref="B11:M11"/>
+    <mergeCell ref="B40:M40"/>
+    <mergeCell ref="B29:M29"/>
+    <mergeCell ref="A100:M100"/>
+    <mergeCell ref="A106:M106"/>
+    <mergeCell ref="D91:F91"/>
+    <mergeCell ref="D92:F92"/>
+    <mergeCell ref="C97:E97"/>
+    <mergeCell ref="C96:E96"/>
+    <mergeCell ref="C98:E98"/>
+    <mergeCell ref="B101:M101"/>
+    <mergeCell ref="A75:M75"/>
+    <mergeCell ref="A80:M80"/>
+    <mergeCell ref="A85:M85"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="G72:H72"/>
+    <mergeCell ref="G73:H73"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="E72:F72"/>
+    <mergeCell ref="E73:F73"/>
   </mergeCells>
   <dataValidations count="59">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -5230,7 +5233,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C2:C11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5287,7 +5290,7 @@
         <v>89</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>103</v>
+        <v>245</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -5295,7 +5298,7 @@
         <v>90</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -5303,7 +5306,7 @@
         <v>91</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -5311,15 +5314,15 @@
         <v>92</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C9" s="1">
-        <v>9504</v>
+      <c r="C9" s="1" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -5327,7 +5330,7 @@
         <v>94</v>
       </c>
       <c r="C10" s="1">
-        <v>9508</v>
+        <v>9504</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -5335,12 +5338,15 @@
         <v>95</v>
       </c>
       <c r="C11" s="1">
-        <v>9516</v>
+        <v>9508</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>96</v>
+      </c>
+      <c r="C12" s="1">
+        <v>9516</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changed Tenant Support to more than net centric
</commit_message>
<xml_diff>
--- a/deploy-fabric-Input-Spreadsheet.xlsx
+++ b/deploy-fabric-Input-Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\tyscott\terraform-aci-fabric-deploy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7139621-DB50-4E4B-9291-E5DAB86C51A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F0FCB0F-3469-41F7-9ECD-7212F5B0A9CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1137,7 +1137,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode=";;;"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1311,8 +1311,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF44546A"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF44546A"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF44546A"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1516,8 +1535,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E1F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="30">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -1662,36 +1686,6 @@
         <color theme="4" tint="0.39994506668294322"/>
       </right>
       <top style="medium">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="medium">
-        <color theme="4" tint="0.39991454817346722"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="4" tint="0.39994506668294322"/>
-      </left>
-      <right style="medium">
-        <color theme="4" tint="0.39994506668294322"/>
-      </right>
-      <top style="medium">
-        <color theme="4" tint="0.39991454817346722"/>
-      </top>
-      <bottom style="medium">
-        <color theme="4" tint="0.39994506668294322"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="4" tint="0.39994506668294322"/>
-      </left>
-      <right style="medium">
-        <color theme="4" tint="0.39994506668294322"/>
-      </right>
-      <top style="medium">
         <color theme="4" tint="0.39994506668294322"/>
       </top>
       <bottom style="medium">
@@ -1751,43 +1745,6 @@
         <color theme="4" tint="0.39994506668294322"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="4" tint="0.39994506668294322"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="medium">
-        <color theme="4" tint="0.39994506668294322"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="medium">
-        <color theme="4" tint="0.39994506668294322"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color theme="4" tint="0.39994506668294322"/>
-      </right>
-      <top style="medium">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="medium">
-        <color theme="4" tint="0.39994506668294322"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1884,8 +1841,123 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF8EA9DB"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF8EA9DB"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF8EA9DB"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF8EA9DB"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF8EA9DB"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="4" tint="0.39994506668294322"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF8EA9DB"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="4" tint="0.39994506668294322"/>
+      </right>
+      <top style="medium">
+        <color theme="4" tint="0.39994506668294322"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF8EA9DB"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF8EA9DB"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF8EA9DB"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF8EA9DB"/>
+      </right>
+      <top style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF8EA9DB"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF8EA9DB"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF8EA9DB"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF8EA9DB"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF8EA9DB"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF8EA9DB"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF8EA9DB"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF8EA9DB"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF8EA9DB"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF8EA9DB"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="44">
+  <cellStyleXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="49" fontId="17" fillId="33" borderId="8" applyAlignment="0" applyProtection="0"/>
@@ -1930,8 +2002,14 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="35" borderId="8" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="37" borderId="25">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="25">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="17" fillId="33" borderId="8" xfId="2" applyNumberFormat="1"/>
@@ -1950,170 +2028,176 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="12" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="13" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="8" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="33" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="34" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="33" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="34" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="34" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="37" borderId="25" xfId="44" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="37" borderId="25" xfId="44" applyNumberFormat="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="34" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="37" borderId="25" xfId="44">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="25" xfId="45" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="0" borderId="25" xfId="45" applyNumberFormat="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="25" xfId="45">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="25" xfId="45" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="37" borderId="25" xfId="44" applyNumberFormat="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="25" xfId="45" applyNumberFormat="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="33" borderId="8" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="30" xfId="45" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="31" xfId="45" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="21" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="37" borderId="26" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="37" borderId="27" xfId="44" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="37" borderId="28" xfId="44" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="37" borderId="29" xfId="44" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="33" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="13" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="14" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="37" borderId="32" xfId="44" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="33" xfId="45" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="34" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="17" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="18" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="19" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="19" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="19" fillId="34" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="19" fillId="34" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="19" fillId="34" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="19" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="27" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="8" xfId="3" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="33" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="34" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="33" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="34" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="34" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="34" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="33" borderId="8" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="25" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="26" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="20" fillId="34" borderId="22" xfId="43" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="19" fillId="34" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="19" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="19" fillId="34" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="19" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="19" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="34" borderId="22" xfId="43" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="33" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="19" fillId="34" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="34" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="23" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="24" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="28" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="23" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="18" fillId="34" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="34" borderId="29" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="34" borderId="24" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="17" fillId="36" borderId="8" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="23" fillId="37" borderId="25" xfId="44" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="37" borderId="25" xfId="44" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="25" xfId="45" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="37" borderId="26" xfId="43" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="37" borderId="27" xfId="44" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="25" fillId="34" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="25" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="44">
+  <cellStyles count="46">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -2158,6 +2242,8 @@
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="ws_even" xfId="45" xr:uid="{91AD35C5-FC4E-4620-A7A5-CB67461C9E9F}"/>
+    <cellStyle name="ws_odd" xfId="44" xr:uid="{0CA9025F-5804-4CA3-88B6-FF827C0201FD}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2471,8 +2557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P133"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14:D26"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C115" sqref="C115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2497,21 +2583,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
     </row>
     <row r="2" spans="1:16" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -2533,63 +2619,63 @@
       <c r="M2" s="8"/>
     </row>
     <row r="3" spans="1:16" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="20">
         <v>100</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
     </row>
     <row r="5" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="39" t="s">
         <v>202</v>
       </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="42"/>
-      <c r="K5" s="42"/>
-      <c r="L5" s="42"/>
-      <c r="M5" s="42"/>
-      <c r="N5" s="22"/>
-      <c r="O5" s="22"/>
-      <c r="P5" s="22"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="39"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
     </row>
     <row r="6" spans="1:16" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="20"/>
-      <c r="B6" s="58" t="s">
+      <c r="A6" s="12"/>
+      <c r="B6" s="53" t="s">
         <v>238</v>
       </c>
-      <c r="C6" s="58"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="58"/>
-      <c r="G6" s="58"/>
-      <c r="H6" s="58"/>
-      <c r="I6" s="58"/>
-      <c r="J6" s="58"/>
-      <c r="K6" s="58"/>
-      <c r="L6" s="58"/>
-      <c r="M6" s="58"/>
-      <c r="N6" s="20"/>
-      <c r="O6" s="20"/>
-      <c r="P6" s="20"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="53"/>
+      <c r="L6" s="53"/>
+      <c r="M6" s="53"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
     </row>
     <row r="7" spans="1:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
@@ -2631,87 +2717,87 @@
       <c r="M7" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="N7" s="53" t="s">
+      <c r="N7" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="O7" s="54"/>
-      <c r="P7" s="55"/>
+      <c r="O7" s="48"/>
+      <c r="P7" s="49"/>
     </row>
     <row r="8" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="19" t="s">
         <v>203</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="28" t="s">
         <v>208</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="57">
         <v>0</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="57">
         <v>15</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="22" t="s">
         <v>209</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="22" t="s">
         <v>211</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="H8" s="58" t="s">
         <v>220</v>
       </c>
-      <c r="I8" s="14">
+      <c r="I8" s="57">
         <v>22</v>
       </c>
-      <c r="J8" s="13" t="s">
+      <c r="J8" s="22" t="s">
         <v>218</v>
       </c>
-      <c r="K8" s="13" t="s">
+      <c r="K8" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="L8" s="27" t="s">
+      <c r="L8" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="M8" s="27"/>
-      <c r="N8" s="56"/>
-      <c r="O8" s="57"/>
-      <c r="P8" s="41"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="50"/>
+      <c r="O8" s="51"/>
+      <c r="P8" s="52"/>
     </row>
     <row r="10" spans="1:16" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="29"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
     </row>
     <row r="11" spans="1:16" s="6" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="21"/>
-      <c r="B11" s="52" t="s">
+      <c r="A11" s="13"/>
+      <c r="B11" s="46" t="s">
         <v>225</v>
       </c>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="52"/>
-      <c r="H11" s="52"/>
-      <c r="I11" s="52"/>
-      <c r="J11" s="52"/>
-      <c r="K11" s="52"/>
-      <c r="L11" s="52"/>
-      <c r="M11" s="52"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="46"/>
+      <c r="K11" s="46"/>
+      <c r="L11" s="46"/>
+      <c r="M11" s="46"/>
     </row>
     <row r="12" spans="1:16" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
@@ -2753,320 +2839,320 @@
       <c r="M12" s="8"/>
     </row>
     <row r="13" spans="1:16" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="57">
         <v>101</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="F13" s="14">
+      <c r="F13" s="57">
         <v>1</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="14">
+      <c r="H13" s="22">
         <v>9508</v>
       </c>
-      <c r="I13" s="13" t="s">
+      <c r="I13" s="22" t="s">
         <v>194</v>
       </c>
-      <c r="J13" s="13" t="s">
+      <c r="J13" s="22" t="s">
         <v>189</v>
       </c>
-      <c r="K13" s="13" t="s">
+      <c r="K13" s="22" t="s">
         <v>195</v>
       </c>
-      <c r="L13" s="13" t="s">
+      <c r="L13" s="22" t="s">
         <v>191</v>
       </c>
-      <c r="M13" s="13"/>
+      <c r="M13" s="22"/>
     </row>
     <row r="14" spans="1:16" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="27">
         <v>201</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14" s="27">
         <v>1</v>
       </c>
-      <c r="G14" s="12" t="s">
+      <c r="G14" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="H14" s="12" t="s">
+      <c r="H14" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="I14" s="11" t="s">
+      <c r="I14" s="26" t="s">
         <v>188</v>
       </c>
-      <c r="J14" s="11" t="s">
+      <c r="J14" s="26" t="s">
         <v>189</v>
       </c>
-      <c r="K14" s="11" t="s">
+      <c r="K14" s="27" t="s">
         <v>190</v>
       </c>
-      <c r="L14" s="11" t="s">
+      <c r="L14" s="26" t="s">
         <v>191</v>
       </c>
-      <c r="M14" s="11"/>
+      <c r="M14" s="26"/>
     </row>
     <row r="15" spans="1:16" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="57">
         <v>202</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="F15" s="14">
+      <c r="F15" s="57">
         <v>1</v>
       </c>
-      <c r="G15" s="14" t="s">
+      <c r="G15" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="H15" s="14" t="s">
+      <c r="H15" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="I15" s="13" t="s">
+      <c r="I15" s="22" t="s">
         <v>192</v>
       </c>
-      <c r="J15" s="13" t="s">
+      <c r="J15" s="22" t="s">
         <v>189</v>
       </c>
-      <c r="K15" s="13" t="s">
+      <c r="K15" s="22" t="s">
         <v>193</v>
       </c>
-      <c r="L15" s="13" t="s">
+      <c r="L15" s="22" t="s">
         <v>191</v>
       </c>
-      <c r="M15" s="13"/>
+      <c r="M15" s="22"/>
     </row>
     <row r="16" spans="1:16" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
+      <c r="A16" s="23"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="26"/>
+      <c r="M16" s="26"/>
     </row>
     <row r="17" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
+      <c r="A17" s="19"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="57"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
     </row>
     <row r="18" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="11"/>
-      <c r="M18" s="11"/>
+      <c r="A18" s="23"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="26"/>
+      <c r="M18" s="26"/>
     </row>
     <row r="19" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="13"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
+      <c r="A19" s="19"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="57"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="22"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="22"/>
     </row>
     <row r="20" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
-      <c r="M20" s="11"/>
+      <c r="A20" s="23"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="26"/>
+      <c r="M20" s="26"/>
     </row>
     <row r="21" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="13"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
+      <c r="A21" s="19"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="57"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="22"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="22"/>
     </row>
     <row r="22" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="11"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="11"/>
+      <c r="A22" s="23"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="26"/>
+      <c r="M22" s="26"/>
     </row>
     <row r="23" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="13"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="57"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="22"/>
+      <c r="L23" s="22"/>
+      <c r="M23" s="22"/>
     </row>
     <row r="24" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="11"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
-      <c r="M24" s="11"/>
+      <c r="A24" s="23"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="27"/>
+      <c r="L24" s="26"/>
+      <c r="M24" s="26"/>
     </row>
     <row r="25" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="13"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
+      <c r="A25" s="19"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="57"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="22"/>
+      <c r="L25" s="22"/>
+      <c r="M25" s="22"/>
     </row>
     <row r="26" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="11"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="11"/>
-      <c r="L26" s="11"/>
-      <c r="M26" s="11"/>
+      <c r="A26" s="23"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="26"/>
+      <c r="K26" s="27"/>
+      <c r="L26" s="26"/>
+      <c r="M26" s="26"/>
     </row>
     <row r="28" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="30" t="s">
         <v>243</v>
       </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
-      <c r="K28" s="29"/>
-      <c r="L28" s="29"/>
-      <c r="M28" s="29"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="30"/>
+      <c r="K28" s="30"/>
+      <c r="L28" s="30"/>
+      <c r="M28" s="30"/>
     </row>
     <row r="29" spans="1:13" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="21"/>
-      <c r="B29" s="52" t="s">
+      <c r="A29" s="13"/>
+      <c r="B29" s="46" t="s">
         <v>244</v>
       </c>
-      <c r="C29" s="52"/>
-      <c r="D29" s="52"/>
-      <c r="E29" s="52"/>
-      <c r="F29" s="52"/>
-      <c r="G29" s="52"/>
-      <c r="H29" s="52"/>
-      <c r="I29" s="52"/>
-      <c r="J29" s="52"/>
-      <c r="K29" s="52"/>
-      <c r="L29" s="52"/>
-      <c r="M29" s="52"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
+      <c r="J29" s="46"/>
+      <c r="K29" s="46"/>
+      <c r="L29" s="46"/>
+      <c r="M29" s="46"/>
     </row>
     <row r="30" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
@@ -3094,153 +3180,153 @@
       <c r="M30" s="8"/>
     </row>
     <row r="31" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="19" t="s">
         <v>177</v>
       </c>
-      <c r="B31" s="14">
+      <c r="B31" s="20">
         <v>201</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="D31" s="14">
+      <c r="D31" s="57">
         <v>201</v>
       </c>
-      <c r="E31" s="14">
+      <c r="E31" s="57">
         <v>202</v>
       </c>
-      <c r="F31" s="13"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="13"/>
-      <c r="J31" s="13"/>
-      <c r="K31" s="13"/>
-      <c r="L31" s="13"/>
-      <c r="M31" s="13"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="22"/>
+      <c r="L31" s="22"/>
+      <c r="M31" s="22"/>
     </row>
     <row r="32" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="11"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11"/>
-      <c r="K32" s="11"/>
-      <c r="L32" s="11"/>
-      <c r="M32" s="11"/>
+      <c r="A32" s="23"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="26"/>
+      <c r="J32" s="26"/>
+      <c r="K32" s="27"/>
+      <c r="L32" s="26"/>
+      <c r="M32" s="26"/>
     </row>
     <row r="33" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="13"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="13"/>
-      <c r="L33" s="13"/>
-      <c r="M33" s="13"/>
+      <c r="A33" s="19"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="57"/>
+      <c r="E33" s="57"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="22"/>
+      <c r="K33" s="22"/>
+      <c r="L33" s="22"/>
+      <c r="M33" s="22"/>
     </row>
     <row r="34" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="11"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="11"/>
-      <c r="K34" s="11"/>
-      <c r="L34" s="11"/>
-      <c r="M34" s="11"/>
+      <c r="A34" s="23"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="26"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="26"/>
+      <c r="J34" s="26"/>
+      <c r="K34" s="27"/>
+      <c r="L34" s="26"/>
+      <c r="M34" s="26"/>
     </row>
     <row r="35" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="13"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="13"/>
-      <c r="K35" s="13"/>
-      <c r="L35" s="13"/>
-      <c r="M35" s="13"/>
+      <c r="A35" s="19"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="57"/>
+      <c r="E35" s="57"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="22"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="22"/>
+      <c r="L35" s="22"/>
+      <c r="M35" s="22"/>
     </row>
     <row r="36" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="11"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="12"/>
-      <c r="H36" s="12"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="11"/>
-      <c r="K36" s="11"/>
-      <c r="L36" s="11"/>
-      <c r="M36" s="11"/>
+      <c r="A36" s="23"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="25"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="26"/>
+      <c r="G36" s="26"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="26"/>
+      <c r="K36" s="27"/>
+      <c r="L36" s="26"/>
+      <c r="M36" s="26"/>
     </row>
     <row r="37" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="13"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="13"/>
-      <c r="J37" s="13"/>
-      <c r="K37" s="13"/>
-      <c r="L37" s="13"/>
-      <c r="M37" s="13"/>
+      <c r="A37" s="19"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="57"/>
+      <c r="E37" s="57"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="22"/>
+      <c r="J37" s="22"/>
+      <c r="K37" s="22"/>
+      <c r="L37" s="22"/>
+      <c r="M37" s="22"/>
     </row>
     <row r="39" spans="1:13" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="29" t="s">
+      <c r="A39" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="B39" s="29"/>
-      <c r="C39" s="29"/>
-      <c r="D39" s="29"/>
-      <c r="E39" s="29"/>
-      <c r="F39" s="29"/>
-      <c r="G39" s="29"/>
-      <c r="H39" s="29"/>
-      <c r="I39" s="29"/>
-      <c r="J39" s="29"/>
-      <c r="K39" s="29"/>
-      <c r="L39" s="29"/>
-      <c r="M39" s="29"/>
+      <c r="B39" s="30"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="30"/>
+      <c r="G39" s="30"/>
+      <c r="H39" s="30"/>
+      <c r="I39" s="30"/>
+      <c r="J39" s="30"/>
+      <c r="K39" s="30"/>
+      <c r="L39" s="30"/>
+      <c r="M39" s="30"/>
     </row>
     <row r="40" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="23"/>
-      <c r="B40" s="51" t="s">
+      <c r="A40" s="15"/>
+      <c r="B40" s="45" t="s">
         <v>226</v>
       </c>
-      <c r="C40" s="51"/>
-      <c r="D40" s="51"/>
-      <c r="E40" s="51"/>
-      <c r="F40" s="51"/>
-      <c r="G40" s="51"/>
-      <c r="H40" s="51"/>
-      <c r="I40" s="51"/>
-      <c r="J40" s="51"/>
-      <c r="K40" s="51"/>
-      <c r="L40" s="51"/>
-      <c r="M40" s="51"/>
+      <c r="C40" s="45"/>
+      <c r="D40" s="45"/>
+      <c r="E40" s="45"/>
+      <c r="F40" s="45"/>
+      <c r="G40" s="45"/>
+      <c r="H40" s="45"/>
+      <c r="I40" s="45"/>
+      <c r="J40" s="45"/>
+      <c r="K40" s="45"/>
+      <c r="L40" s="45"/>
+      <c r="M40" s="45"/>
     </row>
     <row r="41" spans="1:13" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="8" t="s">
@@ -3278,146 +3364,146 @@
       <c r="M41" s="8"/>
     </row>
     <row r="42" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="13" t="s">
+      <c r="A42" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B42" s="13" t="s">
+      <c r="B42" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C42" s="14">
+      <c r="C42" s="57">
         <v>1</v>
       </c>
-      <c r="D42" s="14">
+      <c r="D42" s="57">
         <v>1</v>
       </c>
-      <c r="E42" s="13" t="s">
+      <c r="E42" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="F42" s="13" t="s">
+      <c r="F42" s="22" t="s">
         <v>191</v>
       </c>
-      <c r="G42" s="14" t="s">
+      <c r="G42" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H42" s="14" t="s">
+      <c r="H42" s="58" t="s">
         <v>83</v>
       </c>
-      <c r="I42" s="13" t="s">
+      <c r="I42" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="J42" s="13" t="s">
+      <c r="J42" s="58" t="s">
         <v>83</v>
       </c>
-      <c r="K42" s="13"/>
-      <c r="L42" s="13"/>
-      <c r="M42" s="13"/>
+      <c r="K42" s="22"/>
+      <c r="L42" s="22"/>
+      <c r="M42" s="22"/>
     </row>
     <row r="43" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="11"/>
-      <c r="B43" s="11"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="11"/>
-      <c r="F43" s="11"/>
-      <c r="G43" s="12"/>
-      <c r="H43" s="12"/>
-      <c r="I43" s="11"/>
-      <c r="J43" s="11"/>
-      <c r="K43" s="11"/>
-      <c r="L43" s="11"/>
-      <c r="M43" s="11"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="24"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="26"/>
+      <c r="G43" s="26"/>
+      <c r="H43" s="59"/>
+      <c r="I43" s="26"/>
+      <c r="J43" s="59"/>
+      <c r="K43" s="27"/>
+      <c r="L43" s="26"/>
+      <c r="M43" s="26"/>
     </row>
     <row r="44" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="13"/>
-      <c r="B44" s="13"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="13"/>
-      <c r="J44" s="13"/>
-      <c r="K44" s="13"/>
-      <c r="L44" s="13"/>
-      <c r="M44" s="13"/>
+      <c r="A44" s="19"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="57"/>
+      <c r="D44" s="57"/>
+      <c r="E44" s="22"/>
+      <c r="F44" s="22"/>
+      <c r="G44" s="22"/>
+      <c r="H44" s="58"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="58"/>
+      <c r="K44" s="22"/>
+      <c r="L44" s="22"/>
+      <c r="M44" s="22"/>
     </row>
     <row r="45" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="11"/>
-      <c r="B45" s="11"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="12"/>
-      <c r="I45" s="11"/>
-      <c r="J45" s="11"/>
-      <c r="K45" s="11"/>
-      <c r="L45" s="11"/>
-      <c r="M45" s="11"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="24"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="27"/>
+      <c r="E45" s="26"/>
+      <c r="F45" s="26"/>
+      <c r="G45" s="26"/>
+      <c r="H45" s="59"/>
+      <c r="I45" s="26"/>
+      <c r="J45" s="59"/>
+      <c r="K45" s="27"/>
+      <c r="L45" s="26"/>
+      <c r="M45" s="26"/>
     </row>
     <row r="46" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="13"/>
-      <c r="B46" s="13"/>
-      <c r="C46" s="14"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="14"/>
-      <c r="H46" s="14"/>
-      <c r="I46" s="13"/>
-      <c r="J46" s="13"/>
-      <c r="K46" s="13"/>
-      <c r="L46" s="13"/>
-      <c r="M46" s="13"/>
+      <c r="A46" s="19"/>
+      <c r="B46" s="20"/>
+      <c r="C46" s="57"/>
+      <c r="D46" s="57"/>
+      <c r="E46" s="22"/>
+      <c r="F46" s="22"/>
+      <c r="G46" s="22"/>
+      <c r="H46" s="58"/>
+      <c r="I46" s="22"/>
+      <c r="J46" s="58"/>
+      <c r="K46" s="22"/>
+      <c r="L46" s="22"/>
+      <c r="M46" s="22"/>
     </row>
     <row r="47" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="11"/>
-      <c r="B47" s="11"/>
-      <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
-      <c r="G47" s="12"/>
-      <c r="H47" s="12"/>
-      <c r="I47" s="11"/>
-      <c r="J47" s="11"/>
-      <c r="K47" s="11"/>
-      <c r="L47" s="11"/>
-      <c r="M47" s="11"/>
+      <c r="A47" s="23"/>
+      <c r="B47" s="24"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="27"/>
+      <c r="E47" s="26"/>
+      <c r="F47" s="26"/>
+      <c r="G47" s="26"/>
+      <c r="H47" s="59"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="59"/>
+      <c r="K47" s="27"/>
+      <c r="L47" s="26"/>
+      <c r="M47" s="26"/>
     </row>
     <row r="48" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="13"/>
-      <c r="B48" s="13"/>
-      <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="13"/>
-      <c r="F48" s="13"/>
-      <c r="G48" s="14"/>
-      <c r="H48" s="14"/>
-      <c r="I48" s="13"/>
-      <c r="J48" s="13"/>
-      <c r="K48" s="13"/>
-      <c r="L48" s="13"/>
-      <c r="M48" s="13"/>
+      <c r="A48" s="19"/>
+      <c r="B48" s="20"/>
+      <c r="C48" s="57"/>
+      <c r="D48" s="57"/>
+      <c r="E48" s="22"/>
+      <c r="F48" s="22"/>
+      <c r="G48" s="22"/>
+      <c r="H48" s="58"/>
+      <c r="I48" s="22"/>
+      <c r="J48" s="58"/>
+      <c r="K48" s="22"/>
+      <c r="L48" s="22"/>
+      <c r="M48" s="22"/>
     </row>
     <row r="50" spans="1:13" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="29" t="s">
+      <c r="A50" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="B50" s="29"/>
-      <c r="C50" s="29"/>
-      <c r="D50" s="29"/>
-      <c r="E50" s="29"/>
-      <c r="F50" s="29"/>
-      <c r="G50" s="29"/>
-      <c r="H50" s="29"/>
-      <c r="I50" s="29"/>
-      <c r="J50" s="29"/>
-      <c r="K50" s="29"/>
-      <c r="L50" s="29"/>
-      <c r="M50" s="29"/>
+      <c r="B50" s="30"/>
+      <c r="C50" s="30"/>
+      <c r="D50" s="30"/>
+      <c r="E50" s="30"/>
+      <c r="F50" s="30"/>
+      <c r="G50" s="30"/>
+      <c r="H50" s="30"/>
+      <c r="I50" s="30"/>
+      <c r="J50" s="30"/>
+      <c r="K50" s="30"/>
+      <c r="L50" s="30"/>
+      <c r="M50" s="30"/>
     </row>
     <row r="51" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="8" t="s">
@@ -3439,57 +3525,57 @@
       <c r="M51" s="8"/>
     </row>
     <row r="52" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="13" t="s">
+      <c r="A52" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B52" s="14">
+      <c r="B52" s="57">
         <v>65513</v>
       </c>
-      <c r="C52" s="13"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="13"/>
-      <c r="F52" s="13"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="14"/>
-      <c r="I52" s="13"/>
-      <c r="J52" s="13"/>
-      <c r="K52" s="13"/>
-      <c r="L52" s="13"/>
-      <c r="M52" s="13"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="22"/>
+      <c r="E52" s="22"/>
+      <c r="F52" s="22"/>
+      <c r="G52" s="22"/>
+      <c r="H52" s="22"/>
+      <c r="I52" s="22"/>
+      <c r="J52" s="22"/>
+      <c r="K52" s="22"/>
+      <c r="L52" s="22"/>
+      <c r="M52" s="22"/>
     </row>
     <row r="54" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="29" t="s">
+      <c r="A54" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="B54" s="29"/>
-      <c r="C54" s="29"/>
-      <c r="D54" s="29"/>
-      <c r="E54" s="29"/>
-      <c r="F54" s="29"/>
-      <c r="G54" s="29"/>
-      <c r="H54" s="29"/>
-      <c r="I54" s="29"/>
-      <c r="J54" s="29"/>
-      <c r="K54" s="29"/>
-      <c r="L54" s="29"/>
-      <c r="M54" s="29"/>
+      <c r="B54" s="30"/>
+      <c r="C54" s="30"/>
+      <c r="D54" s="30"/>
+      <c r="E54" s="30"/>
+      <c r="F54" s="30"/>
+      <c r="G54" s="30"/>
+      <c r="H54" s="30"/>
+      <c r="I54" s="30"/>
+      <c r="J54" s="30"/>
+      <c r="K54" s="30"/>
+      <c r="L54" s="30"/>
+      <c r="M54" s="30"/>
     </row>
     <row r="55" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="23"/>
-      <c r="B55" s="51" t="s">
+      <c r="A55" s="15"/>
+      <c r="B55" s="45" t="s">
         <v>227</v>
       </c>
-      <c r="C55" s="51"/>
-      <c r="D55" s="51"/>
-      <c r="E55" s="51"/>
-      <c r="F55" s="51"/>
-      <c r="G55" s="51"/>
-      <c r="H55" s="51"/>
-      <c r="I55" s="51"/>
-      <c r="J55" s="51"/>
-      <c r="K55" s="51"/>
-      <c r="L55" s="51"/>
-      <c r="M55" s="51"/>
+      <c r="C55" s="45"/>
+      <c r="D55" s="45"/>
+      <c r="E55" s="45"/>
+      <c r="F55" s="45"/>
+      <c r="G55" s="45"/>
+      <c r="H55" s="45"/>
+      <c r="I55" s="45"/>
+      <c r="J55" s="45"/>
+      <c r="K55" s="45"/>
+      <c r="L55" s="45"/>
+      <c r="M55" s="45"/>
     </row>
     <row r="56" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="8" t="s">
@@ -3513,57 +3599,57 @@
       <c r="M56" s="8"/>
     </row>
     <row r="57" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="13" t="s">
+      <c r="A57" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B57" s="13" t="s">
+      <c r="B57" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C57" s="14">
+      <c r="C57" s="20">
         <v>101</v>
       </c>
-      <c r="D57" s="14"/>
-      <c r="E57" s="13"/>
-      <c r="F57" s="13"/>
-      <c r="G57" s="14"/>
-      <c r="H57" s="14"/>
-      <c r="I57" s="13"/>
-      <c r="J57" s="13"/>
-      <c r="K57" s="13"/>
-      <c r="L57" s="13"/>
-      <c r="M57" s="13"/>
+      <c r="D57" s="22"/>
+      <c r="E57" s="22"/>
+      <c r="F57" s="22"/>
+      <c r="G57" s="22"/>
+      <c r="H57" s="22"/>
+      <c r="I57" s="22"/>
+      <c r="J57" s="22"/>
+      <c r="K57" s="22"/>
+      <c r="L57" s="22"/>
+      <c r="M57" s="22"/>
     </row>
     <row r="58" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="11"/>
-      <c r="B58" s="11"/>
-      <c r="C58" s="12"/>
-      <c r="D58" s="12"/>
-      <c r="E58" s="11"/>
-      <c r="F58" s="11"/>
-      <c r="G58" s="12"/>
-      <c r="H58" s="12"/>
-      <c r="I58" s="11"/>
-      <c r="J58" s="11"/>
-      <c r="K58" s="11"/>
-      <c r="L58" s="11"/>
-      <c r="M58" s="11"/>
+      <c r="A58" s="23"/>
+      <c r="B58" s="24"/>
+      <c r="C58" s="24"/>
+      <c r="D58" s="26"/>
+      <c r="E58" s="26"/>
+      <c r="F58" s="26"/>
+      <c r="G58" s="26"/>
+      <c r="H58" s="26"/>
+      <c r="I58" s="26"/>
+      <c r="J58" s="26"/>
+      <c r="K58" s="27"/>
+      <c r="L58" s="26"/>
+      <c r="M58" s="26"/>
     </row>
     <row r="60" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="29" t="s">
+      <c r="A60" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="B60" s="29"/>
-      <c r="C60" s="29"/>
-      <c r="D60" s="29"/>
-      <c r="E60" s="29"/>
-      <c r="F60" s="29"/>
-      <c r="G60" s="29"/>
-      <c r="H60" s="29"/>
-      <c r="I60" s="29"/>
-      <c r="J60" s="29"/>
-      <c r="K60" s="29"/>
-      <c r="L60" s="29"/>
-      <c r="M60" s="29"/>
+      <c r="B60" s="30"/>
+      <c r="C60" s="30"/>
+      <c r="D60" s="30"/>
+      <c r="E60" s="30"/>
+      <c r="F60" s="30"/>
+      <c r="G60" s="30"/>
+      <c r="H60" s="30"/>
+      <c r="I60" s="30"/>
+      <c r="J60" s="30"/>
+      <c r="K60" s="30"/>
+      <c r="L60" s="30"/>
+      <c r="M60" s="30"/>
     </row>
     <row r="61" spans="1:13" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="8" t="s">
@@ -3585,57 +3671,57 @@
       <c r="M61" s="8"/>
     </row>
     <row r="62" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="13" t="s">
+      <c r="A62" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B62" s="15" t="s">
+      <c r="B62" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C62" s="14"/>
-      <c r="D62" s="14"/>
-      <c r="E62" s="13"/>
-      <c r="F62" s="13"/>
-      <c r="G62" s="14"/>
-      <c r="H62" s="14"/>
-      <c r="I62" s="13"/>
-      <c r="J62" s="13"/>
-      <c r="K62" s="13"/>
-      <c r="L62" s="13"/>
-      <c r="M62" s="13"/>
+      <c r="C62" s="21"/>
+      <c r="D62" s="22"/>
+      <c r="E62" s="22"/>
+      <c r="F62" s="22"/>
+      <c r="G62" s="22"/>
+      <c r="H62" s="22"/>
+      <c r="I62" s="22"/>
+      <c r="J62" s="22"/>
+      <c r="K62" s="22"/>
+      <c r="L62" s="22"/>
+      <c r="M62" s="22"/>
     </row>
     <row r="64" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="29" t="s">
+      <c r="A64" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="B64" s="29"/>
-      <c r="C64" s="29"/>
-      <c r="D64" s="29"/>
-      <c r="E64" s="29"/>
-      <c r="F64" s="29"/>
-      <c r="G64" s="29"/>
-      <c r="H64" s="29"/>
-      <c r="I64" s="29"/>
-      <c r="J64" s="29"/>
-      <c r="K64" s="29"/>
-      <c r="L64" s="29"/>
-      <c r="M64" s="29"/>
+      <c r="B64" s="30"/>
+      <c r="C64" s="30"/>
+      <c r="D64" s="30"/>
+      <c r="E64" s="30"/>
+      <c r="F64" s="30"/>
+      <c r="G64" s="30"/>
+      <c r="H64" s="30"/>
+      <c r="I64" s="30"/>
+      <c r="J64" s="30"/>
+      <c r="K64" s="30"/>
+      <c r="L64" s="30"/>
+      <c r="M64" s="30"/>
     </row>
     <row r="65" spans="1:16" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="23"/>
-      <c r="B65" s="51" t="s">
+      <c r="A65" s="15"/>
+      <c r="B65" s="45" t="s">
         <v>228</v>
       </c>
-      <c r="C65" s="51"/>
-      <c r="D65" s="51"/>
-      <c r="E65" s="51"/>
-      <c r="F65" s="51"/>
-      <c r="G65" s="51"/>
-      <c r="H65" s="51"/>
-      <c r="I65" s="51"/>
-      <c r="J65" s="51"/>
-      <c r="K65" s="51"/>
-      <c r="L65" s="51"/>
-      <c r="M65" s="51"/>
+      <c r="C65" s="45"/>
+      <c r="D65" s="45"/>
+      <c r="E65" s="45"/>
+      <c r="F65" s="45"/>
+      <c r="G65" s="45"/>
+      <c r="H65" s="45"/>
+      <c r="I65" s="45"/>
+      <c r="J65" s="45"/>
+      <c r="K65" s="45"/>
+      <c r="L65" s="45"/>
+      <c r="M65" s="45"/>
     </row>
     <row r="66" spans="1:16" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="8" t="s">
@@ -3659,86 +3745,86 @@
       <c r="M66" s="8"/>
     </row>
     <row r="67" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="13" t="s">
+      <c r="A67" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B67" s="13" t="s">
+      <c r="B67" s="20" t="s">
         <v>196</v>
       </c>
-      <c r="C67" s="13" t="s">
+      <c r="C67" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D67" s="14"/>
-      <c r="E67" s="13"/>
-      <c r="F67" s="13"/>
-      <c r="G67" s="14"/>
-      <c r="H67" s="14"/>
-      <c r="I67" s="13"/>
-      <c r="J67" s="13"/>
-      <c r="K67" s="13"/>
-      <c r="L67" s="13"/>
-      <c r="M67" s="13"/>
+      <c r="D67" s="22"/>
+      <c r="E67" s="22"/>
+      <c r="F67" s="22"/>
+      <c r="G67" s="22"/>
+      <c r="H67" s="22"/>
+      <c r="I67" s="22"/>
+      <c r="J67" s="22"/>
+      <c r="K67" s="22"/>
+      <c r="L67" s="22"/>
+      <c r="M67" s="22"/>
     </row>
     <row r="68" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="11" t="s">
+      <c r="A68" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B68" s="11" t="s">
+      <c r="B68" s="24" t="s">
         <v>197</v>
       </c>
-      <c r="C68" s="11" t="s">
+      <c r="C68" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="D68" s="12"/>
-      <c r="E68" s="11"/>
-      <c r="F68" s="11"/>
-      <c r="G68" s="12"/>
-      <c r="H68" s="12"/>
-      <c r="I68" s="11"/>
-      <c r="J68" s="11"/>
-      <c r="K68" s="11"/>
-      <c r="L68" s="11"/>
-      <c r="M68" s="11"/>
+      <c r="D68" s="26"/>
+      <c r="E68" s="26"/>
+      <c r="F68" s="26"/>
+      <c r="G68" s="26"/>
+      <c r="H68" s="26"/>
+      <c r="I68" s="26"/>
+      <c r="J68" s="26"/>
+      <c r="K68" s="27"/>
+      <c r="L68" s="26"/>
+      <c r="M68" s="26"/>
     </row>
     <row r="70" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="42" t="s">
+      <c r="A70" s="39" t="s">
         <v>120</v>
       </c>
-      <c r="B70" s="42"/>
-      <c r="C70" s="42"/>
-      <c r="D70" s="42"/>
-      <c r="E70" s="42"/>
-      <c r="F70" s="42"/>
-      <c r="G70" s="42"/>
-      <c r="H70" s="42"/>
-      <c r="I70" s="42"/>
-      <c r="J70" s="42"/>
-      <c r="K70" s="42"/>
-      <c r="L70" s="42"/>
-      <c r="M70" s="42"/>
-      <c r="N70" s="24"/>
-      <c r="O70" s="24"/>
-      <c r="P70" s="24"/>
+      <c r="B70" s="39"/>
+      <c r="C70" s="39"/>
+      <c r="D70" s="39"/>
+      <c r="E70" s="39"/>
+      <c r="F70" s="39"/>
+      <c r="G70" s="39"/>
+      <c r="H70" s="39"/>
+      <c r="I70" s="39"/>
+      <c r="J70" s="39"/>
+      <c r="K70" s="39"/>
+      <c r="L70" s="39"/>
+      <c r="M70" s="39"/>
+      <c r="N70" s="16"/>
+      <c r="O70" s="16"/>
+      <c r="P70" s="16"/>
     </row>
     <row r="71" spans="1:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="25"/>
-      <c r="B71" s="59" t="s">
+      <c r="A71" s="17"/>
+      <c r="B71" s="54" t="s">
         <v>229</v>
       </c>
-      <c r="C71" s="59"/>
-      <c r="D71" s="59"/>
-      <c r="E71" s="59"/>
-      <c r="F71" s="59"/>
-      <c r="G71" s="59"/>
-      <c r="H71" s="59"/>
-      <c r="I71" s="59"/>
-      <c r="J71" s="59"/>
-      <c r="K71" s="59"/>
-      <c r="L71" s="59"/>
-      <c r="M71" s="59"/>
-      <c r="N71" s="25"/>
-      <c r="O71" s="25"/>
-      <c r="P71" s="25"/>
+      <c r="C71" s="54"/>
+      <c r="D71" s="54"/>
+      <c r="E71" s="54"/>
+      <c r="F71" s="54"/>
+      <c r="G71" s="54"/>
+      <c r="H71" s="54"/>
+      <c r="I71" s="54"/>
+      <c r="J71" s="54"/>
+      <c r="K71" s="54"/>
+      <c r="L71" s="54"/>
+      <c r="M71" s="54"/>
+      <c r="N71" s="17"/>
+      <c r="O71" s="17"/>
+      <c r="P71" s="17"/>
     </row>
     <row r="72" spans="1:16" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="8" t="s">
@@ -3753,25 +3839,25 @@
       <c r="D72" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="E72" s="32" t="s">
+      <c r="E72" s="33" t="s">
         <v>131</v>
       </c>
-      <c r="F72" s="33"/>
-      <c r="G72" s="32" t="s">
+      <c r="F72" s="34"/>
+      <c r="G72" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="H72" s="33"/>
-      <c r="I72" s="32" t="s">
+      <c r="H72" s="34"/>
+      <c r="I72" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="J72" s="33"/>
+      <c r="J72" s="34"/>
       <c r="K72" s="8" t="s">
         <v>134</v>
       </c>
       <c r="L72" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="M72" s="18" t="s">
+      <c r="M72" s="11" t="s">
         <v>135</v>
       </c>
       <c r="N72" s="8" t="s">
@@ -3784,67 +3870,67 @@
         <v>138</v>
       </c>
     </row>
-    <row r="73" spans="1:16" s="4" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="13" t="s">
+    <row r="73" spans="1:16" s="4" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B73" s="14">
+      <c r="B73" s="20">
         <v>25</v>
       </c>
-      <c r="C73" s="13" t="s">
+      <c r="C73" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="D73" s="14" t="s">
+      <c r="D73" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="E73" s="40" t="s">
+      <c r="E73" s="60" t="s">
         <v>183</v>
       </c>
-      <c r="F73" s="41"/>
-      <c r="G73" s="34" t="s">
+      <c r="F73" s="61"/>
+      <c r="G73" s="60" t="s">
         <v>184</v>
       </c>
-      <c r="H73" s="35"/>
-      <c r="I73" s="34" t="s">
+      <c r="H73" s="61"/>
+      <c r="I73" s="60" t="s">
         <v>184</v>
       </c>
-      <c r="J73" s="35"/>
-      <c r="K73" s="13" t="s">
+      <c r="J73" s="61"/>
+      <c r="K73" s="21" t="s">
         <v>185</v>
       </c>
-      <c r="L73" s="14" t="s">
+      <c r="L73" s="58" t="s">
         <v>186</v>
       </c>
-      <c r="M73" s="19" t="s">
+      <c r="M73" s="21" t="s">
         <v>187</v>
       </c>
-      <c r="N73" s="13">
+      <c r="N73" s="58">
         <v>5555555</v>
       </c>
-      <c r="O73" s="13">
+      <c r="O73" s="21">
         <v>5555555</v>
       </c>
-      <c r="P73" s="13">
+      <c r="P73" s="58">
         <v>555555</v>
       </c>
     </row>
     <row r="74" spans="1:16" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="75" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="29" t="s">
+      <c r="A75" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="B75" s="29"/>
-      <c r="C75" s="29"/>
-      <c r="D75" s="29"/>
-      <c r="E75" s="29"/>
-      <c r="F75" s="29"/>
-      <c r="G75" s="29"/>
-      <c r="H75" s="29"/>
-      <c r="I75" s="29"/>
-      <c r="J75" s="29"/>
-      <c r="K75" s="29"/>
-      <c r="L75" s="29"/>
-      <c r="M75" s="29"/>
+      <c r="B75" s="30"/>
+      <c r="C75" s="30"/>
+      <c r="D75" s="30"/>
+      <c r="E75" s="30"/>
+      <c r="F75" s="30"/>
+      <c r="G75" s="30"/>
+      <c r="H75" s="30"/>
+      <c r="I75" s="30"/>
+      <c r="J75" s="30"/>
+      <c r="K75" s="30"/>
+      <c r="L75" s="30"/>
+      <c r="M75" s="30"/>
     </row>
     <row r="76" spans="1:16" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="8" t="s">
@@ -3870,80 +3956,80 @@
       <c r="M76" s="8"/>
     </row>
     <row r="77" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="13" t="s">
+      <c r="A77" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B77" s="13" t="s">
+      <c r="B77" s="20" t="s">
         <v>196</v>
       </c>
-      <c r="C77" s="13" t="s">
+      <c r="C77" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="D77" s="14" t="s">
+      <c r="D77" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="E77" s="13"/>
-      <c r="F77" s="13"/>
-      <c r="G77" s="14"/>
-      <c r="H77" s="14"/>
-      <c r="I77" s="13"/>
-      <c r="J77" s="13"/>
-      <c r="K77" s="13"/>
-      <c r="L77" s="13"/>
-      <c r="M77" s="13"/>
+      <c r="E77" s="22"/>
+      <c r="F77" s="22"/>
+      <c r="G77" s="22"/>
+      <c r="H77" s="22"/>
+      <c r="I77" s="22"/>
+      <c r="J77" s="22"/>
+      <c r="K77" s="22"/>
+      <c r="L77" s="22"/>
+      <c r="M77" s="22"/>
     </row>
     <row r="78" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="11" t="s">
+      <c r="A78" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="B78" s="11" t="s">
+      <c r="B78" s="24" t="s">
         <v>197</v>
       </c>
-      <c r="C78" s="11" t="s">
+      <c r="C78" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="D78" s="12" t="s">
+      <c r="D78" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="E78" s="11"/>
-      <c r="F78" s="11"/>
-      <c r="G78" s="12"/>
-      <c r="H78" s="12"/>
-      <c r="I78" s="11"/>
-      <c r="J78" s="11"/>
-      <c r="K78" s="11"/>
-      <c r="L78" s="11"/>
-      <c r="M78" s="11"/>
+      <c r="E78" s="26"/>
+      <c r="F78" s="26"/>
+      <c r="G78" s="26"/>
+      <c r="H78" s="26"/>
+      <c r="I78" s="26"/>
+      <c r="J78" s="26"/>
+      <c r="K78" s="27"/>
+      <c r="L78" s="26"/>
+      <c r="M78" s="26"/>
     </row>
     <row r="80" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="29" t="s">
+      <c r="A80" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="B80" s="29"/>
-      <c r="C80" s="29"/>
-      <c r="D80" s="29"/>
-      <c r="E80" s="29"/>
-      <c r="F80" s="29"/>
-      <c r="G80" s="29"/>
-      <c r="H80" s="29"/>
-      <c r="I80" s="29"/>
-      <c r="J80" s="29"/>
-      <c r="K80" s="29"/>
-      <c r="L80" s="29"/>
-      <c r="M80" s="29"/>
+      <c r="B80" s="30"/>
+      <c r="C80" s="30"/>
+      <c r="D80" s="30"/>
+      <c r="E80" s="30"/>
+      <c r="F80" s="30"/>
+      <c r="G80" s="30"/>
+      <c r="H80" s="30"/>
+      <c r="I80" s="30"/>
+      <c r="J80" s="30"/>
+      <c r="K80" s="30"/>
+      <c r="L80" s="30"/>
+      <c r="M80" s="30"/>
     </row>
     <row r="81" spans="1:13" s="3" customFormat="1" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B81" s="43" t="s">
+      <c r="B81" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="C81" s="45"/>
-      <c r="D81" s="43" t="s">
+      <c r="C81" s="42"/>
+      <c r="D81" s="40" t="s">
         <v>125</v>
       </c>
-      <c r="E81" s="45"/>
+      <c r="E81" s="42"/>
       <c r="F81" s="8"/>
       <c r="G81" s="8"/>
       <c r="H81" s="8"/>
@@ -3953,64 +4039,64 @@
       <c r="L81" s="8"/>
       <c r="M81" s="8"/>
     </row>
-    <row r="82" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="13" t="s">
+    <row r="82" spans="1:13" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B82" s="47" t="s">
+      <c r="B82" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="C82" s="49"/>
-      <c r="D82" s="36" t="s">
+      <c r="C82" s="38"/>
+      <c r="D82" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="E82" s="37"/>
-      <c r="F82" s="13"/>
-      <c r="G82" s="14"/>
-      <c r="H82" s="14"/>
-      <c r="I82" s="13"/>
-      <c r="J82" s="13"/>
-      <c r="K82" s="13"/>
-      <c r="L82" s="13"/>
-      <c r="M82" s="13"/>
+      <c r="E82" s="38"/>
+      <c r="F82" s="22"/>
+      <c r="G82" s="22"/>
+      <c r="H82" s="22"/>
+      <c r="I82" s="22"/>
+      <c r="J82" s="22"/>
+      <c r="K82" s="22"/>
+      <c r="L82" s="22"/>
+      <c r="M82" s="22"/>
     </row>
     <row r="83" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="11" t="s">
+      <c r="A83" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="B83" s="30" t="s">
+      <c r="B83" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="C83" s="31"/>
-      <c r="D83" s="38" t="s">
+      <c r="C83" s="32"/>
+      <c r="D83" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="E83" s="39"/>
-      <c r="F83" s="11"/>
-      <c r="G83" s="12"/>
-      <c r="H83" s="12"/>
-      <c r="I83" s="11"/>
-      <c r="J83" s="11"/>
-      <c r="K83" s="11"/>
-      <c r="L83" s="11"/>
-      <c r="M83" s="11"/>
+      <c r="E83" s="32"/>
+      <c r="F83" s="26"/>
+      <c r="G83" s="26"/>
+      <c r="H83" s="26"/>
+      <c r="I83" s="26"/>
+      <c r="J83" s="26"/>
+      <c r="K83" s="27"/>
+      <c r="L83" s="26"/>
+      <c r="M83" s="26"/>
     </row>
     <row r="85" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="29" t="s">
+      <c r="A85" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="B85" s="29"/>
-      <c r="C85" s="29"/>
-      <c r="D85" s="29"/>
-      <c r="E85" s="29"/>
-      <c r="F85" s="29"/>
-      <c r="G85" s="29"/>
-      <c r="H85" s="29"/>
-      <c r="I85" s="29"/>
-      <c r="J85" s="29"/>
-      <c r="K85" s="29"/>
-      <c r="L85" s="29"/>
-      <c r="M85" s="29"/>
+      <c r="B85" s="30"/>
+      <c r="C85" s="30"/>
+      <c r="D85" s="30"/>
+      <c r="E85" s="30"/>
+      <c r="F85" s="30"/>
+      <c r="G85" s="30"/>
+      <c r="H85" s="30"/>
+      <c r="I85" s="30"/>
+      <c r="J85" s="30"/>
+      <c r="K85" s="30"/>
+      <c r="L85" s="30"/>
+      <c r="M85" s="30"/>
     </row>
     <row r="86" spans="1:13" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="8" t="s">
@@ -4036,81 +4122,81 @@
       <c r="M86" s="8"/>
     </row>
     <row r="87" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="13" t="s">
+      <c r="A87" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B87" s="13" t="s">
+      <c r="B87" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C87" s="13" t="s">
+      <c r="C87" s="21" t="s">
         <v>198</v>
       </c>
-      <c r="D87" s="14" t="s">
+      <c r="D87" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="E87" s="13"/>
-      <c r="F87" s="13"/>
-      <c r="G87" s="14"/>
-      <c r="H87" s="14"/>
-      <c r="I87" s="13"/>
-      <c r="J87" s="13"/>
-      <c r="K87" s="13"/>
-      <c r="L87" s="13"/>
-      <c r="M87" s="13"/>
+      <c r="E87" s="22"/>
+      <c r="F87" s="22"/>
+      <c r="G87" s="22"/>
+      <c r="H87" s="22"/>
+      <c r="I87" s="22"/>
+      <c r="J87" s="22"/>
+      <c r="K87" s="22"/>
+      <c r="L87" s="22"/>
+      <c r="M87" s="22"/>
     </row>
     <row r="88" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="11" t="s">
+      <c r="A88" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="B88" s="11" t="s">
+      <c r="B88" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C88" s="11" t="s">
+      <c r="C88" s="25" t="s">
         <v>199</v>
       </c>
-      <c r="D88" s="12" t="s">
+      <c r="D88" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="E88" s="11"/>
-      <c r="F88" s="11"/>
-      <c r="G88" s="12"/>
-      <c r="H88" s="12"/>
-      <c r="I88" s="11"/>
-      <c r="J88" s="11"/>
-      <c r="K88" s="11"/>
-      <c r="L88" s="11"/>
-      <c r="M88" s="11"/>
+      <c r="E88" s="26"/>
+      <c r="F88" s="26"/>
+      <c r="G88" s="26"/>
+      <c r="H88" s="26"/>
+      <c r="I88" s="26"/>
+      <c r="J88" s="26"/>
+      <c r="K88" s="27"/>
+      <c r="L88" s="26"/>
+      <c r="M88" s="26"/>
     </row>
     <row r="90" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="29" t="s">
+      <c r="A90" s="30" t="s">
         <v>147</v>
       </c>
-      <c r="B90" s="29"/>
-      <c r="C90" s="29"/>
-      <c r="D90" s="29"/>
-      <c r="E90" s="29"/>
-      <c r="F90" s="29"/>
-      <c r="G90" s="29"/>
-      <c r="H90" s="29"/>
-      <c r="I90" s="29"/>
-      <c r="J90" s="29"/>
-      <c r="K90" s="29"/>
-      <c r="L90" s="29"/>
-      <c r="M90" s="29"/>
+      <c r="B90" s="30"/>
+      <c r="C90" s="30"/>
+      <c r="D90" s="30"/>
+      <c r="E90" s="30"/>
+      <c r="F90" s="30"/>
+      <c r="G90" s="30"/>
+      <c r="H90" s="30"/>
+      <c r="I90" s="30"/>
+      <c r="J90" s="30"/>
+      <c r="K90" s="30"/>
+      <c r="L90" s="30"/>
+      <c r="M90" s="30"/>
     </row>
     <row r="91" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B91" s="44" t="s">
+      <c r="B91" s="41" t="s">
         <v>145</v>
       </c>
-      <c r="C91" s="44"/>
-      <c r="D91" s="43" t="s">
+      <c r="C91" s="41"/>
+      <c r="D91" s="40" t="s">
         <v>146</v>
       </c>
-      <c r="E91" s="44"/>
-      <c r="F91" s="45"/>
+      <c r="E91" s="41"/>
+      <c r="F91" s="42"/>
       <c r="G91" s="8"/>
       <c r="H91" s="8"/>
       <c r="I91" s="8"/>
@@ -4120,62 +4206,62 @@
       <c r="M91" s="8"/>
     </row>
     <row r="92" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="13" t="s">
+      <c r="A92" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="B92" s="47" t="s">
+      <c r="B92" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="C92" s="49"/>
-      <c r="D92" s="36" t="s">
+      <c r="C92" s="36"/>
+      <c r="D92" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="E92" s="46"/>
-      <c r="F92" s="37"/>
-      <c r="G92" s="14"/>
-      <c r="H92" s="14"/>
-      <c r="I92" s="13"/>
-      <c r="J92" s="13"/>
-      <c r="K92" s="13"/>
-      <c r="L92" s="13"/>
-      <c r="M92" s="13"/>
+      <c r="E92" s="22"/>
+      <c r="F92" s="22"/>
+      <c r="G92" s="22"/>
+      <c r="H92" s="22"/>
+      <c r="I92" s="22"/>
+      <c r="J92" s="22"/>
+      <c r="K92" s="22"/>
+      <c r="L92" s="22"/>
+      <c r="M92" s="22"/>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B93" s="7"/>
     </row>
     <row r="94" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="29" t="s">
+      <c r="A94" s="30" t="s">
         <v>140</v>
       </c>
-      <c r="B94" s="29"/>
-      <c r="C94" s="29"/>
-      <c r="D94" s="29"/>
-      <c r="E94" s="29"/>
-      <c r="F94" s="29"/>
-      <c r="G94" s="29"/>
-      <c r="H94" s="29"/>
-      <c r="I94" s="29"/>
-      <c r="J94" s="29"/>
-      <c r="K94" s="29"/>
-      <c r="L94" s="29"/>
-      <c r="M94" s="29"/>
+      <c r="B94" s="30"/>
+      <c r="C94" s="30"/>
+      <c r="D94" s="30"/>
+      <c r="E94" s="30"/>
+      <c r="F94" s="30"/>
+      <c r="G94" s="30"/>
+      <c r="H94" s="30"/>
+      <c r="I94" s="30"/>
+      <c r="J94" s="30"/>
+      <c r="K94" s="30"/>
+      <c r="L94" s="30"/>
+      <c r="M94" s="30"/>
     </row>
     <row r="95" spans="1:13" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="23"/>
-      <c r="B95" s="51" t="s">
+      <c r="A95" s="15"/>
+      <c r="B95" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="C95" s="51"/>
-      <c r="D95" s="51"/>
-      <c r="E95" s="51"/>
-      <c r="F95" s="51"/>
-      <c r="G95" s="51"/>
-      <c r="H95" s="51"/>
-      <c r="I95" s="51"/>
-      <c r="J95" s="51"/>
-      <c r="K95" s="51"/>
-      <c r="L95" s="51"/>
-      <c r="M95" s="51"/>
+      <c r="C95" s="45"/>
+      <c r="D95" s="45"/>
+      <c r="E95" s="45"/>
+      <c r="F95" s="45"/>
+      <c r="G95" s="45"/>
+      <c r="H95" s="45"/>
+      <c r="I95" s="45"/>
+      <c r="J95" s="45"/>
+      <c r="K95" s="45"/>
+      <c r="L95" s="45"/>
+      <c r="M95" s="45"/>
     </row>
     <row r="96" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="8" t="s">
@@ -4184,11 +4270,11 @@
       <c r="B96" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="C96" s="43" t="s">
+      <c r="C96" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="D96" s="44"/>
-      <c r="E96" s="45"/>
+      <c r="D96" s="41"/>
+      <c r="E96" s="42"/>
       <c r="F96" s="8"/>
       <c r="G96" s="8"/>
       <c r="H96" s="8"/>
@@ -4199,81 +4285,81 @@
       <c r="M96" s="8"/>
     </row>
     <row r="97" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="13" t="s">
+      <c r="A97" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B97" s="27" t="s">
+      <c r="B97" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="C97" s="47" t="s">
+      <c r="C97" s="37" t="s">
         <v>223</v>
       </c>
-      <c r="D97" s="48"/>
-      <c r="E97" s="49"/>
-      <c r="F97" s="13"/>
-      <c r="G97" s="14"/>
-      <c r="H97" s="14"/>
-      <c r="I97" s="13"/>
-      <c r="J97" s="13"/>
-      <c r="K97" s="13"/>
-      <c r="L97" s="13"/>
-      <c r="M97" s="13"/>
+      <c r="D97" s="43"/>
+      <c r="E97" s="38"/>
+      <c r="F97" s="22"/>
+      <c r="G97" s="22"/>
+      <c r="H97" s="22"/>
+      <c r="I97" s="22"/>
+      <c r="J97" s="22"/>
+      <c r="K97" s="22"/>
+      <c r="L97" s="22"/>
+      <c r="M97" s="22"/>
     </row>
     <row r="98" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="11" t="s">
+      <c r="A98" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="B98" s="28" t="s">
+      <c r="B98" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="C98" s="30" t="s">
+      <c r="C98" s="31" t="s">
         <v>224</v>
       </c>
-      <c r="D98" s="50"/>
-      <c r="E98" s="31"/>
-      <c r="F98" s="11"/>
-      <c r="G98" s="12"/>
-      <c r="H98" s="12"/>
-      <c r="I98" s="11"/>
-      <c r="J98" s="11"/>
-      <c r="K98" s="11"/>
-      <c r="L98" s="11"/>
-      <c r="M98" s="11"/>
+      <c r="D98" s="44"/>
+      <c r="E98" s="32"/>
+      <c r="F98" s="26"/>
+      <c r="G98" s="26"/>
+      <c r="H98" s="26"/>
+      <c r="I98" s="26"/>
+      <c r="J98" s="26"/>
+      <c r="K98" s="27"/>
+      <c r="L98" s="26"/>
+      <c r="M98" s="26"/>
     </row>
     <row r="99" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="100" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="42" t="s">
+      <c r="A100" s="39" t="s">
         <v>148</v>
       </c>
-      <c r="B100" s="42"/>
-      <c r="C100" s="42"/>
-      <c r="D100" s="42"/>
-      <c r="E100" s="42"/>
-      <c r="F100" s="42"/>
-      <c r="G100" s="42"/>
-      <c r="H100" s="42"/>
-      <c r="I100" s="42"/>
-      <c r="J100" s="42"/>
-      <c r="K100" s="42"/>
-      <c r="L100" s="42"/>
-      <c r="M100" s="42"/>
+      <c r="B100" s="39"/>
+      <c r="C100" s="39"/>
+      <c r="D100" s="39"/>
+      <c r="E100" s="39"/>
+      <c r="F100" s="39"/>
+      <c r="G100" s="39"/>
+      <c r="H100" s="39"/>
+      <c r="I100" s="39"/>
+      <c r="J100" s="39"/>
+      <c r="K100" s="39"/>
+      <c r="L100" s="39"/>
+      <c r="M100" s="39"/>
     </row>
     <row r="101" spans="1:13" ht="35.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="23"/>
-      <c r="B101" s="51" t="s">
+      <c r="A101" s="15"/>
+      <c r="B101" s="45" t="s">
         <v>236</v>
       </c>
-      <c r="C101" s="51"/>
-      <c r="D101" s="51"/>
-      <c r="E101" s="51"/>
-      <c r="F101" s="51"/>
-      <c r="G101" s="51"/>
-      <c r="H101" s="51"/>
-      <c r="I101" s="51"/>
-      <c r="J101" s="51"/>
-      <c r="K101" s="51"/>
-      <c r="L101" s="51"/>
-      <c r="M101" s="51"/>
+      <c r="C101" s="45"/>
+      <c r="D101" s="45"/>
+      <c r="E101" s="45"/>
+      <c r="F101" s="45"/>
+      <c r="G101" s="45"/>
+      <c r="H101" s="45"/>
+      <c r="I101" s="45"/>
+      <c r="J101" s="45"/>
+      <c r="K101" s="45"/>
+      <c r="L101" s="45"/>
+      <c r="M101" s="45"/>
     </row>
     <row r="102" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="8" t="s">
@@ -4305,97 +4391,97 @@
       <c r="M102" s="8"/>
     </row>
     <row r="103" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="13" t="s">
+      <c r="A103" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="B103" s="13" t="s">
+      <c r="B103" s="20" t="s">
         <v>198</v>
       </c>
-      <c r="C103" s="14">
+      <c r="C103" s="62">
         <v>162</v>
       </c>
-      <c r="D103" s="14" t="s">
+      <c r="D103" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="E103" s="27" t="s">
+      <c r="E103" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="F103" s="13" t="s">
+      <c r="F103" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="G103" s="14" t="s">
+      <c r="G103" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="H103" s="14"/>
-      <c r="I103" s="13"/>
-      <c r="J103" s="13"/>
-      <c r="K103" s="13"/>
-      <c r="L103" s="13"/>
-      <c r="M103" s="13"/>
+      <c r="H103" s="22"/>
+      <c r="I103" s="22"/>
+      <c r="J103" s="22"/>
+      <c r="K103" s="22"/>
+      <c r="L103" s="22"/>
+      <c r="M103" s="22"/>
     </row>
     <row r="104" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="11" t="s">
+      <c r="A104" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="B104" s="11" t="s">
+      <c r="B104" s="24" t="s">
         <v>199</v>
       </c>
-      <c r="C104" s="12">
+      <c r="C104" s="63">
         <v>162</v>
       </c>
-      <c r="D104" s="12" t="s">
+      <c r="D104" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="E104" s="28" t="s">
+      <c r="E104" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="F104" s="11" t="s">
+      <c r="F104" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="G104" s="12" t="s">
+      <c r="G104" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="H104" s="12"/>
-      <c r="I104" s="11"/>
-      <c r="J104" s="11"/>
-      <c r="K104" s="11"/>
-      <c r="L104" s="11"/>
-      <c r="M104" s="11"/>
+      <c r="H104" s="26"/>
+      <c r="I104" s="26"/>
+      <c r="J104" s="26"/>
+      <c r="K104" s="27"/>
+      <c r="L104" s="26"/>
+      <c r="M104" s="26"/>
     </row>
     <row r="105" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="106" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="29" t="s">
+      <c r="A106" s="30" t="s">
         <v>149</v>
       </c>
-      <c r="B106" s="29"/>
-      <c r="C106" s="29"/>
-      <c r="D106" s="29"/>
-      <c r="E106" s="29"/>
-      <c r="F106" s="29"/>
-      <c r="G106" s="29"/>
-      <c r="H106" s="29"/>
-      <c r="I106" s="29"/>
-      <c r="J106" s="29"/>
-      <c r="K106" s="29"/>
-      <c r="L106" s="29"/>
-      <c r="M106" s="29"/>
+      <c r="B106" s="30"/>
+      <c r="C106" s="30"/>
+      <c r="D106" s="30"/>
+      <c r="E106" s="30"/>
+      <c r="F106" s="30"/>
+      <c r="G106" s="30"/>
+      <c r="H106" s="30"/>
+      <c r="I106" s="30"/>
+      <c r="J106" s="30"/>
+      <c r="K106" s="30"/>
+      <c r="L106" s="30"/>
+      <c r="M106" s="30"/>
     </row>
     <row r="107" spans="1:13" s="3" customFormat="1" ht="36.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="23"/>
-      <c r="B107" s="51" t="s">
+      <c r="A107" s="15"/>
+      <c r="B107" s="45" t="s">
         <v>237</v>
       </c>
-      <c r="C107" s="51"/>
-      <c r="D107" s="51"/>
-      <c r="E107" s="51"/>
-      <c r="F107" s="51"/>
-      <c r="G107" s="51"/>
-      <c r="H107" s="51"/>
-      <c r="I107" s="51"/>
-      <c r="J107" s="51"/>
-      <c r="K107" s="51"/>
-      <c r="L107" s="51"/>
-      <c r="M107" s="51"/>
+      <c r="C107" s="45"/>
+      <c r="D107" s="45"/>
+      <c r="E107" s="45"/>
+      <c r="F107" s="45"/>
+      <c r="G107" s="45"/>
+      <c r="H107" s="45"/>
+      <c r="I107" s="45"/>
+      <c r="J107" s="45"/>
+      <c r="K107" s="45"/>
+      <c r="L107" s="45"/>
+      <c r="M107" s="45"/>
     </row>
     <row r="108" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="8" t="s">
@@ -4425,101 +4511,101 @@
       <c r="M108" s="8"/>
     </row>
     <row r="109" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="13" t="s">
+      <c r="A109" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="B109" s="13" t="s">
+      <c r="B109" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="C109" s="13" t="s">
+      <c r="C109" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="D109" s="27" t="s">
+      <c r="D109" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="E109" s="13" t="s">
+      <c r="E109" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="F109" s="27" t="s">
+      <c r="F109" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="G109" s="14"/>
-      <c r="H109" s="14"/>
-      <c r="I109" s="13"/>
-      <c r="J109" s="13"/>
-      <c r="K109" s="13"/>
-      <c r="L109" s="13"/>
-      <c r="M109" s="13"/>
+      <c r="G109" s="22"/>
+      <c r="H109" s="22"/>
+      <c r="I109" s="22"/>
+      <c r="J109" s="22"/>
+      <c r="K109" s="22"/>
+      <c r="L109" s="22"/>
+      <c r="M109" s="22"/>
     </row>
     <row r="110" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="11" t="s">
+      <c r="A110" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="B110" s="11" t="s">
+      <c r="B110" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="C110" s="11" t="s">
+      <c r="C110" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="D110" s="28" t="s">
+      <c r="D110" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="E110" s="11" t="s">
+      <c r="E110" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="F110" s="28" t="s">
+      <c r="F110" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="G110" s="12"/>
-      <c r="H110" s="12"/>
-      <c r="I110" s="11"/>
-      <c r="J110" s="11"/>
-      <c r="K110" s="11"/>
-      <c r="L110" s="11"/>
-      <c r="M110" s="11"/>
+      <c r="G110" s="26"/>
+      <c r="H110" s="26"/>
+      <c r="I110" s="26"/>
+      <c r="J110" s="26"/>
+      <c r="K110" s="27"/>
+      <c r="L110" s="26"/>
+      <c r="M110" s="26"/>
     </row>
     <row r="111" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="13" t="s">
+      <c r="A111" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="B111" s="13" t="s">
+      <c r="B111" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="C111" s="13" t="s">
+      <c r="C111" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D111" s="27"/>
-      <c r="E111" s="13" t="s">
+      <c r="D111" s="28"/>
+      <c r="E111" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="F111" s="27" t="s">
+      <c r="F111" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="G111" s="14"/>
-      <c r="H111" s="14"/>
-      <c r="I111" s="13"/>
-      <c r="J111" s="13"/>
-      <c r="K111" s="13"/>
-      <c r="L111" s="13"/>
-      <c r="M111" s="13"/>
+      <c r="G111" s="22"/>
+      <c r="H111" s="22"/>
+      <c r="I111" s="22"/>
+      <c r="J111" s="22"/>
+      <c r="K111" s="22"/>
+      <c r="L111" s="22"/>
+      <c r="M111" s="22"/>
     </row>
     <row r="112" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="113" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="29" t="s">
+      <c r="A113" s="30" t="s">
         <v>151</v>
       </c>
-      <c r="B113" s="29"/>
-      <c r="C113" s="29"/>
-      <c r="D113" s="29"/>
-      <c r="E113" s="29"/>
-      <c r="F113" s="29"/>
-      <c r="G113" s="29"/>
-      <c r="H113" s="29"/>
-      <c r="I113" s="29"/>
-      <c r="J113" s="29"/>
-      <c r="K113" s="29"/>
-      <c r="L113" s="29"/>
-      <c r="M113" s="29"/>
+      <c r="B113" s="30"/>
+      <c r="C113" s="30"/>
+      <c r="D113" s="30"/>
+      <c r="E113" s="30"/>
+      <c r="F113" s="30"/>
+      <c r="G113" s="30"/>
+      <c r="H113" s="30"/>
+      <c r="I113" s="30"/>
+      <c r="J113" s="30"/>
+      <c r="K113" s="30"/>
+      <c r="L113" s="30"/>
+      <c r="M113" s="30"/>
     </row>
     <row r="114" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="8" t="s">
@@ -4557,74 +4643,74 @@
       <c r="M114" s="8"/>
     </row>
     <row r="115" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="13" t="s">
+      <c r="A115" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="B115" s="13" t="s">
+      <c r="B115" s="20" t="s">
         <v>198</v>
       </c>
-      <c r="C115" s="14">
+      <c r="C115" s="62">
         <v>514</v>
       </c>
-      <c r="D115" s="14" t="s">
+      <c r="D115" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="E115" s="13" t="s">
+      <c r="E115" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="F115" s="13" t="s">
+      <c r="F115" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="G115" s="14" t="s">
+      <c r="G115" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="H115" s="14" t="s">
+      <c r="H115" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="I115" s="13" t="s">
+      <c r="I115" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="J115" s="13" t="s">
+      <c r="J115" s="22" t="s">
         <v>152</v>
       </c>
-      <c r="K115" s="13"/>
-      <c r="L115" s="13"/>
-      <c r="M115" s="13"/>
+      <c r="K115" s="22"/>
+      <c r="L115" s="22"/>
+      <c r="M115" s="22"/>
     </row>
     <row r="116" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="117" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="29" t="s">
+      <c r="A117" s="30" t="s">
         <v>159</v>
       </c>
-      <c r="B117" s="29"/>
-      <c r="C117" s="29"/>
-      <c r="D117" s="29"/>
-      <c r="E117" s="29"/>
-      <c r="F117" s="29"/>
-      <c r="G117" s="29"/>
-      <c r="H117" s="29"/>
-      <c r="I117" s="29"/>
-      <c r="J117" s="29"/>
-      <c r="K117" s="29"/>
-      <c r="L117" s="29"/>
-      <c r="M117" s="29"/>
+      <c r="B117" s="30"/>
+      <c r="C117" s="30"/>
+      <c r="D117" s="30"/>
+      <c r="E117" s="30"/>
+      <c r="F117" s="30"/>
+      <c r="G117" s="30"/>
+      <c r="H117" s="30"/>
+      <c r="I117" s="30"/>
+      <c r="J117" s="30"/>
+      <c r="K117" s="30"/>
+      <c r="L117" s="30"/>
+      <c r="M117" s="30"/>
     </row>
     <row r="118" spans="1:13" ht="63.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="26"/>
-      <c r="B118" s="60" t="s">
+      <c r="A118" s="18"/>
+      <c r="B118" s="55" t="s">
         <v>241</v>
       </c>
-      <c r="C118" s="60"/>
-      <c r="D118" s="60"/>
-      <c r="E118" s="60"/>
-      <c r="F118" s="60"/>
-      <c r="G118" s="60"/>
-      <c r="H118" s="60"/>
-      <c r="I118" s="60"/>
-      <c r="J118" s="60"/>
-      <c r="K118" s="60"/>
-      <c r="L118" s="60"/>
-      <c r="M118" s="60"/>
+      <c r="C118" s="55"/>
+      <c r="D118" s="55"/>
+      <c r="E118" s="55"/>
+      <c r="F118" s="55"/>
+      <c r="G118" s="55"/>
+      <c r="H118" s="55"/>
+      <c r="I118" s="55"/>
+      <c r="J118" s="55"/>
+      <c r="K118" s="55"/>
+      <c r="L118" s="55"/>
+      <c r="M118" s="55"/>
     </row>
     <row r="119" spans="1:13" s="4" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="8" t="s">
@@ -4660,105 +4746,105 @@
       <c r="M119" s="8"/>
     </row>
     <row r="120" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="13" t="s">
+      <c r="A120" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="B120" s="13" t="s">
+      <c r="B120" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="C120" s="13" t="s">
+      <c r="C120" s="21" t="s">
         <v>200</v>
       </c>
-      <c r="D120" s="14">
+      <c r="D120" s="62">
         <v>1812</v>
       </c>
-      <c r="E120" s="27" t="s">
+      <c r="E120" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="F120" s="13" t="s">
+      <c r="F120" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="G120" s="14">
+      <c r="G120" s="62">
         <v>5</v>
       </c>
-      <c r="H120" s="14">
+      <c r="H120" s="62">
         <v>5</v>
       </c>
-      <c r="I120" s="13" t="s">
+      <c r="I120" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="J120" s="13"/>
-      <c r="K120" s="13"/>
-      <c r="L120" s="13"/>
-      <c r="M120" s="13"/>
+      <c r="J120" s="22"/>
+      <c r="K120" s="22"/>
+      <c r="L120" s="22"/>
+      <c r="M120" s="22"/>
     </row>
     <row r="121" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="11" t="s">
+      <c r="A121" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="B121" s="11" t="s">
+      <c r="B121" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="C121" s="11" t="s">
+      <c r="C121" s="25" t="s">
         <v>201</v>
       </c>
-      <c r="D121" s="12">
+      <c r="D121" s="63">
         <v>1812</v>
       </c>
-      <c r="E121" s="28" t="s">
+      <c r="E121" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="F121" s="11" t="s">
+      <c r="F121" s="26" t="s">
         <v>160</v>
       </c>
-      <c r="G121" s="12">
+      <c r="G121" s="63">
         <v>5</v>
       </c>
-      <c r="H121" s="12">
+      <c r="H121" s="63">
         <v>5</v>
       </c>
-      <c r="I121" s="11" t="s">
+      <c r="I121" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="J121" s="11"/>
-      <c r="K121" s="11"/>
-      <c r="L121" s="11"/>
-      <c r="M121" s="11"/>
+      <c r="J121" s="26"/>
+      <c r="K121" s="27"/>
+      <c r="L121" s="26"/>
+      <c r="M121" s="26"/>
     </row>
     <row r="122" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="123" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="29" t="s">
+      <c r="A123" s="30" t="s">
         <v>172</v>
       </c>
-      <c r="B123" s="29"/>
-      <c r="C123" s="29"/>
-      <c r="D123" s="29"/>
-      <c r="E123" s="29"/>
-      <c r="F123" s="29"/>
-      <c r="G123" s="29"/>
-      <c r="H123" s="29"/>
-      <c r="I123" s="29"/>
-      <c r="J123" s="29"/>
-      <c r="K123" s="29"/>
-      <c r="L123" s="29"/>
-      <c r="M123" s="29"/>
+      <c r="B123" s="30"/>
+      <c r="C123" s="30"/>
+      <c r="D123" s="30"/>
+      <c r="E123" s="30"/>
+      <c r="F123" s="30"/>
+      <c r="G123" s="30"/>
+      <c r="H123" s="30"/>
+      <c r="I123" s="30"/>
+      <c r="J123" s="30"/>
+      <c r="K123" s="30"/>
+      <c r="L123" s="30"/>
+      <c r="M123" s="30"/>
     </row>
     <row r="124" spans="1:13" ht="69.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="26"/>
-      <c r="B124" s="60" t="s">
+      <c r="A124" s="18"/>
+      <c r="B124" s="55" t="s">
         <v>242</v>
       </c>
-      <c r="C124" s="60"/>
-      <c r="D124" s="60"/>
-      <c r="E124" s="60"/>
-      <c r="F124" s="60"/>
-      <c r="G124" s="60"/>
-      <c r="H124" s="60"/>
-      <c r="I124" s="60"/>
-      <c r="J124" s="60"/>
-      <c r="K124" s="60"/>
-      <c r="L124" s="60"/>
-      <c r="M124" s="60"/>
+      <c r="C124" s="55"/>
+      <c r="D124" s="55"/>
+      <c r="E124" s="55"/>
+      <c r="F124" s="55"/>
+      <c r="G124" s="55"/>
+      <c r="H124" s="55"/>
+      <c r="I124" s="55"/>
+      <c r="J124" s="55"/>
+      <c r="K124" s="55"/>
+      <c r="L124" s="55"/>
+      <c r="M124" s="55"/>
     </row>
     <row r="125" spans="1:13" s="4" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="10" t="s">
@@ -4794,104 +4880,104 @@
       <c r="M125" s="10"/>
     </row>
     <row r="126" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="13" t="s">
+      <c r="A126" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="B126" s="13" t="s">
+      <c r="B126" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="C126" s="13" t="s">
+      <c r="C126" s="21" t="s">
         <v>200</v>
       </c>
-      <c r="D126" s="14">
+      <c r="D126" s="62">
         <v>49</v>
       </c>
-      <c r="E126" s="27" t="s">
+      <c r="E126" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="F126" s="13" t="s">
+      <c r="F126" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="G126" s="14">
+      <c r="G126" s="62">
         <v>5</v>
       </c>
-      <c r="H126" s="14">
+      <c r="H126" s="62">
         <v>5</v>
       </c>
-      <c r="I126" s="13" t="s">
+      <c r="I126" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="J126" s="13"/>
-      <c r="K126" s="13"/>
-      <c r="L126" s="13"/>
-      <c r="M126" s="13"/>
+      <c r="J126" s="22"/>
+      <c r="K126" s="22"/>
+      <c r="L126" s="22"/>
+      <c r="M126" s="22"/>
     </row>
     <row r="127" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="11" t="s">
+      <c r="A127" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="B127" s="11" t="s">
+      <c r="B127" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="C127" s="11" t="s">
+      <c r="C127" s="25" t="s">
         <v>201</v>
       </c>
-      <c r="D127" s="12">
+      <c r="D127" s="63">
         <v>49</v>
       </c>
-      <c r="E127" s="28" t="s">
+      <c r="E127" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="F127" s="11" t="s">
+      <c r="F127" s="26" t="s">
         <v>160</v>
       </c>
-      <c r="G127" s="12">
+      <c r="G127" s="63">
         <v>5</v>
       </c>
-      <c r="H127" s="12">
+      <c r="H127" s="63">
         <v>5</v>
       </c>
-      <c r="I127" s="11" t="s">
+      <c r="I127" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="J127" s="11"/>
-      <c r="K127" s="11"/>
-      <c r="L127" s="11"/>
-      <c r="M127" s="11"/>
+      <c r="J127" s="26"/>
+      <c r="K127" s="27"/>
+      <c r="L127" s="26"/>
+      <c r="M127" s="26"/>
     </row>
     <row r="129" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="61" t="s">
+      <c r="A129" s="56" t="s">
         <v>239</v>
       </c>
-      <c r="B129" s="61"/>
-      <c r="C129" s="61"/>
-      <c r="D129" s="61"/>
-      <c r="E129" s="61"/>
-      <c r="F129" s="61"/>
-      <c r="G129" s="61"/>
-      <c r="H129" s="61"/>
-      <c r="I129" s="61"/>
-      <c r="J129" s="61"/>
-      <c r="K129" s="61"/>
-      <c r="L129" s="61"/>
-      <c r="M129" s="61"/>
+      <c r="B129" s="56"/>
+      <c r="C129" s="56"/>
+      <c r="D129" s="56"/>
+      <c r="E129" s="56"/>
+      <c r="F129" s="56"/>
+      <c r="G129" s="56"/>
+      <c r="H129" s="56"/>
+      <c r="I129" s="56"/>
+      <c r="J129" s="56"/>
+      <c r="K129" s="56"/>
+      <c r="L129" s="56"/>
+      <c r="M129" s="56"/>
     </row>
     <row r="130" spans="1:13" s="3" customFormat="1" ht="51.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="26"/>
-      <c r="B130" s="60" t="s">
+      <c r="A130" s="18"/>
+      <c r="B130" s="55" t="s">
         <v>240</v>
       </c>
-      <c r="C130" s="60"/>
-      <c r="D130" s="60"/>
-      <c r="E130" s="60"/>
-      <c r="F130" s="60"/>
-      <c r="G130" s="60"/>
-      <c r="H130" s="60"/>
-      <c r="I130" s="60"/>
-      <c r="J130" s="60"/>
-      <c r="K130" s="60"/>
-      <c r="L130" s="60"/>
-      <c r="M130" s="60"/>
+      <c r="C130" s="55"/>
+      <c r="D130" s="55"/>
+      <c r="E130" s="55"/>
+      <c r="F130" s="55"/>
+      <c r="G130" s="55"/>
+      <c r="H130" s="55"/>
+      <c r="I130" s="55"/>
+      <c r="J130" s="55"/>
+      <c r="K130" s="55"/>
+      <c r="L130" s="55"/>
+      <c r="M130" s="55"/>
     </row>
     <row r="131" spans="1:13" s="4" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="8" t="s">
@@ -4917,51 +5003,51 @@
       <c r="M131" s="8"/>
     </row>
     <row r="132" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="16" t="s">
+      <c r="A132" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="B132" s="16" t="s">
+      <c r="B132" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="C132" s="16" t="s">
+      <c r="C132" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="D132" s="16" t="s">
+      <c r="D132" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="E132" s="16"/>
-      <c r="F132" s="16"/>
-      <c r="G132" s="16"/>
-      <c r="H132" s="16"/>
-      <c r="I132" s="16"/>
-      <c r="J132" s="16"/>
-      <c r="K132" s="16"/>
-      <c r="L132" s="16"/>
-      <c r="M132" s="16"/>
+      <c r="E132" s="22"/>
+      <c r="F132" s="22"/>
+      <c r="G132" s="22"/>
+      <c r="H132" s="22"/>
+      <c r="I132" s="22"/>
+      <c r="J132" s="22"/>
+      <c r="K132" s="22"/>
+      <c r="L132" s="22"/>
+      <c r="M132" s="22"/>
     </row>
     <row r="133" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="17" t="s">
+      <c r="A133" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="B133" s="17" t="s">
+      <c r="B133" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="C133" s="17"/>
-      <c r="D133" s="17" t="s">
+      <c r="C133" s="25"/>
+      <c r="D133" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="E133" s="17"/>
-      <c r="F133" s="17"/>
-      <c r="G133" s="17"/>
-      <c r="H133" s="17"/>
-      <c r="I133" s="17"/>
-      <c r="J133" s="17"/>
-      <c r="K133" s="17"/>
-      <c r="L133" s="17"/>
-      <c r="M133" s="17"/>
+      <c r="E133" s="26"/>
+      <c r="F133" s="26"/>
+      <c r="G133" s="26"/>
+      <c r="H133" s="26"/>
+      <c r="I133" s="26"/>
+      <c r="J133" s="26"/>
+      <c r="K133" s="27"/>
+      <c r="L133" s="26"/>
+      <c r="M133" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="55">
+  <mergeCells count="54">
     <mergeCell ref="B107:M107"/>
     <mergeCell ref="B118:M118"/>
     <mergeCell ref="B130:M130"/>
@@ -5002,7 +5088,6 @@
     <mergeCell ref="A100:M100"/>
     <mergeCell ref="A106:M106"/>
     <mergeCell ref="D91:F91"/>
-    <mergeCell ref="D92:F92"/>
     <mergeCell ref="C97:E97"/>
     <mergeCell ref="C96:E96"/>
     <mergeCell ref="C98:E98"/>

</xml_diff>

<commit_message>
Updated to Provider 0.5.2
</commit_message>
<xml_diff>
--- a/deploy-fabric-Input-Spreadsheet.xlsx
+++ b/deploy-fabric-Input-Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\tyscott\terraform-aci-fabric-deploy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F0FCB0F-3469-41F7-9ECD-7212F5B0A9CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED8EBAA-7BC3-4621-B18A-160170A68E84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,6 +19,8 @@
   <definedNames>
     <definedName name="leaf">formulas!$B$2:$B$18</definedName>
     <definedName name="spine">formulas!$C$2:$C$12</definedName>
+    <definedName name="spine_modules">formulas!$F$2:$F$5</definedName>
+    <definedName name="spine_type">formulas!$E$2:$E$4</definedName>
     <definedName name="switch_role">formulas!$A$2:$A$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="273">
   <si>
     <t>Type</t>
   </si>
@@ -1128,6 +1130,108 @@
   </si>
   <si>
     <t>9336PQ</t>
+  </si>
+  <si>
+    <t>Define Spine Modules</t>
+  </si>
+  <si>
+    <t>Module 1</t>
+  </si>
+  <si>
+    <t>Module 2</t>
+  </si>
+  <si>
+    <t>Module 3</t>
+  </si>
+  <si>
+    <t>Module 4</t>
+  </si>
+  <si>
+    <t>Module 5</t>
+  </si>
+  <si>
+    <t>Module 6</t>
+  </si>
+  <si>
+    <t>Module 7</t>
+  </si>
+  <si>
+    <t>Module 8</t>
+  </si>
+  <si>
+    <t>Module 9</t>
+  </si>
+  <si>
+    <t>Module 10</t>
+  </si>
+  <si>
+    <t>Module 12</t>
+  </si>
+  <si>
+    <t>Module 13</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Notes:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> This Section is only needed if you have a Modular Spine</t>
+    </r>
+  </si>
+  <si>
+    <t>Module 14</t>
+  </si>
+  <si>
+    <t>Module 15</t>
+  </si>
+  <si>
+    <t>Module 16</t>
+  </si>
+  <si>
+    <t>Spine Type</t>
+  </si>
+  <si>
+    <t>9504</t>
+  </si>
+  <si>
+    <t>9508</t>
+  </si>
+  <si>
+    <t>9516</t>
+  </si>
+  <si>
+    <t>Spine Modules</t>
+  </si>
+  <si>
+    <t>X9716D-GX</t>
+  </si>
+  <si>
+    <t>X9732C-EX</t>
+  </si>
+  <si>
+    <t>X9736C-FX</t>
+  </si>
+  <si>
+    <t>X9736PQ</t>
+  </si>
+  <si>
+    <t>Switch Interface Profile</t>
   </si>
 </sst>
 </file>
@@ -2009,7 +2113,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="17" fillId="33" borderId="8" xfId="2" applyNumberFormat="1"/>
@@ -2094,6 +2198,30 @@
     <xf numFmtId="164" fontId="24" fillId="0" borderId="25" xfId="45" applyNumberFormat="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="23" fillId="37" borderId="25" xfId="44" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="37" borderId="25" xfId="44" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="25" xfId="45" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="25" fillId="34" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="25" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="24" fillId="37" borderId="25" xfId="44" applyNumberFormat="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="24" fillId="0" borderId="25" xfId="45" applyNumberFormat="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="17" fillId="33" borderId="8" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2109,91 +2237,76 @@
     <xf numFmtId="49" fontId="18" fillId="0" borderId="21" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="20" fillId="37" borderId="26" xfId="43" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="37" borderId="27" xfId="44" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="37" borderId="28" xfId="44" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="37" borderId="29" xfId="44" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="33" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="13" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="14" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="37" borderId="32" xfId="44" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="33" xfId="45" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="34" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="23" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="17" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="18" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="19" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="34" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="34" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="34" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="37" borderId="26" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="37" borderId="27" xfId="44" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="37" borderId="28" xfId="44" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="37" borderId="29" xfId="44" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="33" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="13" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="14" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="37" borderId="32" xfId="44" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="33" xfId="45" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="34" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="17" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="18" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="19" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="23" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="34" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="18" fillId="34" borderId="24" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="17" fillId="36" borderId="8" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="23" fillId="37" borderId="25" xfId="44" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="23" fillId="37" borderId="25" xfId="44" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="23" fillId="0" borderId="25" xfId="45" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="37" borderId="26" xfId="43" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="23" fillId="37" borderId="27" xfId="44" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="25" fillId="34" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="25" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2245,7 +2358,92 @@
     <cellStyle name="ws_even" xfId="45" xr:uid="{91AD35C5-FC4E-4620-A7A5-CB67461C9E9F}"/>
     <cellStyle name="ws_odd" xfId="44" xr:uid="{0CA9025F-5804-4CA3-88B6-FF827C0201FD}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="12">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2555,10 +2753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P133"/>
+  <dimension ref="A1:Q143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C115" sqref="C115"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E113" sqref="E113:E114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2579,25 +2777,26 @@
     <col min="14" max="14" width="12.140625" style="5" customWidth="1"/>
     <col min="15" max="15" width="12.5703125" style="5" customWidth="1"/>
     <col min="16" max="16" width="12.42578125" style="5" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="5"/>
+    <col min="17" max="17" width="11.85546875" style="5" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
     </row>
     <row r="2" spans="1:16" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -2638,41 +2837,41 @@
       <c r="M3" s="22"/>
     </row>
     <row r="5" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="47" t="s">
         <v>202</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="39"/>
-      <c r="L5" s="39"/>
-      <c r="M5" s="39"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
       <c r="N5" s="14"/>
       <c r="O5" s="14"/>
       <c r="P5" s="14"/>
     </row>
     <row r="6" spans="1:16" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="12"/>
-      <c r="B6" s="53" t="s">
+      <c r="B6" s="55" t="s">
         <v>238</v>
       </c>
-      <c r="C6" s="53"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="53"/>
-      <c r="H6" s="53"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="53"/>
-      <c r="K6" s="53"/>
-      <c r="L6" s="53"/>
-      <c r="M6" s="53"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="55"/>
+      <c r="I6" s="55"/>
+      <c r="J6" s="55"/>
+      <c r="K6" s="55"/>
+      <c r="L6" s="55"/>
+      <c r="M6" s="55"/>
       <c r="N6" s="12"/>
       <c r="O6" s="12"/>
       <c r="P6" s="12"/>
@@ -2717,11 +2916,11 @@
       <c r="M7" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="N7" s="47" t="s">
+      <c r="N7" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="O7" s="48"/>
-      <c r="P7" s="49"/>
+      <c r="O7" s="57"/>
+      <c r="P7" s="58"/>
     </row>
     <row r="8" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
@@ -2730,10 +2929,10 @@
       <c r="B8" s="28" t="s">
         <v>208</v>
       </c>
-      <c r="C8" s="57">
+      <c r="C8" s="30">
         <v>0</v>
       </c>
-      <c r="D8" s="57">
+      <c r="D8" s="30">
         <v>15</v>
       </c>
       <c r="E8" s="22" t="s">
@@ -2745,10 +2944,10 @@
       <c r="G8" s="22" t="s">
         <v>211</v>
       </c>
-      <c r="H8" s="58" t="s">
+      <c r="H8" s="31" t="s">
         <v>220</v>
       </c>
-      <c r="I8" s="57">
+      <c r="I8" s="30">
         <v>22</v>
       </c>
       <c r="J8" s="22" t="s">
@@ -2761,43 +2960,43 @@
         <v>48</v>
       </c>
       <c r="M8" s="28"/>
-      <c r="N8" s="50"/>
-      <c r="O8" s="51"/>
-      <c r="P8" s="52"/>
+      <c r="N8" s="59"/>
+      <c r="O8" s="60"/>
+      <c r="P8" s="61"/>
     </row>
     <row r="10" spans="1:16" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="30"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="30"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="38"/>
+      <c r="M10" s="38"/>
     </row>
     <row r="11" spans="1:16" s="6" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="13"/>
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="54" t="s">
         <v>225</v>
       </c>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="46"/>
-      <c r="J11" s="46"/>
-      <c r="K11" s="46"/>
-      <c r="L11" s="46"/>
-      <c r="M11" s="46"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="54"/>
+      <c r="I11" s="54"/>
+      <c r="J11" s="54"/>
+      <c r="K11" s="54"/>
+      <c r="L11" s="54"/>
+      <c r="M11" s="54"/>
     </row>
     <row r="12" spans="1:16" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
@@ -2848,13 +3047,13 @@
       <c r="C13" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="57">
+      <c r="D13" s="30">
         <v>101</v>
       </c>
       <c r="E13" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="F13" s="57">
+      <c r="F13" s="30">
         <v>1</v>
       </c>
       <c r="G13" s="22" t="s">
@@ -2926,13 +3125,13 @@
       <c r="C15" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="57">
+      <c r="D15" s="30">
         <v>202</v>
       </c>
       <c r="E15" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="F15" s="57">
+      <c r="F15" s="30">
         <v>1</v>
       </c>
       <c r="G15" s="22" t="s">
@@ -2970,13 +3169,13 @@
       <c r="L16" s="26"/>
       <c r="M16" s="26"/>
     </row>
-    <row r="17" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="19"/>
       <c r="B17" s="20"/>
       <c r="C17" s="21"/>
-      <c r="D17" s="57"/>
+      <c r="D17" s="30"/>
       <c r="E17" s="22"/>
-      <c r="F17" s="57"/>
+      <c r="F17" s="30"/>
       <c r="G17" s="22"/>
       <c r="H17" s="22"/>
       <c r="I17" s="22"/>
@@ -2985,7 +3184,7 @@
       <c r="L17" s="22"/>
       <c r="M17" s="22"/>
     </row>
-    <row r="18" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="23"/>
       <c r="B18" s="24"/>
       <c r="C18" s="25"/>
@@ -3000,13 +3199,13 @@
       <c r="L18" s="26"/>
       <c r="M18" s="26"/>
     </row>
-    <row r="19" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="19"/>
       <c r="B19" s="20"/>
       <c r="C19" s="21"/>
-      <c r="D19" s="57"/>
+      <c r="D19" s="30"/>
       <c r="E19" s="22"/>
-      <c r="F19" s="57"/>
+      <c r="F19" s="30"/>
       <c r="G19" s="22"/>
       <c r="H19" s="22"/>
       <c r="I19" s="22"/>
@@ -3015,7 +3214,7 @@
       <c r="L19" s="22"/>
       <c r="M19" s="22"/>
     </row>
-    <row r="20" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="23"/>
       <c r="B20" s="24"/>
       <c r="C20" s="25"/>
@@ -3030,13 +3229,13 @@
       <c r="L20" s="26"/>
       <c r="M20" s="26"/>
     </row>
-    <row r="21" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="19"/>
       <c r="B21" s="20"/>
       <c r="C21" s="21"/>
-      <c r="D21" s="57"/>
+      <c r="D21" s="30"/>
       <c r="E21" s="22"/>
-      <c r="F21" s="57"/>
+      <c r="F21" s="30"/>
       <c r="G21" s="22"/>
       <c r="H21" s="22"/>
       <c r="I21" s="22"/>
@@ -3045,7 +3244,7 @@
       <c r="L21" s="22"/>
       <c r="M21" s="22"/>
     </row>
-    <row r="22" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="23"/>
       <c r="B22" s="24"/>
       <c r="C22" s="25"/>
@@ -3060,13 +3259,13 @@
       <c r="L22" s="26"/>
       <c r="M22" s="26"/>
     </row>
-    <row r="23" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="19"/>
       <c r="B23" s="20"/>
       <c r="C23" s="21"/>
-      <c r="D23" s="57"/>
+      <c r="D23" s="30"/>
       <c r="E23" s="22"/>
-      <c r="F23" s="57"/>
+      <c r="F23" s="30"/>
       <c r="G23" s="22"/>
       <c r="H23" s="22"/>
       <c r="I23" s="22"/>
@@ -3075,7 +3274,7 @@
       <c r="L23" s="22"/>
       <c r="M23" s="22"/>
     </row>
-    <row r="24" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="23"/>
       <c r="B24" s="24"/>
       <c r="C24" s="25"/>
@@ -3090,13 +3289,13 @@
       <c r="L24" s="26"/>
       <c r="M24" s="26"/>
     </row>
-    <row r="25" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="19"/>
       <c r="B25" s="20"/>
       <c r="C25" s="21"/>
-      <c r="D25" s="57"/>
+      <c r="D25" s="30"/>
       <c r="E25" s="22"/>
-      <c r="F25" s="57"/>
+      <c r="F25" s="30"/>
       <c r="G25" s="22"/>
       <c r="H25" s="22"/>
       <c r="I25" s="22"/>
@@ -3105,7 +3304,7 @@
       <c r="L25" s="22"/>
       <c r="M25" s="22"/>
     </row>
-    <row r="26" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="23"/>
       <c r="B26" s="24"/>
       <c r="C26" s="25"/>
@@ -3120,111 +3319,155 @@
       <c r="L26" s="26"/>
       <c r="M26" s="26"/>
     </row>
-    <row r="28" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="30" t="s">
-        <v>243</v>
-      </c>
-      <c r="B28" s="30"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="30"/>
-      <c r="G28" s="30"/>
-      <c r="H28" s="30"/>
-      <c r="I28" s="30"/>
-      <c r="J28" s="30"/>
-      <c r="K28" s="30"/>
-      <c r="L28" s="30"/>
-      <c r="M28" s="30"/>
-    </row>
-    <row r="29" spans="1:13" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" s="6" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="47" t="s">
+        <v>246</v>
+      </c>
+      <c r="B28" s="47"/>
+      <c r="C28" s="47"/>
+      <c r="D28" s="47"/>
+      <c r="E28" s="47"/>
+      <c r="F28" s="47"/>
+      <c r="G28" s="47"/>
+      <c r="H28" s="47"/>
+      <c r="I28" s="47"/>
+      <c r="J28" s="47"/>
+      <c r="K28" s="47"/>
+      <c r="L28" s="47"/>
+      <c r="M28" s="47"/>
+      <c r="N28" s="16"/>
+      <c r="O28" s="16"/>
+      <c r="P28" s="16"/>
+      <c r="Q28" s="16"/>
+    </row>
+    <row r="29" spans="1:17" s="6" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="13"/>
-      <c r="B29" s="46" t="s">
-        <v>244</v>
-      </c>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="46"/>
-      <c r="H29" s="46"/>
-      <c r="I29" s="46"/>
-      <c r="J29" s="46"/>
-      <c r="K29" s="46"/>
-      <c r="L29" s="46"/>
-      <c r="M29" s="46"/>
-    </row>
-    <row r="30" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="55" t="s">
+        <v>259</v>
+      </c>
+      <c r="C29" s="55"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="55"/>
+      <c r="H29" s="55"/>
+      <c r="I29" s="55"/>
+      <c r="J29" s="55"/>
+      <c r="K29" s="55"/>
+      <c r="L29" s="55"/>
+      <c r="M29" s="55"/>
+      <c r="N29" s="35"/>
+      <c r="O29" s="35"/>
+      <c r="P29" s="35"/>
+      <c r="Q29" s="35"/>
+    </row>
+    <row r="30" spans="1:17" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>178</v>
+        <v>272</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>3</v>
+        <v>247</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>179</v>
+        <v>248</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="8"/>
-    </row>
-    <row r="31" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="19" t="s">
-        <v>177</v>
-      </c>
-      <c r="B31" s="20">
-        <v>201</v>
-      </c>
-      <c r="C31" s="21" t="s">
-        <v>181</v>
-      </c>
-      <c r="D31" s="57">
-        <v>201</v>
-      </c>
-      <c r="E31" s="57">
-        <v>202</v>
-      </c>
+        <v>249</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="I30" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="J30" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="K30" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="L30" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="M30" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="N30" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="O30" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="P30" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q30" s="8" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="36" t="s">
+        <v>265</v>
+      </c>
+      <c r="B31" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="22" t="s">
+        <v>269</v>
+      </c>
+      <c r="D31" s="22" t="s">
+        <v>270</v>
+      </c>
+      <c r="E31" s="22"/>
       <c r="F31" s="22"/>
       <c r="G31" s="22"/>
       <c r="H31" s="22"/>
-      <c r="I31" s="22"/>
+      <c r="I31" s="22" t="s">
+        <v>269</v>
+      </c>
       <c r="J31" s="22"/>
       <c r="K31" s="22"/>
       <c r="L31" s="22"/>
       <c r="M31" s="22"/>
-    </row>
-    <row r="32" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="23"/>
-      <c r="B32" s="24"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="27"/>
+      <c r="N31" s="22"/>
+      <c r="O31" s="22"/>
+      <c r="P31" s="22"/>
+      <c r="Q31" s="22"/>
+    </row>
+    <row r="32" spans="1:17" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="37"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
       <c r="F32" s="26"/>
       <c r="G32" s="26"/>
       <c r="H32" s="26"/>
       <c r="I32" s="26"/>
       <c r="J32" s="26"/>
-      <c r="K32" s="27"/>
+      <c r="K32" s="26"/>
       <c r="L32" s="26"/>
       <c r="M32" s="26"/>
-    </row>
-    <row r="33" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="19"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="57"/>
-      <c r="E33" s="57"/>
+      <c r="N32" s="26"/>
+      <c r="O32" s="27"/>
+      <c r="P32" s="26"/>
+      <c r="Q32" s="26"/>
+    </row>
+    <row r="33" spans="1:17" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="36"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
       <c r="F33" s="22"/>
       <c r="G33" s="22"/>
       <c r="H33" s="22"/>
@@ -3233,28 +3476,36 @@
       <c r="K33" s="22"/>
       <c r="L33" s="22"/>
       <c r="M33" s="22"/>
-    </row>
-    <row r="34" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="23"/>
-      <c r="B34" s="24"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27"/>
+      <c r="N33" s="22"/>
+      <c r="O33" s="22"/>
+      <c r="P33" s="22"/>
+      <c r="Q33" s="22"/>
+    </row>
+    <row r="34" spans="1:17" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="37"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
       <c r="F34" s="26"/>
       <c r="G34" s="26"/>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
       <c r="J34" s="26"/>
-      <c r="K34" s="27"/>
+      <c r="K34" s="26"/>
       <c r="L34" s="26"/>
       <c r="M34" s="26"/>
-    </row>
-    <row r="35" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="19"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="57"/>
-      <c r="E35" s="57"/>
+      <c r="N34" s="26"/>
+      <c r="O34" s="27"/>
+      <c r="P34" s="26"/>
+      <c r="Q34" s="26"/>
+    </row>
+    <row r="35" spans="1:17" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="36"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
       <c r="F35" s="22"/>
       <c r="G35" s="22"/>
       <c r="H35" s="22"/>
@@ -3263,400 +3514,421 @@
       <c r="K35" s="22"/>
       <c r="L35" s="22"/>
       <c r="M35" s="22"/>
-    </row>
-    <row r="36" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="23"/>
-      <c r="B36" s="24"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="27"/>
-      <c r="E36" s="27"/>
+      <c r="N35" s="22"/>
+      <c r="O35" s="22"/>
+      <c r="P35" s="22"/>
+      <c r="Q35" s="22"/>
+    </row>
+    <row r="36" spans="1:17" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="37"/>
+      <c r="B36" s="25"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="26"/>
       <c r="F36" s="26"/>
       <c r="G36" s="26"/>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
       <c r="J36" s="26"/>
-      <c r="K36" s="27"/>
+      <c r="K36" s="26"/>
       <c r="L36" s="26"/>
       <c r="M36" s="26"/>
-    </row>
-    <row r="37" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="19"/>
-      <c r="B37" s="20"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="57"/>
-      <c r="E37" s="57"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="22"/>
-      <c r="I37" s="22"/>
-      <c r="J37" s="22"/>
-      <c r="K37" s="22"/>
-      <c r="L37" s="22"/>
-      <c r="M37" s="22"/>
-    </row>
-    <row r="39" spans="1:13" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="30" t="s">
+      <c r="N36" s="26"/>
+      <c r="O36" s="27"/>
+      <c r="P36" s="26"/>
+      <c r="Q36" s="26"/>
+    </row>
+    <row r="38" spans="1:17" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="38" t="s">
+        <v>243</v>
+      </c>
+      <c r="B38" s="38"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="38"/>
+      <c r="G38" s="38"/>
+      <c r="H38" s="38"/>
+      <c r="I38" s="38"/>
+      <c r="J38" s="38"/>
+      <c r="K38" s="38"/>
+      <c r="L38" s="38"/>
+      <c r="M38" s="38"/>
+    </row>
+    <row r="39" spans="1:17" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="13"/>
+      <c r="B39" s="54" t="s">
+        <v>244</v>
+      </c>
+      <c r="C39" s="54"/>
+      <c r="D39" s="54"/>
+      <c r="E39" s="54"/>
+      <c r="F39" s="54"/>
+      <c r="G39" s="54"/>
+      <c r="H39" s="54"/>
+      <c r="I39" s="54"/>
+      <c r="J39" s="54"/>
+      <c r="K39" s="54"/>
+      <c r="L39" s="54"/>
+      <c r="M39" s="54"/>
+    </row>
+    <row r="40" spans="1:17" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="8"/>
+      <c r="K40" s="8"/>
+      <c r="L40" s="8"/>
+      <c r="M40" s="8"/>
+    </row>
+    <row r="41" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="B41" s="36">
+        <v>201</v>
+      </c>
+      <c r="C41" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="D41" s="30">
+        <v>201</v>
+      </c>
+      <c r="E41" s="30">
+        <v>202</v>
+      </c>
+      <c r="F41" s="22"/>
+      <c r="G41" s="22"/>
+      <c r="H41" s="22"/>
+      <c r="I41" s="22"/>
+      <c r="J41" s="22"/>
+      <c r="K41" s="22"/>
+      <c r="L41" s="22"/>
+      <c r="M41" s="22"/>
+    </row>
+    <row r="42" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="23"/>
+      <c r="B42" s="37"/>
+      <c r="C42" s="25"/>
+      <c r="D42" s="27"/>
+      <c r="E42" s="27"/>
+      <c r="F42" s="26"/>
+      <c r="G42" s="26"/>
+      <c r="H42" s="26"/>
+      <c r="I42" s="26"/>
+      <c r="J42" s="26"/>
+      <c r="K42" s="27"/>
+      <c r="L42" s="26"/>
+      <c r="M42" s="26"/>
+    </row>
+    <row r="43" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="19"/>
+      <c r="B43" s="36"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="30"/>
+      <c r="F43" s="22"/>
+      <c r="G43" s="22"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
+      <c r="K43" s="22"/>
+      <c r="L43" s="22"/>
+      <c r="M43" s="22"/>
+    </row>
+    <row r="44" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="23"/>
+      <c r="B44" s="37"/>
+      <c r="C44" s="25"/>
+      <c r="D44" s="27"/>
+      <c r="E44" s="27"/>
+      <c r="F44" s="26"/>
+      <c r="G44" s="26"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="26"/>
+      <c r="K44" s="27"/>
+      <c r="L44" s="26"/>
+      <c r="M44" s="26"/>
+    </row>
+    <row r="45" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="19"/>
+      <c r="B45" s="36"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="30"/>
+      <c r="F45" s="22"/>
+      <c r="G45" s="22"/>
+      <c r="H45" s="22"/>
+      <c r="I45" s="22"/>
+      <c r="J45" s="22"/>
+      <c r="K45" s="22"/>
+      <c r="L45" s="22"/>
+      <c r="M45" s="22"/>
+    </row>
+    <row r="46" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="23"/>
+      <c r="B46" s="37"/>
+      <c r="C46" s="25"/>
+      <c r="D46" s="27"/>
+      <c r="E46" s="27"/>
+      <c r="F46" s="26"/>
+      <c r="G46" s="26"/>
+      <c r="H46" s="26"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
+      <c r="K46" s="27"/>
+      <c r="L46" s="26"/>
+      <c r="M46" s="26"/>
+    </row>
+    <row r="47" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="19"/>
+      <c r="B47" s="36"/>
+      <c r="C47" s="21"/>
+      <c r="D47" s="30"/>
+      <c r="E47" s="30"/>
+      <c r="F47" s="22"/>
+      <c r="G47" s="22"/>
+      <c r="H47" s="22"/>
+      <c r="I47" s="22"/>
+      <c r="J47" s="22"/>
+      <c r="K47" s="22"/>
+      <c r="L47" s="22"/>
+      <c r="M47" s="22"/>
+    </row>
+    <row r="49" spans="1:13" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="B39" s="30"/>
-      <c r="C39" s="30"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="30"/>
-      <c r="G39" s="30"/>
-      <c r="H39" s="30"/>
-      <c r="I39" s="30"/>
-      <c r="J39" s="30"/>
-      <c r="K39" s="30"/>
-      <c r="L39" s="30"/>
-      <c r="M39" s="30"/>
-    </row>
-    <row r="40" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="15"/>
-      <c r="B40" s="45" t="s">
+      <c r="B49" s="38"/>
+      <c r="C49" s="38"/>
+      <c r="D49" s="38"/>
+      <c r="E49" s="38"/>
+      <c r="F49" s="38"/>
+      <c r="G49" s="38"/>
+      <c r="H49" s="38"/>
+      <c r="I49" s="38"/>
+      <c r="J49" s="38"/>
+      <c r="K49" s="38"/>
+      <c r="L49" s="38"/>
+      <c r="M49" s="38"/>
+    </row>
+    <row r="50" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="15"/>
+      <c r="B50" s="53" t="s">
         <v>226</v>
       </c>
-      <c r="C40" s="45"/>
-      <c r="D40" s="45"/>
-      <c r="E40" s="45"/>
-      <c r="F40" s="45"/>
-      <c r="G40" s="45"/>
-      <c r="H40" s="45"/>
-      <c r="I40" s="45"/>
-      <c r="J40" s="45"/>
-      <c r="K40" s="45"/>
-      <c r="L40" s="45"/>
-      <c r="M40" s="45"/>
-    </row>
-    <row r="41" spans="1:13" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="E41" s="8" t="s">
-        <v>222</v>
-      </c>
-      <c r="F41" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="G41" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="H41" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="I41" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="J41" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="K41" s="8"/>
-      <c r="L41" s="8"/>
-      <c r="M41" s="8"/>
-    </row>
-    <row r="42" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B42" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C42" s="57">
-        <v>1</v>
-      </c>
-      <c r="D42" s="57">
-        <v>1</v>
-      </c>
-      <c r="E42" s="22" t="s">
-        <v>221</v>
-      </c>
-      <c r="F42" s="22" t="s">
-        <v>191</v>
-      </c>
-      <c r="G42" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="H42" s="58" t="s">
-        <v>83</v>
-      </c>
-      <c r="I42" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="J42" s="58" t="s">
-        <v>83</v>
-      </c>
-      <c r="K42" s="22"/>
-      <c r="L42" s="22"/>
-      <c r="M42" s="22"/>
-    </row>
-    <row r="43" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="23"/>
-      <c r="B43" s="24"/>
-      <c r="C43" s="27"/>
-      <c r="D43" s="27"/>
-      <c r="E43" s="26"/>
-      <c r="F43" s="26"/>
-      <c r="G43" s="26"/>
-      <c r="H43" s="59"/>
-      <c r="I43" s="26"/>
-      <c r="J43" s="59"/>
-      <c r="K43" s="27"/>
-      <c r="L43" s="26"/>
-      <c r="M43" s="26"/>
-    </row>
-    <row r="44" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="19"/>
-      <c r="B44" s="20"/>
-      <c r="C44" s="57"/>
-      <c r="D44" s="57"/>
-      <c r="E44" s="22"/>
-      <c r="F44" s="22"/>
-      <c r="G44" s="22"/>
-      <c r="H44" s="58"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="58"/>
-      <c r="K44" s="22"/>
-      <c r="L44" s="22"/>
-      <c r="M44" s="22"/>
-    </row>
-    <row r="45" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="23"/>
-      <c r="B45" s="24"/>
-      <c r="C45" s="27"/>
-      <c r="D45" s="27"/>
-      <c r="E45" s="26"/>
-      <c r="F45" s="26"/>
-      <c r="G45" s="26"/>
-      <c r="H45" s="59"/>
-      <c r="I45" s="26"/>
-      <c r="J45" s="59"/>
-      <c r="K45" s="27"/>
-      <c r="L45" s="26"/>
-      <c r="M45" s="26"/>
-    </row>
-    <row r="46" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="19"/>
-      <c r="B46" s="20"/>
-      <c r="C46" s="57"/>
-      <c r="D46" s="57"/>
-      <c r="E46" s="22"/>
-      <c r="F46" s="22"/>
-      <c r="G46" s="22"/>
-      <c r="H46" s="58"/>
-      <c r="I46" s="22"/>
-      <c r="J46" s="58"/>
-      <c r="K46" s="22"/>
-      <c r="L46" s="22"/>
-      <c r="M46" s="22"/>
-    </row>
-    <row r="47" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="23"/>
-      <c r="B47" s="24"/>
-      <c r="C47" s="27"/>
-      <c r="D47" s="27"/>
-      <c r="E47" s="26"/>
-      <c r="F47" s="26"/>
-      <c r="G47" s="26"/>
-      <c r="H47" s="59"/>
-      <c r="I47" s="26"/>
-      <c r="J47" s="59"/>
-      <c r="K47" s="27"/>
-      <c r="L47" s="26"/>
-      <c r="M47" s="26"/>
-    </row>
-    <row r="48" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="19"/>
-      <c r="B48" s="20"/>
-      <c r="C48" s="57"/>
-      <c r="D48" s="57"/>
-      <c r="E48" s="22"/>
-      <c r="F48" s="22"/>
-      <c r="G48" s="22"/>
-      <c r="H48" s="58"/>
-      <c r="I48" s="22"/>
-      <c r="J48" s="58"/>
-      <c r="K48" s="22"/>
-      <c r="L48" s="22"/>
-      <c r="M48" s="22"/>
-    </row>
-    <row r="50" spans="1:13" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="30" t="s">
-        <v>115</v>
-      </c>
-      <c r="B50" s="30"/>
-      <c r="C50" s="30"/>
-      <c r="D50" s="30"/>
-      <c r="E50" s="30"/>
-      <c r="F50" s="30"/>
-      <c r="G50" s="30"/>
-      <c r="H50" s="30"/>
-      <c r="I50" s="30"/>
-      <c r="J50" s="30"/>
-      <c r="K50" s="30"/>
-      <c r="L50" s="30"/>
-      <c r="M50" s="30"/>
-    </row>
-    <row r="51" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C50" s="53"/>
+      <c r="D50" s="53"/>
+      <c r="E50" s="53"/>
+      <c r="F50" s="53"/>
+      <c r="G50" s="53"/>
+      <c r="H50" s="53"/>
+      <c r="I50" s="53"/>
+      <c r="J50" s="53"/>
+      <c r="K50" s="53"/>
+      <c r="L50" s="53"/>
+      <c r="M50" s="53"/>
+    </row>
+    <row r="51" spans="1:13" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C51" s="8"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="8"/>
-      <c r="F51" s="8"/>
-      <c r="G51" s="8"/>
-      <c r="H51" s="8"/>
-      <c r="I51" s="8"/>
-      <c r="J51" s="8"/>
+        <v>114</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="G51" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="H51" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="I51" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="J51" s="8" t="s">
+        <v>174</v>
+      </c>
       <c r="K51" s="8"/>
       <c r="L51" s="8"/>
       <c r="M51" s="8"/>
     </row>
     <row r="52" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B52" s="57">
-        <v>65513</v>
-      </c>
-      <c r="C52" s="21"/>
-      <c r="D52" s="22"/>
-      <c r="E52" s="22"/>
-      <c r="F52" s="22"/>
-      <c r="G52" s="22"/>
-      <c r="H52" s="22"/>
-      <c r="I52" s="22"/>
-      <c r="J52" s="22"/>
+        <v>14</v>
+      </c>
+      <c r="B52" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C52" s="30">
+        <v>1</v>
+      </c>
+      <c r="D52" s="30">
+        <v>1</v>
+      </c>
+      <c r="E52" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="F52" s="22" t="s">
+        <v>191</v>
+      </c>
+      <c r="G52" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="H52" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="I52" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J52" s="31" t="s">
+        <v>83</v>
+      </c>
       <c r="K52" s="22"/>
       <c r="L52" s="22"/>
       <c r="M52" s="22"/>
     </row>
-    <row r="54" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="B54" s="30"/>
+    <row r="53" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="23"/>
+      <c r="B53" s="24"/>
+      <c r="C53" s="27"/>
+      <c r="D53" s="27"/>
+      <c r="E53" s="26"/>
+      <c r="F53" s="26"/>
+      <c r="G53" s="26"/>
+      <c r="H53" s="32"/>
+      <c r="I53" s="26"/>
+      <c r="J53" s="32"/>
+      <c r="K53" s="27"/>
+      <c r="L53" s="26"/>
+      <c r="M53" s="26"/>
+    </row>
+    <row r="54" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="19"/>
+      <c r="B54" s="20"/>
       <c r="C54" s="30"/>
       <c r="D54" s="30"/>
-      <c r="E54" s="30"/>
-      <c r="F54" s="30"/>
-      <c r="G54" s="30"/>
-      <c r="H54" s="30"/>
-      <c r="I54" s="30"/>
-      <c r="J54" s="30"/>
-      <c r="K54" s="30"/>
-      <c r="L54" s="30"/>
-      <c r="M54" s="30"/>
-    </row>
-    <row r="55" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="15"/>
-      <c r="B55" s="45" t="s">
-        <v>227</v>
-      </c>
-      <c r="C55" s="45"/>
-      <c r="D55" s="45"/>
-      <c r="E55" s="45"/>
-      <c r="F55" s="45"/>
-      <c r="G55" s="45"/>
-      <c r="H55" s="45"/>
-      <c r="I55" s="45"/>
-      <c r="J55" s="45"/>
-      <c r="K55" s="45"/>
-      <c r="L55" s="45"/>
-      <c r="M55" s="45"/>
-    </row>
-    <row r="56" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B56" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="C56" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="D56" s="8"/>
-      <c r="E56" s="8"/>
-      <c r="F56" s="8"/>
-      <c r="G56" s="8"/>
-      <c r="H56" s="8"/>
-      <c r="I56" s="8"/>
-      <c r="J56" s="8"/>
-      <c r="K56" s="8"/>
-      <c r="L56" s="8"/>
-      <c r="M56" s="8"/>
-    </row>
-    <row r="57" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B57" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="C57" s="20">
-        <v>101</v>
-      </c>
-      <c r="D57" s="22"/>
-      <c r="E57" s="22"/>
-      <c r="F57" s="22"/>
-      <c r="G57" s="22"/>
-      <c r="H57" s="22"/>
-      <c r="I57" s="22"/>
-      <c r="J57" s="22"/>
-      <c r="K57" s="22"/>
-      <c r="L57" s="22"/>
-      <c r="M57" s="22"/>
-    </row>
-    <row r="58" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="23"/>
-      <c r="B58" s="24"/>
-      <c r="C58" s="24"/>
-      <c r="D58" s="26"/>
-      <c r="E58" s="26"/>
-      <c r="F58" s="26"/>
-      <c r="G58" s="26"/>
-      <c r="H58" s="26"/>
-      <c r="I58" s="26"/>
-      <c r="J58" s="26"/>
-      <c r="K58" s="27"/>
-      <c r="L58" s="26"/>
-      <c r="M58" s="26"/>
-    </row>
-    <row r="60" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="30" t="s">
-        <v>118</v>
-      </c>
-      <c r="B60" s="30"/>
-      <c r="C60" s="30"/>
-      <c r="D60" s="30"/>
-      <c r="E60" s="30"/>
-      <c r="F60" s="30"/>
-      <c r="G60" s="30"/>
-      <c r="H60" s="30"/>
-      <c r="I60" s="30"/>
-      <c r="J60" s="30"/>
-      <c r="K60" s="30"/>
-      <c r="L60" s="30"/>
-      <c r="M60" s="30"/>
-    </row>
-    <row r="61" spans="1:13" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E54" s="22"/>
+      <c r="F54" s="22"/>
+      <c r="G54" s="22"/>
+      <c r="H54" s="31"/>
+      <c r="I54" s="22"/>
+      <c r="J54" s="31"/>
+      <c r="K54" s="22"/>
+      <c r="L54" s="22"/>
+      <c r="M54" s="22"/>
+    </row>
+    <row r="55" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="23"/>
+      <c r="B55" s="24"/>
+      <c r="C55" s="27"/>
+      <c r="D55" s="27"/>
+      <c r="E55" s="26"/>
+      <c r="F55" s="26"/>
+      <c r="G55" s="26"/>
+      <c r="H55" s="32"/>
+      <c r="I55" s="26"/>
+      <c r="J55" s="32"/>
+      <c r="K55" s="27"/>
+      <c r="L55" s="26"/>
+      <c r="M55" s="26"/>
+    </row>
+    <row r="56" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="19"/>
+      <c r="B56" s="20"/>
+      <c r="C56" s="30"/>
+      <c r="D56" s="30"/>
+      <c r="E56" s="22"/>
+      <c r="F56" s="22"/>
+      <c r="G56" s="22"/>
+      <c r="H56" s="31"/>
+      <c r="I56" s="22"/>
+      <c r="J56" s="31"/>
+      <c r="K56" s="22"/>
+      <c r="L56" s="22"/>
+      <c r="M56" s="22"/>
+    </row>
+    <row r="57" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="23"/>
+      <c r="B57" s="24"/>
+      <c r="C57" s="27"/>
+      <c r="D57" s="27"/>
+      <c r="E57" s="26"/>
+      <c r="F57" s="26"/>
+      <c r="G57" s="26"/>
+      <c r="H57" s="32"/>
+      <c r="I57" s="26"/>
+      <c r="J57" s="32"/>
+      <c r="K57" s="27"/>
+      <c r="L57" s="26"/>
+      <c r="M57" s="26"/>
+    </row>
+    <row r="58" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="19"/>
+      <c r="B58" s="20"/>
+      <c r="C58" s="30"/>
+      <c r="D58" s="30"/>
+      <c r="E58" s="22"/>
+      <c r="F58" s="22"/>
+      <c r="G58" s="22"/>
+      <c r="H58" s="31"/>
+      <c r="I58" s="22"/>
+      <c r="J58" s="31"/>
+      <c r="K58" s="22"/>
+      <c r="L58" s="22"/>
+      <c r="M58" s="22"/>
+    </row>
+    <row r="60" spans="1:13" s="6" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="38" t="s">
+        <v>115</v>
+      </c>
+      <c r="B60" s="38"/>
+      <c r="C60" s="38"/>
+      <c r="D60" s="38"/>
+      <c r="E60" s="38"/>
+      <c r="F60" s="38"/>
+      <c r="G60" s="38"/>
+      <c r="H60" s="38"/>
+      <c r="I60" s="38"/>
+      <c r="J60" s="38"/>
+      <c r="K60" s="38"/>
+      <c r="L60" s="38"/>
+      <c r="M60" s="38"/>
+    </row>
+    <row r="61" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B61" s="9" t="s">
-        <v>106</v>
+      <c r="B61" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="C61" s="8"/>
       <c r="D61" s="8"/>
@@ -3672,10 +3944,10 @@
     </row>
     <row r="62" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B62" s="20" t="s">
-        <v>20</v>
+        <v>17</v>
+      </c>
+      <c r="B62" s="30">
+        <v>65513</v>
       </c>
       <c r="C62" s="21"/>
       <c r="D62" s="22"/>
@@ -3690,48 +3962,48 @@
       <c r="M62" s="22"/>
     </row>
     <row r="64" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="B64" s="30"/>
-      <c r="C64" s="30"/>
-      <c r="D64" s="30"/>
-      <c r="E64" s="30"/>
-      <c r="F64" s="30"/>
-      <c r="G64" s="30"/>
-      <c r="H64" s="30"/>
-      <c r="I64" s="30"/>
-      <c r="J64" s="30"/>
-      <c r="K64" s="30"/>
-      <c r="L64" s="30"/>
-      <c r="M64" s="30"/>
+      <c r="A64" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="B64" s="38"/>
+      <c r="C64" s="38"/>
+      <c r="D64" s="38"/>
+      <c r="E64" s="38"/>
+      <c r="F64" s="38"/>
+      <c r="G64" s="38"/>
+      <c r="H64" s="38"/>
+      <c r="I64" s="38"/>
+      <c r="J64" s="38"/>
+      <c r="K64" s="38"/>
+      <c r="L64" s="38"/>
+      <c r="M64" s="38"/>
     </row>
     <row r="65" spans="1:16" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="15"/>
-      <c r="B65" s="45" t="s">
-        <v>228</v>
-      </c>
-      <c r="C65" s="45"/>
-      <c r="D65" s="45"/>
-      <c r="E65" s="45"/>
-      <c r="F65" s="45"/>
-      <c r="G65" s="45"/>
-      <c r="H65" s="45"/>
-      <c r="I65" s="45"/>
-      <c r="J65" s="45"/>
-      <c r="K65" s="45"/>
-      <c r="L65" s="45"/>
-      <c r="M65" s="45"/>
+      <c r="B65" s="53" t="s">
+        <v>227</v>
+      </c>
+      <c r="C65" s="53"/>
+      <c r="D65" s="53"/>
+      <c r="E65" s="53"/>
+      <c r="F65" s="53"/>
+      <c r="G65" s="53"/>
+      <c r="H65" s="53"/>
+      <c r="I65" s="53"/>
+      <c r="J65" s="53"/>
+      <c r="K65" s="53"/>
+      <c r="L65" s="53"/>
+      <c r="M65" s="53"/>
     </row>
     <row r="66" spans="1:16" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>21</v>
+        <v>108</v>
       </c>
       <c r="D66" s="8"/>
       <c r="E66" s="8"/>
@@ -3744,15 +4016,15 @@
       <c r="L66" s="8"/>
       <c r="M66" s="8"/>
     </row>
-    <row r="67" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:16" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="19" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B67" s="20" t="s">
-        <v>196</v>
-      </c>
-      <c r="C67" s="21" t="s">
-        <v>23</v>
+        <v>12</v>
+      </c>
+      <c r="C67" s="36">
+        <v>101</v>
       </c>
       <c r="D67" s="22"/>
       <c r="E67" s="22"/>
@@ -3765,16 +4037,10 @@
       <c r="L67" s="22"/>
       <c r="M67" s="22"/>
     </row>
-    <row r="68" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="B68" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="C68" s="25" t="s">
-        <v>24</v>
-      </c>
+    <row r="68" spans="1:16" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="23"/>
+      <c r="B68" s="24"/>
+      <c r="C68" s="37"/>
       <c r="D68" s="26"/>
       <c r="E68" s="26"/>
       <c r="F68" s="26"/>
@@ -3786,165 +4052,106 @@
       <c r="L68" s="26"/>
       <c r="M68" s="26"/>
     </row>
-    <row r="70" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="39" t="s">
-        <v>120</v>
-      </c>
-      <c r="B70" s="39"/>
-      <c r="C70" s="39"/>
-      <c r="D70" s="39"/>
-      <c r="E70" s="39"/>
-      <c r="F70" s="39"/>
-      <c r="G70" s="39"/>
-      <c r="H70" s="39"/>
-      <c r="I70" s="39"/>
-      <c r="J70" s="39"/>
-      <c r="K70" s="39"/>
-      <c r="L70" s="39"/>
-      <c r="M70" s="39"/>
-      <c r="N70" s="16"/>
-      <c r="O70" s="16"/>
-      <c r="P70" s="16"/>
-    </row>
-    <row r="71" spans="1:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="17"/>
-      <c r="B71" s="54" t="s">
-        <v>229</v>
-      </c>
-      <c r="C71" s="54"/>
-      <c r="D71" s="54"/>
-      <c r="E71" s="54"/>
-      <c r="F71" s="54"/>
-      <c r="G71" s="54"/>
-      <c r="H71" s="54"/>
-      <c r="I71" s="54"/>
-      <c r="J71" s="54"/>
-      <c r="K71" s="54"/>
-      <c r="L71" s="54"/>
-      <c r="M71" s="54"/>
-      <c r="N71" s="17"/>
-      <c r="O71" s="17"/>
-      <c r="P71" s="17"/>
-    </row>
-    <row r="72" spans="1:16" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="8" t="s">
+    <row r="70" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="B70" s="38"/>
+      <c r="C70" s="38"/>
+      <c r="D70" s="38"/>
+      <c r="E70" s="38"/>
+      <c r="F70" s="38"/>
+      <c r="G70" s="38"/>
+      <c r="H70" s="38"/>
+      <c r="I70" s="38"/>
+      <c r="J70" s="38"/>
+      <c r="K70" s="38"/>
+      <c r="L70" s="38"/>
+      <c r="M70" s="38"/>
+    </row>
+    <row r="71" spans="1:16" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B72" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="C72" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="D72" s="8" t="s">
+      <c r="B71" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="E72" s="33" t="s">
-        <v>131</v>
-      </c>
-      <c r="F72" s="34"/>
-      <c r="G72" s="33" t="s">
-        <v>132</v>
-      </c>
-      <c r="H72" s="34"/>
-      <c r="I72" s="33" t="s">
-        <v>133</v>
-      </c>
-      <c r="J72" s="34"/>
-      <c r="K72" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="L72" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="M72" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="N72" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="O72" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="P72" s="8" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="73" spans="1:16" s="4" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="B73" s="20">
-        <v>25</v>
-      </c>
-      <c r="C73" s="21" t="s">
-        <v>182</v>
-      </c>
-      <c r="D73" s="58" t="s">
+      <c r="C71" s="8"/>
+      <c r="D71" s="8"/>
+      <c r="E71" s="8"/>
+      <c r="F71" s="8"/>
+      <c r="G71" s="8"/>
+      <c r="H71" s="8"/>
+      <c r="I71" s="8"/>
+      <c r="J71" s="8"/>
+      <c r="K71" s="8"/>
+      <c r="L71" s="8"/>
+      <c r="M71" s="8"/>
+    </row>
+    <row r="72" spans="1:16" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B72" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="E73" s="60" t="s">
-        <v>183</v>
-      </c>
-      <c r="F73" s="61"/>
-      <c r="G73" s="60" t="s">
-        <v>184</v>
-      </c>
-      <c r="H73" s="61"/>
-      <c r="I73" s="60" t="s">
-        <v>184</v>
-      </c>
-      <c r="J73" s="61"/>
-      <c r="K73" s="21" t="s">
-        <v>185</v>
-      </c>
-      <c r="L73" s="58" t="s">
-        <v>186</v>
-      </c>
-      <c r="M73" s="21" t="s">
-        <v>187</v>
-      </c>
-      <c r="N73" s="58">
-        <v>5555555</v>
-      </c>
-      <c r="O73" s="21">
-        <v>5555555</v>
-      </c>
-      <c r="P73" s="58">
-        <v>555555</v>
-      </c>
-    </row>
-    <row r="74" spans="1:16" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="75" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="30" t="s">
-        <v>123</v>
-      </c>
-      <c r="B75" s="30"/>
-      <c r="C75" s="30"/>
-      <c r="D75" s="30"/>
-      <c r="E75" s="30"/>
-      <c r="F75" s="30"/>
-      <c r="G75" s="30"/>
-      <c r="H75" s="30"/>
-      <c r="I75" s="30"/>
-      <c r="J75" s="30"/>
-      <c r="K75" s="30"/>
-      <c r="L75" s="30"/>
-      <c r="M75" s="30"/>
-    </row>
-    <row r="76" spans="1:16" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C72" s="21"/>
+      <c r="D72" s="22"/>
+      <c r="E72" s="22"/>
+      <c r="F72" s="22"/>
+      <c r="G72" s="22"/>
+      <c r="H72" s="22"/>
+      <c r="I72" s="22"/>
+      <c r="J72" s="22"/>
+      <c r="K72" s="22"/>
+      <c r="L72" s="22"/>
+      <c r="M72" s="22"/>
+    </row>
+    <row r="74" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="B74" s="38"/>
+      <c r="C74" s="38"/>
+      <c r="D74" s="38"/>
+      <c r="E74" s="38"/>
+      <c r="F74" s="38"/>
+      <c r="G74" s="38"/>
+      <c r="H74" s="38"/>
+      <c r="I74" s="38"/>
+      <c r="J74" s="38"/>
+      <c r="K74" s="38"/>
+      <c r="L74" s="38"/>
+      <c r="M74" s="38"/>
+    </row>
+    <row r="75" spans="1:16" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="15"/>
+      <c r="B75" s="53" t="s">
+        <v>228</v>
+      </c>
+      <c r="C75" s="53"/>
+      <c r="D75" s="53"/>
+      <c r="E75" s="53"/>
+      <c r="F75" s="53"/>
+      <c r="G75" s="53"/>
+      <c r="H75" s="53"/>
+      <c r="I75" s="53"/>
+      <c r="J75" s="53"/>
+      <c r="K75" s="53"/>
+      <c r="L75" s="53"/>
+      <c r="M75" s="53"/>
+    </row>
+    <row r="76" spans="1:16" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C76" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D76" s="8" t="s">
-        <v>106</v>
-      </c>
+      <c r="D76" s="8"/>
       <c r="E76" s="8"/>
       <c r="F76" s="8"/>
       <c r="G76" s="8"/>
@@ -3957,17 +4164,15 @@
     </row>
     <row r="77" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="19" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B77" s="20" t="s">
         <v>196</v>
       </c>
       <c r="C77" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="D77" s="22" t="s">
-        <v>20</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="D77" s="22"/>
       <c r="E77" s="22"/>
       <c r="F77" s="22"/>
       <c r="G77" s="22"/>
@@ -3980,17 +4185,15 @@
     </row>
     <row r="78" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="23" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B78" s="24" t="s">
         <v>197</v>
       </c>
       <c r="C78" s="25" t="s">
-        <v>122</v>
-      </c>
-      <c r="D78" s="26" t="s">
-        <v>20</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="D78" s="26"/>
       <c r="E78" s="26"/>
       <c r="F78" s="26"/>
       <c r="G78" s="26"/>
@@ -4001,112 +4204,161 @@
       <c r="L78" s="26"/>
       <c r="M78" s="26"/>
     </row>
-    <row r="80" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="30" t="s">
-        <v>124</v>
-      </c>
-      <c r="B80" s="30"/>
-      <c r="C80" s="30"/>
-      <c r="D80" s="30"/>
-      <c r="E80" s="30"/>
-      <c r="F80" s="30"/>
-      <c r="G80" s="30"/>
-      <c r="H80" s="30"/>
-      <c r="I80" s="30"/>
-      <c r="J80" s="30"/>
-      <c r="K80" s="30"/>
-      <c r="L80" s="30"/>
-      <c r="M80" s="30"/>
-    </row>
-    <row r="81" spans="1:13" s="3" customFormat="1" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="8" t="s">
+    <row r="80" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="B80" s="47"/>
+      <c r="C80" s="47"/>
+      <c r="D80" s="47"/>
+      <c r="E80" s="47"/>
+      <c r="F80" s="47"/>
+      <c r="G80" s="47"/>
+      <c r="H80" s="47"/>
+      <c r="I80" s="47"/>
+      <c r="J80" s="47"/>
+      <c r="K80" s="47"/>
+      <c r="L80" s="47"/>
+      <c r="M80" s="47"/>
+      <c r="N80" s="16"/>
+      <c r="O80" s="16"/>
+      <c r="P80" s="16"/>
+    </row>
+    <row r="81" spans="1:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="17"/>
+      <c r="B81" s="62" t="s">
+        <v>229</v>
+      </c>
+      <c r="C81" s="62"/>
+      <c r="D81" s="62"/>
+      <c r="E81" s="62"/>
+      <c r="F81" s="62"/>
+      <c r="G81" s="62"/>
+      <c r="H81" s="62"/>
+      <c r="I81" s="62"/>
+      <c r="J81" s="62"/>
+      <c r="K81" s="62"/>
+      <c r="L81" s="62"/>
+      <c r="M81" s="62"/>
+      <c r="N81" s="17"/>
+      <c r="O81" s="17"/>
+      <c r="P81" s="17"/>
+    </row>
+    <row r="82" spans="1:16" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B81" s="40" t="s">
-        <v>28</v>
-      </c>
-      <c r="C81" s="42"/>
-      <c r="D81" s="40" t="s">
-        <v>125</v>
-      </c>
-      <c r="E81" s="42"/>
-      <c r="F81" s="8"/>
-      <c r="G81" s="8"/>
-      <c r="H81" s="8"/>
-      <c r="I81" s="8"/>
-      <c r="J81" s="8"/>
-      <c r="K81" s="8"/>
-      <c r="L81" s="8"/>
-      <c r="M81" s="8"/>
-    </row>
-    <row r="82" spans="1:13" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="B82" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="C82" s="38"/>
-      <c r="D82" s="37" t="s">
-        <v>24</v>
-      </c>
-      <c r="E82" s="38"/>
-      <c r="F82" s="22"/>
-      <c r="G82" s="22"/>
-      <c r="H82" s="22"/>
-      <c r="I82" s="22"/>
-      <c r="J82" s="22"/>
-      <c r="K82" s="22"/>
-      <c r="L82" s="22"/>
-      <c r="M82" s="22"/>
-    </row>
-    <row r="83" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="B83" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="C83" s="32"/>
+      <c r="B82" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C82" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="D82" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="E82" s="41" t="s">
+        <v>131</v>
+      </c>
+      <c r="F82" s="42"/>
+      <c r="G82" s="41" t="s">
+        <v>132</v>
+      </c>
+      <c r="H82" s="42"/>
+      <c r="I82" s="41" t="s">
+        <v>133</v>
+      </c>
+      <c r="J82" s="42"/>
+      <c r="K82" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="L82" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="M82" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="N82" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="O82" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="P82" s="8" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16" s="4" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B83" s="36">
+        <v>25</v>
+      </c>
+      <c r="C83" s="21" t="s">
+        <v>182</v>
+      </c>
       <c r="D83" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="E83" s="32"/>
-      <c r="F83" s="26"/>
-      <c r="G83" s="26"/>
-      <c r="H83" s="26"/>
-      <c r="I83" s="26"/>
-      <c r="J83" s="26"/>
-      <c r="K83" s="27"/>
-      <c r="L83" s="26"/>
-      <c r="M83" s="26"/>
-    </row>
-    <row r="85" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="30" t="s">
-        <v>126</v>
-      </c>
-      <c r="B85" s="30"/>
-      <c r="C85" s="30"/>
-      <c r="D85" s="30"/>
-      <c r="E85" s="30"/>
-      <c r="F85" s="30"/>
-      <c r="G85" s="30"/>
-      <c r="H85" s="30"/>
-      <c r="I85" s="30"/>
-      <c r="J85" s="30"/>
-      <c r="K85" s="30"/>
-      <c r="L85" s="30"/>
-      <c r="M85" s="30"/>
-    </row>
-    <row r="86" spans="1:13" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="E83" s="43" t="s">
+        <v>183</v>
+      </c>
+      <c r="F83" s="44"/>
+      <c r="G83" s="43" t="s">
+        <v>184</v>
+      </c>
+      <c r="H83" s="44"/>
+      <c r="I83" s="43" t="s">
+        <v>184</v>
+      </c>
+      <c r="J83" s="44"/>
+      <c r="K83" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="L83" s="31" t="s">
+        <v>186</v>
+      </c>
+      <c r="M83" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="N83" s="31">
+        <v>5555555</v>
+      </c>
+      <c r="O83" s="21">
+        <v>5555555</v>
+      </c>
+      <c r="P83" s="31">
+        <v>555555</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="85" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="B85" s="38"/>
+      <c r="C85" s="38"/>
+      <c r="D85" s="38"/>
+      <c r="E85" s="38"/>
+      <c r="F85" s="38"/>
+      <c r="G85" s="38"/>
+      <c r="H85" s="38"/>
+      <c r="I85" s="38"/>
+      <c r="J85" s="38"/>
+      <c r="K85" s="38"/>
+      <c r="L85" s="38"/>
+      <c r="M85" s="38"/>
+    </row>
+    <row r="86" spans="1:16" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>169</v>
+        <v>139</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>170</v>
+        <v>21</v>
       </c>
       <c r="D86" s="8" t="s">
         <v>106</v>
@@ -4121,15 +4373,15 @@
       <c r="L86" s="8"/>
       <c r="M86" s="8"/>
     </row>
-    <row r="87" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="19" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B87" s="20" t="s">
-        <v>32</v>
+        <v>196</v>
       </c>
       <c r="C87" s="21" t="s">
-        <v>198</v>
+        <v>121</v>
       </c>
       <c r="D87" s="22" t="s">
         <v>20</v>
@@ -4144,15 +4396,15 @@
       <c r="L87" s="22"/>
       <c r="M87" s="22"/>
     </row>
-    <row r="88" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="23" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B88" s="24" t="s">
-        <v>33</v>
+        <v>197</v>
       </c>
       <c r="C88" s="25" t="s">
-        <v>199</v>
+        <v>122</v>
       </c>
       <c r="D88" s="26" t="s">
         <v>20</v>
@@ -4167,36 +4419,36 @@
       <c r="L88" s="26"/>
       <c r="M88" s="26"/>
     </row>
-    <row r="90" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="30" t="s">
-        <v>147</v>
-      </c>
-      <c r="B90" s="30"/>
-      <c r="C90" s="30"/>
-      <c r="D90" s="30"/>
-      <c r="E90" s="30"/>
-      <c r="F90" s="30"/>
-      <c r="G90" s="30"/>
-      <c r="H90" s="30"/>
-      <c r="I90" s="30"/>
-      <c r="J90" s="30"/>
-      <c r="K90" s="30"/>
-      <c r="L90" s="30"/>
-      <c r="M90" s="30"/>
-    </row>
-    <row r="91" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="B90" s="38"/>
+      <c r="C90" s="38"/>
+      <c r="D90" s="38"/>
+      <c r="E90" s="38"/>
+      <c r="F90" s="38"/>
+      <c r="G90" s="38"/>
+      <c r="H90" s="38"/>
+      <c r="I90" s="38"/>
+      <c r="J90" s="38"/>
+      <c r="K90" s="38"/>
+      <c r="L90" s="38"/>
+      <c r="M90" s="38"/>
+    </row>
+    <row r="91" spans="1:16" s="3" customFormat="1" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B91" s="41" t="s">
-        <v>145</v>
-      </c>
-      <c r="C91" s="41"/>
-      <c r="D91" s="40" t="s">
-        <v>146</v>
-      </c>
-      <c r="E91" s="41"/>
-      <c r="F91" s="42"/>
+      <c r="B91" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="C91" s="50"/>
+      <c r="D91" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="E91" s="50"/>
+      <c r="F91" s="8"/>
       <c r="G91" s="8"/>
       <c r="H91" s="8"/>
       <c r="I91" s="8"/>
@@ -4205,18 +4457,18 @@
       <c r="L91" s="8"/>
       <c r="M91" s="8"/>
     </row>
-    <row r="92" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="B92" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="C92" s="36"/>
-      <c r="D92" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="E92" s="22"/>
+        <v>29</v>
+      </c>
+      <c r="B92" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="C92" s="46"/>
+      <c r="D92" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="E92" s="46"/>
       <c r="F92" s="22"/>
       <c r="G92" s="22"/>
       <c r="H92" s="22"/>
@@ -4226,55 +4478,58 @@
       <c r="L92" s="22"/>
       <c r="M92" s="22"/>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B93" s="7"/>
-    </row>
-    <row r="94" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="30" t="s">
-        <v>140</v>
-      </c>
-      <c r="B94" s="30"/>
-      <c r="C94" s="30"/>
-      <c r="D94" s="30"/>
-      <c r="E94" s="30"/>
-      <c r="F94" s="30"/>
-      <c r="G94" s="30"/>
-      <c r="H94" s="30"/>
-      <c r="I94" s="30"/>
-      <c r="J94" s="30"/>
-      <c r="K94" s="30"/>
-      <c r="L94" s="30"/>
-      <c r="M94" s="30"/>
-    </row>
-    <row r="95" spans="1:13" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="15"/>
-      <c r="B95" s="45" t="s">
-        <v>235</v>
-      </c>
-      <c r="C95" s="45"/>
-      <c r="D95" s="45"/>
-      <c r="E95" s="45"/>
-      <c r="F95" s="45"/>
-      <c r="G95" s="45"/>
-      <c r="H95" s="45"/>
-      <c r="I95" s="45"/>
-      <c r="J95" s="45"/>
-      <c r="K95" s="45"/>
-      <c r="L95" s="45"/>
-      <c r="M95" s="45"/>
-    </row>
-    <row r="96" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B93" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="C93" s="40"/>
+      <c r="D93" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="E93" s="40"/>
+      <c r="F93" s="26"/>
+      <c r="G93" s="26"/>
+      <c r="H93" s="26"/>
+      <c r="I93" s="26"/>
+      <c r="J93" s="26"/>
+      <c r="K93" s="27"/>
+      <c r="L93" s="26"/>
+      <c r="M93" s="26"/>
+    </row>
+    <row r="95" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="38" t="s">
+        <v>126</v>
+      </c>
+      <c r="B95" s="38"/>
+      <c r="C95" s="38"/>
+      <c r="D95" s="38"/>
+      <c r="E95" s="38"/>
+      <c r="F95" s="38"/>
+      <c r="G95" s="38"/>
+      <c r="H95" s="38"/>
+      <c r="I95" s="38"/>
+      <c r="J95" s="38"/>
+      <c r="K95" s="38"/>
+      <c r="L95" s="38"/>
+      <c r="M95" s="38"/>
+    </row>
+    <row r="96" spans="1:16" s="3" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="C96" s="40" t="s">
-        <v>36</v>
-      </c>
-      <c r="D96" s="41"/>
-      <c r="E96" s="42"/>
+        <v>169</v>
+      </c>
+      <c r="C96" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="D96" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="E96" s="8"/>
       <c r="F96" s="8"/>
       <c r="G96" s="8"/>
       <c r="H96" s="8"/>
@@ -4284,18 +4539,20 @@
       <c r="L96" s="8"/>
       <c r="M96" s="8"/>
     </row>
-    <row r="97" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="B97" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="C97" s="37" t="s">
-        <v>223</v>
-      </c>
-      <c r="D97" s="43"/>
-      <c r="E97" s="38"/>
+        <v>31</v>
+      </c>
+      <c r="B97" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C97" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="D97" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="E97" s="22"/>
       <c r="F97" s="22"/>
       <c r="G97" s="22"/>
       <c r="H97" s="22"/>
@@ -4305,18 +4562,20 @@
       <c r="L97" s="22"/>
       <c r="M97" s="22"/>
     </row>
-    <row r="98" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="B98" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="C98" s="31" t="s">
-        <v>224</v>
-      </c>
-      <c r="D98" s="44"/>
-      <c r="E98" s="32"/>
+        <v>31</v>
+      </c>
+      <c r="B98" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C98" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="D98" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="E98" s="26"/>
       <c r="F98" s="26"/>
       <c r="G98" s="26"/>
       <c r="H98" s="26"/>
@@ -4326,954 +4585,1145 @@
       <c r="L98" s="26"/>
       <c r="M98" s="26"/>
     </row>
-    <row r="99" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="100" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="39" t="s">
+      <c r="A100" s="38" t="s">
+        <v>147</v>
+      </c>
+      <c r="B100" s="38"/>
+      <c r="C100" s="38"/>
+      <c r="D100" s="38"/>
+      <c r="E100" s="38"/>
+      <c r="F100" s="38"/>
+      <c r="G100" s="38"/>
+      <c r="H100" s="38"/>
+      <c r="I100" s="38"/>
+      <c r="J100" s="38"/>
+      <c r="K100" s="38"/>
+      <c r="L100" s="38"/>
+      <c r="M100" s="38"/>
+    </row>
+    <row r="101" spans="1:13" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B101" s="49" t="s">
+        <v>145</v>
+      </c>
+      <c r="C101" s="49"/>
+      <c r="D101" s="48" t="s">
+        <v>146</v>
+      </c>
+      <c r="E101" s="49"/>
+      <c r="F101" s="50"/>
+      <c r="G101" s="8"/>
+      <c r="H101" s="8"/>
+      <c r="I101" s="8"/>
+      <c r="J101" s="8"/>
+      <c r="K101" s="8"/>
+      <c r="L101" s="8"/>
+      <c r="M101" s="8"/>
+    </row>
+    <row r="102" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B102" s="63" t="s">
+        <v>26</v>
+      </c>
+      <c r="C102" s="64"/>
+      <c r="D102" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="E102" s="22"/>
+      <c r="F102" s="22"/>
+      <c r="G102" s="22"/>
+      <c r="H102" s="22"/>
+      <c r="I102" s="22"/>
+      <c r="J102" s="22"/>
+      <c r="K102" s="22"/>
+      <c r="L102" s="22"/>
+      <c r="M102" s="22"/>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B103" s="7"/>
+    </row>
+    <row r="104" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="38" t="s">
+        <v>140</v>
+      </c>
+      <c r="B104" s="38"/>
+      <c r="C104" s="38"/>
+      <c r="D104" s="38"/>
+      <c r="E104" s="38"/>
+      <c r="F104" s="38"/>
+      <c r="G104" s="38"/>
+      <c r="H104" s="38"/>
+      <c r="I104" s="38"/>
+      <c r="J104" s="38"/>
+      <c r="K104" s="38"/>
+      <c r="L104" s="38"/>
+      <c r="M104" s="38"/>
+    </row>
+    <row r="105" spans="1:13" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="15"/>
+      <c r="B105" s="53" t="s">
+        <v>235</v>
+      </c>
+      <c r="C105" s="53"/>
+      <c r="D105" s="53"/>
+      <c r="E105" s="53"/>
+      <c r="F105" s="53"/>
+      <c r="G105" s="53"/>
+      <c r="H105" s="53"/>
+      <c r="I105" s="53"/>
+      <c r="J105" s="53"/>
+      <c r="K105" s="53"/>
+      <c r="L105" s="53"/>
+      <c r="M105" s="53"/>
+    </row>
+    <row r="106" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B106" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="C106" s="48" t="s">
+        <v>36</v>
+      </c>
+      <c r="D106" s="49"/>
+      <c r="E106" s="50"/>
+      <c r="F106" s="8"/>
+      <c r="G106" s="8"/>
+      <c r="H106" s="8"/>
+      <c r="I106" s="8"/>
+      <c r="J106" s="8"/>
+      <c r="K106" s="8"/>
+      <c r="L106" s="8"/>
+      <c r="M106" s="8"/>
+    </row>
+    <row r="107" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B107" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="C107" s="45" t="s">
+        <v>223</v>
+      </c>
+      <c r="D107" s="51"/>
+      <c r="E107" s="46"/>
+      <c r="F107" s="22"/>
+      <c r="G107" s="22"/>
+      <c r="H107" s="22"/>
+      <c r="I107" s="22"/>
+      <c r="J107" s="22"/>
+      <c r="K107" s="22"/>
+      <c r="L107" s="22"/>
+      <c r="M107" s="22"/>
+    </row>
+    <row r="108" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B108" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C108" s="39" t="s">
+        <v>224</v>
+      </c>
+      <c r="D108" s="52"/>
+      <c r="E108" s="40"/>
+      <c r="F108" s="26"/>
+      <c r="G108" s="26"/>
+      <c r="H108" s="26"/>
+      <c r="I108" s="26"/>
+      <c r="J108" s="26"/>
+      <c r="K108" s="27"/>
+      <c r="L108" s="26"/>
+      <c r="M108" s="26"/>
+    </row>
+    <row r="109" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="110" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="47" t="s">
         <v>148</v>
       </c>
-      <c r="B100" s="39"/>
-      <c r="C100" s="39"/>
-      <c r="D100" s="39"/>
-      <c r="E100" s="39"/>
-      <c r="F100" s="39"/>
-      <c r="G100" s="39"/>
-      <c r="H100" s="39"/>
-      <c r="I100" s="39"/>
-      <c r="J100" s="39"/>
-      <c r="K100" s="39"/>
-      <c r="L100" s="39"/>
-      <c r="M100" s="39"/>
-    </row>
-    <row r="101" spans="1:13" ht="35.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="15"/>
-      <c r="B101" s="45" t="s">
+      <c r="B110" s="47"/>
+      <c r="C110" s="47"/>
+      <c r="D110" s="47"/>
+      <c r="E110" s="47"/>
+      <c r="F110" s="47"/>
+      <c r="G110" s="47"/>
+      <c r="H110" s="47"/>
+      <c r="I110" s="47"/>
+      <c r="J110" s="47"/>
+      <c r="K110" s="47"/>
+      <c r="L110" s="47"/>
+      <c r="M110" s="47"/>
+    </row>
+    <row r="111" spans="1:13" ht="35.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="15"/>
+      <c r="B111" s="53" t="s">
         <v>236</v>
       </c>
-      <c r="C101" s="45"/>
-      <c r="D101" s="45"/>
-      <c r="E101" s="45"/>
-      <c r="F101" s="45"/>
-      <c r="G101" s="45"/>
-      <c r="H101" s="45"/>
-      <c r="I101" s="45"/>
-      <c r="J101" s="45"/>
-      <c r="K101" s="45"/>
-      <c r="L101" s="45"/>
-      <c r="M101" s="45"/>
-    </row>
-    <row r="102" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="8" t="s">
+      <c r="C111" s="53"/>
+      <c r="D111" s="53"/>
+      <c r="E111" s="53"/>
+      <c r="F111" s="53"/>
+      <c r="G111" s="53"/>
+      <c r="H111" s="53"/>
+      <c r="I111" s="53"/>
+      <c r="J111" s="53"/>
+      <c r="K111" s="53"/>
+      <c r="L111" s="53"/>
+      <c r="M111" s="53"/>
+    </row>
+    <row r="112" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B102" s="8" t="s">
+      <c r="B112" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="C102" s="8" t="s">
+      <c r="C112" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="D102" s="8" t="s">
+      <c r="D112" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="E102" s="8" t="s">
+      <c r="E112" s="8" t="s">
         <v>230</v>
       </c>
-      <c r="F102" s="8" t="s">
+      <c r="F112" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="G102" s="8" t="s">
+      <c r="G112" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="H102" s="8"/>
-      <c r="I102" s="8"/>
-      <c r="J102" s="8"/>
-      <c r="K102" s="8"/>
-      <c r="L102" s="8"/>
-      <c r="M102" s="8"/>
-    </row>
-    <row r="103" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="19" t="s">
+      <c r="H112" s="8"/>
+      <c r="I112" s="8"/>
+      <c r="J112" s="8"/>
+      <c r="K112" s="8"/>
+      <c r="L112" s="8"/>
+      <c r="M112" s="8"/>
+    </row>
+    <row r="113" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="B103" s="20" t="s">
+      <c r="B113" s="20" t="s">
         <v>198</v>
       </c>
-      <c r="C103" s="62">
+      <c r="C113" s="33">
         <v>162</v>
       </c>
-      <c r="D103" s="22" t="s">
+      <c r="D113" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="E103" s="22" t="s">
+      <c r="E113" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="F103" s="22" t="s">
+      <c r="F113" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="G103" s="22" t="s">
+      <c r="G113" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="H103" s="22"/>
-      <c r="I103" s="22"/>
-      <c r="J103" s="22"/>
-      <c r="K103" s="22"/>
-      <c r="L103" s="22"/>
-      <c r="M103" s="22"/>
-    </row>
-    <row r="104" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="23" t="s">
+      <c r="H113" s="22"/>
+      <c r="I113" s="22"/>
+      <c r="J113" s="22"/>
+      <c r="K113" s="22"/>
+      <c r="L113" s="22"/>
+      <c r="M113" s="22"/>
+    </row>
+    <row r="114" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="B104" s="24" t="s">
+      <c r="B114" s="24" t="s">
         <v>199</v>
       </c>
-      <c r="C104" s="63">
+      <c r="C114" s="34">
         <v>162</v>
       </c>
-      <c r="D104" s="26" t="s">
+      <c r="D114" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="E104" s="26" t="s">
+      <c r="E114" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="F104" s="26" t="s">
+      <c r="F114" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="G104" s="26" t="s">
+      <c r="G114" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="H104" s="26"/>
-      <c r="I104" s="26"/>
-      <c r="J104" s="26"/>
-      <c r="K104" s="27"/>
-      <c r="L104" s="26"/>
-      <c r="M104" s="26"/>
-    </row>
-    <row r="105" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="106" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="30" t="s">
+      <c r="H114" s="26"/>
+      <c r="I114" s="26"/>
+      <c r="J114" s="26"/>
+      <c r="K114" s="27"/>
+      <c r="L114" s="26"/>
+      <c r="M114" s="26"/>
+    </row>
+    <row r="115" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="116" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="38" t="s">
         <v>149</v>
       </c>
-      <c r="B106" s="30"/>
-      <c r="C106" s="30"/>
-      <c r="D106" s="30"/>
-      <c r="E106" s="30"/>
-      <c r="F106" s="30"/>
-      <c r="G106" s="30"/>
-      <c r="H106" s="30"/>
-      <c r="I106" s="30"/>
-      <c r="J106" s="30"/>
-      <c r="K106" s="30"/>
-      <c r="L106" s="30"/>
-      <c r="M106" s="30"/>
-    </row>
-    <row r="107" spans="1:13" s="3" customFormat="1" ht="36.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="15"/>
-      <c r="B107" s="45" t="s">
+      <c r="B116" s="38"/>
+      <c r="C116" s="38"/>
+      <c r="D116" s="38"/>
+      <c r="E116" s="38"/>
+      <c r="F116" s="38"/>
+      <c r="G116" s="38"/>
+      <c r="H116" s="38"/>
+      <c r="I116" s="38"/>
+      <c r="J116" s="38"/>
+      <c r="K116" s="38"/>
+      <c r="L116" s="38"/>
+      <c r="M116" s="38"/>
+    </row>
+    <row r="117" spans="1:13" s="3" customFormat="1" ht="36.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="15"/>
+      <c r="B117" s="53" t="s">
         <v>237</v>
       </c>
-      <c r="C107" s="45"/>
-      <c r="D107" s="45"/>
-      <c r="E107" s="45"/>
-      <c r="F107" s="45"/>
-      <c r="G107" s="45"/>
-      <c r="H107" s="45"/>
-      <c r="I107" s="45"/>
-      <c r="J107" s="45"/>
-      <c r="K107" s="45"/>
-      <c r="L107" s="45"/>
-      <c r="M107" s="45"/>
-    </row>
-    <row r="108" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="8" t="s">
+      <c r="C117" s="53"/>
+      <c r="D117" s="53"/>
+      <c r="E117" s="53"/>
+      <c r="F117" s="53"/>
+      <c r="G117" s="53"/>
+      <c r="H117" s="53"/>
+      <c r="I117" s="53"/>
+      <c r="J117" s="53"/>
+      <c r="K117" s="53"/>
+      <c r="L117" s="53"/>
+      <c r="M117" s="53"/>
+    </row>
+    <row r="118" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B108" s="8" t="s">
+      <c r="B118" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="C108" s="8" t="s">
+      <c r="C118" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="D108" s="8" t="s">
+      <c r="D118" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="E108" s="8" t="s">
+      <c r="E118" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="F108" s="8" t="s">
+      <c r="F118" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="G108" s="8"/>
-      <c r="H108" s="8"/>
-      <c r="I108" s="8"/>
-      <c r="J108" s="8"/>
-      <c r="K108" s="8"/>
-      <c r="L108" s="8"/>
-      <c r="M108" s="8"/>
-    </row>
-    <row r="109" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="19" t="s">
+      <c r="G118" s="8"/>
+      <c r="H118" s="8"/>
+      <c r="I118" s="8"/>
+      <c r="J118" s="8"/>
+      <c r="K118" s="8"/>
+      <c r="L118" s="8"/>
+      <c r="M118" s="8"/>
+    </row>
+    <row r="119" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="B109" s="20" t="s">
+      <c r="B119" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="C109" s="21" t="s">
+      <c r="C119" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="D109" s="28" t="s">
+      <c r="D119" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="E109" s="22" t="s">
+      <c r="E119" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="F109" s="28" t="s">
+      <c r="F119" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="G109" s="22"/>
-      <c r="H109" s="22"/>
-      <c r="I109" s="22"/>
-      <c r="J109" s="22"/>
-      <c r="K109" s="22"/>
-      <c r="L109" s="22"/>
-      <c r="M109" s="22"/>
-    </row>
-    <row r="110" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="23" t="s">
+      <c r="G119" s="22"/>
+      <c r="H119" s="22"/>
+      <c r="I119" s="22"/>
+      <c r="J119" s="22"/>
+      <c r="K119" s="22"/>
+      <c r="L119" s="22"/>
+      <c r="M119" s="22"/>
+    </row>
+    <row r="120" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="B110" s="24" t="s">
+      <c r="B120" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="C110" s="25" t="s">
+      <c r="C120" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="D110" s="29" t="s">
+      <c r="D120" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="E110" s="26" t="s">
+      <c r="E120" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="F110" s="29" t="s">
+      <c r="F120" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="G110" s="26"/>
-      <c r="H110" s="26"/>
-      <c r="I110" s="26"/>
-      <c r="J110" s="26"/>
-      <c r="K110" s="27"/>
-      <c r="L110" s="26"/>
-      <c r="M110" s="26"/>
-    </row>
-    <row r="111" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="19" t="s">
+      <c r="G120" s="26"/>
+      <c r="H120" s="26"/>
+      <c r="I120" s="26"/>
+      <c r="J120" s="26"/>
+      <c r="K120" s="27"/>
+      <c r="L120" s="26"/>
+      <c r="M120" s="26"/>
+    </row>
+    <row r="121" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="B111" s="20" t="s">
+      <c r="B121" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="C111" s="21" t="s">
+      <c r="C121" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D111" s="28"/>
-      <c r="E111" s="22" t="s">
+      <c r="D121" s="28"/>
+      <c r="E121" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="F111" s="28" t="s">
+      <c r="F121" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="G111" s="22"/>
-      <c r="H111" s="22"/>
-      <c r="I111" s="22"/>
-      <c r="J111" s="22"/>
-      <c r="K111" s="22"/>
-      <c r="L111" s="22"/>
-      <c r="M111" s="22"/>
-    </row>
-    <row r="112" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="113" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="30" t="s">
-        <v>151</v>
-      </c>
-      <c r="B113" s="30"/>
-      <c r="C113" s="30"/>
-      <c r="D113" s="30"/>
-      <c r="E113" s="30"/>
-      <c r="F113" s="30"/>
-      <c r="G113" s="30"/>
-      <c r="H113" s="30"/>
-      <c r="I113" s="30"/>
-      <c r="J113" s="30"/>
-      <c r="K113" s="30"/>
-      <c r="L113" s="30"/>
-      <c r="M113" s="30"/>
-    </row>
-    <row r="114" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B114" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="C114" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="D114" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="E114" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F114" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="G114" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="H114" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="I114" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="J114" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="K114" s="8"/>
-      <c r="L114" s="8"/>
-      <c r="M114" s="8"/>
-    </row>
-    <row r="115" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="B115" s="20" t="s">
-        <v>198</v>
-      </c>
-      <c r="C115" s="62">
-        <v>514</v>
-      </c>
-      <c r="D115" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="E115" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="F115" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="G115" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="H115" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="I115" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="J115" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="K115" s="22"/>
-      <c r="L115" s="22"/>
-      <c r="M115" s="22"/>
-    </row>
-    <row r="116" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="117" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="30" t="s">
-        <v>159</v>
-      </c>
-      <c r="B117" s="30"/>
-      <c r="C117" s="30"/>
-      <c r="D117" s="30"/>
-      <c r="E117" s="30"/>
-      <c r="F117" s="30"/>
-      <c r="G117" s="30"/>
-      <c r="H117" s="30"/>
-      <c r="I117" s="30"/>
-      <c r="J117" s="30"/>
-      <c r="K117" s="30"/>
-      <c r="L117" s="30"/>
-      <c r="M117" s="30"/>
-    </row>
-    <row r="118" spans="1:13" ht="63.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="18"/>
-      <c r="B118" s="55" t="s">
-        <v>241</v>
-      </c>
-      <c r="C118" s="55"/>
-      <c r="D118" s="55"/>
-      <c r="E118" s="55"/>
-      <c r="F118" s="55"/>
-      <c r="G118" s="55"/>
-      <c r="H118" s="55"/>
-      <c r="I118" s="55"/>
-      <c r="J118" s="55"/>
-      <c r="K118" s="55"/>
-      <c r="L118" s="55"/>
-      <c r="M118" s="55"/>
-    </row>
-    <row r="119" spans="1:13" s="4" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B119" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="C119" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="D119" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="E119" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="F119" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="G119" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="H119" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="I119" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="J119" s="8"/>
-      <c r="K119" s="8"/>
-      <c r="L119" s="8"/>
-      <c r="M119" s="8"/>
-    </row>
-    <row r="120" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="B120" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="C120" s="21" t="s">
-        <v>200</v>
-      </c>
-      <c r="D120" s="62">
-        <v>1812</v>
-      </c>
-      <c r="E120" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="F120" s="22" t="s">
-        <v>160</v>
-      </c>
-      <c r="G120" s="62">
-        <v>5</v>
-      </c>
-      <c r="H120" s="62">
-        <v>5</v>
-      </c>
-      <c r="I120" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="J120" s="22"/>
-      <c r="K120" s="22"/>
-      <c r="L120" s="22"/>
-      <c r="M120" s="22"/>
-    </row>
-    <row r="121" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="B121" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="C121" s="25" t="s">
-        <v>201</v>
-      </c>
-      <c r="D121" s="63">
-        <v>1812</v>
-      </c>
-      <c r="E121" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="F121" s="26" t="s">
-        <v>160</v>
-      </c>
-      <c r="G121" s="63">
-        <v>5</v>
-      </c>
-      <c r="H121" s="63">
-        <v>5</v>
-      </c>
-      <c r="I121" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="J121" s="26"/>
-      <c r="K121" s="27"/>
-      <c r="L121" s="26"/>
-      <c r="M121" s="26"/>
+      <c r="G121" s="22"/>
+      <c r="H121" s="22"/>
+      <c r="I121" s="22"/>
+      <c r="J121" s="22"/>
+      <c r="K121" s="22"/>
+      <c r="L121" s="22"/>
+      <c r="M121" s="22"/>
     </row>
     <row r="122" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="123" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="30" t="s">
+      <c r="A123" s="38" t="s">
+        <v>151</v>
+      </c>
+      <c r="B123" s="38"/>
+      <c r="C123" s="38"/>
+      <c r="D123" s="38"/>
+      <c r="E123" s="38"/>
+      <c r="F123" s="38"/>
+      <c r="G123" s="38"/>
+      <c r="H123" s="38"/>
+      <c r="I123" s="38"/>
+      <c r="J123" s="38"/>
+      <c r="K123" s="38"/>
+      <c r="L123" s="38"/>
+      <c r="M123" s="38"/>
+    </row>
+    <row r="124" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B124" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="C124" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D124" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="E124" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F124" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="G124" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="H124" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="I124" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="J124" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="K124" s="8"/>
+      <c r="L124" s="8"/>
+      <c r="M124" s="8"/>
+    </row>
+    <row r="125" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B125" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="C125" s="33">
+        <v>514</v>
+      </c>
+      <c r="D125" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="E125" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="F125" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="G125" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="H125" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="I125" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="J125" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="K125" s="22"/>
+      <c r="L125" s="22"/>
+      <c r="M125" s="22"/>
+    </row>
+    <row r="126" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="127" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="38" t="s">
+        <v>159</v>
+      </c>
+      <c r="B127" s="38"/>
+      <c r="C127" s="38"/>
+      <c r="D127" s="38"/>
+      <c r="E127" s="38"/>
+      <c r="F127" s="38"/>
+      <c r="G127" s="38"/>
+      <c r="H127" s="38"/>
+      <c r="I127" s="38"/>
+      <c r="J127" s="38"/>
+      <c r="K127" s="38"/>
+      <c r="L127" s="38"/>
+      <c r="M127" s="38"/>
+    </row>
+    <row r="128" spans="1:13" ht="63.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A128" s="18"/>
+      <c r="B128" s="65" t="s">
+        <v>241</v>
+      </c>
+      <c r="C128" s="65"/>
+      <c r="D128" s="65"/>
+      <c r="E128" s="65"/>
+      <c r="F128" s="65"/>
+      <c r="G128" s="65"/>
+      <c r="H128" s="65"/>
+      <c r="I128" s="65"/>
+      <c r="J128" s="65"/>
+      <c r="K128" s="65"/>
+      <c r="L128" s="65"/>
+      <c r="M128" s="65"/>
+    </row>
+    <row r="129" spans="1:13" s="4" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A129" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B129" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="C129" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="D129" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="E129" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="F129" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="G129" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="H129" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="I129" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="J129" s="8"/>
+      <c r="K129" s="8"/>
+      <c r="L129" s="8"/>
+      <c r="M129" s="8"/>
+    </row>
+    <row r="130" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A130" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B130" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C130" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="D130" s="33">
+        <v>1812</v>
+      </c>
+      <c r="E130" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="F130" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="G130" s="33">
+        <v>5</v>
+      </c>
+      <c r="H130" s="33">
+        <v>5</v>
+      </c>
+      <c r="I130" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="J130" s="22"/>
+      <c r="K130" s="22"/>
+      <c r="L130" s="22"/>
+      <c r="M130" s="22"/>
+    </row>
+    <row r="131" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A131" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="B131" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="C131" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="D131" s="34">
+        <v>1812</v>
+      </c>
+      <c r="E131" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="F131" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="G131" s="34">
+        <v>5</v>
+      </c>
+      <c r="H131" s="34">
+        <v>5</v>
+      </c>
+      <c r="I131" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="J131" s="26"/>
+      <c r="K131" s="27"/>
+      <c r="L131" s="26"/>
+      <c r="M131" s="26"/>
+    </row>
+    <row r="132" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="133" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="38" t="s">
         <v>172</v>
       </c>
-      <c r="B123" s="30"/>
-      <c r="C123" s="30"/>
-      <c r="D123" s="30"/>
-      <c r="E123" s="30"/>
-      <c r="F123" s="30"/>
-      <c r="G123" s="30"/>
-      <c r="H123" s="30"/>
-      <c r="I123" s="30"/>
-      <c r="J123" s="30"/>
-      <c r="K123" s="30"/>
-      <c r="L123" s="30"/>
-      <c r="M123" s="30"/>
-    </row>
-    <row r="124" spans="1:13" ht="69.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="18"/>
-      <c r="B124" s="55" t="s">
+      <c r="B133" s="38"/>
+      <c r="C133" s="38"/>
+      <c r="D133" s="38"/>
+      <c r="E133" s="38"/>
+      <c r="F133" s="38"/>
+      <c r="G133" s="38"/>
+      <c r="H133" s="38"/>
+      <c r="I133" s="38"/>
+      <c r="J133" s="38"/>
+      <c r="K133" s="38"/>
+      <c r="L133" s="38"/>
+      <c r="M133" s="38"/>
+    </row>
+    <row r="134" spans="1:13" ht="69.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A134" s="18"/>
+      <c r="B134" s="65" t="s">
         <v>242</v>
       </c>
-      <c r="C124" s="55"/>
-      <c r="D124" s="55"/>
-      <c r="E124" s="55"/>
-      <c r="F124" s="55"/>
-      <c r="G124" s="55"/>
-      <c r="H124" s="55"/>
-      <c r="I124" s="55"/>
-      <c r="J124" s="55"/>
-      <c r="K124" s="55"/>
-      <c r="L124" s="55"/>
-      <c r="M124" s="55"/>
-    </row>
-    <row r="125" spans="1:13" s="4" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="10" t="s">
+      <c r="C134" s="65"/>
+      <c r="D134" s="65"/>
+      <c r="E134" s="65"/>
+      <c r="F134" s="65"/>
+      <c r="G134" s="65"/>
+      <c r="H134" s="65"/>
+      <c r="I134" s="65"/>
+      <c r="J134" s="65"/>
+      <c r="K134" s="65"/>
+      <c r="L134" s="65"/>
+      <c r="M134" s="65"/>
+    </row>
+    <row r="135" spans="1:13" s="4" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A135" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B125" s="10" t="s">
+      <c r="B135" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="C125" s="10" t="s">
+      <c r="C135" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="D125" s="10" t="s">
+      <c r="D135" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="E125" s="10" t="s">
+      <c r="E135" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="F125" s="10" t="s">
+      <c r="F135" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="G125" s="10" t="s">
+      <c r="G135" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="H125" s="10" t="s">
+      <c r="H135" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="I125" s="10" t="s">
+      <c r="I135" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="J125" s="10"/>
-      <c r="K125" s="10"/>
-      <c r="L125" s="10"/>
-      <c r="M125" s="10"/>
-    </row>
-    <row r="126" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="19" t="s">
+      <c r="J135" s="10"/>
+      <c r="K135" s="10"/>
+      <c r="L135" s="10"/>
+      <c r="M135" s="10"/>
+    </row>
+    <row r="136" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A136" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="B126" s="20" t="s">
+      <c r="B136" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="C126" s="21" t="s">
+      <c r="C136" s="21" t="s">
         <v>200</v>
       </c>
-      <c r="D126" s="62">
+      <c r="D136" s="33">
         <v>49</v>
       </c>
-      <c r="E126" s="28" t="s">
+      <c r="E136" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="F126" s="22" t="s">
+      <c r="F136" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="G126" s="62">
+      <c r="G136" s="33">
         <v>5</v>
       </c>
-      <c r="H126" s="62">
+      <c r="H136" s="33">
         <v>5</v>
       </c>
-      <c r="I126" s="22" t="s">
+      <c r="I136" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="J126" s="22"/>
-      <c r="K126" s="22"/>
-      <c r="L126" s="22"/>
-      <c r="M126" s="22"/>
-    </row>
-    <row r="127" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="23" t="s">
+      <c r="J136" s="22"/>
+      <c r="K136" s="22"/>
+      <c r="L136" s="22"/>
+      <c r="M136" s="22"/>
+    </row>
+    <row r="137" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A137" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="B127" s="24" t="s">
+      <c r="B137" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="C127" s="25" t="s">
+      <c r="C137" s="25" t="s">
         <v>201</v>
       </c>
-      <c r="D127" s="63">
+      <c r="D137" s="34">
         <v>49</v>
       </c>
-      <c r="E127" s="29" t="s">
+      <c r="E137" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="F127" s="26" t="s">
+      <c r="F137" s="26" t="s">
         <v>160</v>
       </c>
-      <c r="G127" s="63">
+      <c r="G137" s="34">
         <v>5</v>
       </c>
-      <c r="H127" s="63">
+      <c r="H137" s="34">
         <v>5</v>
       </c>
-      <c r="I127" s="26" t="s">
+      <c r="I137" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="J127" s="26"/>
-      <c r="K127" s="27"/>
-      <c r="L127" s="26"/>
-      <c r="M127" s="26"/>
-    </row>
-    <row r="129" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="56" t="s">
+      <c r="J137" s="26"/>
+      <c r="K137" s="27"/>
+      <c r="L137" s="26"/>
+      <c r="M137" s="26"/>
+    </row>
+    <row r="139" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A139" s="66" t="s">
         <v>239</v>
       </c>
-      <c r="B129" s="56"/>
-      <c r="C129" s="56"/>
-      <c r="D129" s="56"/>
-      <c r="E129" s="56"/>
-      <c r="F129" s="56"/>
-      <c r="G129" s="56"/>
-      <c r="H129" s="56"/>
-      <c r="I129" s="56"/>
-      <c r="J129" s="56"/>
-      <c r="K129" s="56"/>
-      <c r="L129" s="56"/>
-      <c r="M129" s="56"/>
-    </row>
-    <row r="130" spans="1:13" s="3" customFormat="1" ht="51.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="18"/>
-      <c r="B130" s="55" t="s">
+      <c r="B139" s="66"/>
+      <c r="C139" s="66"/>
+      <c r="D139" s="66"/>
+      <c r="E139" s="66"/>
+      <c r="F139" s="66"/>
+      <c r="G139" s="66"/>
+      <c r="H139" s="66"/>
+      <c r="I139" s="66"/>
+      <c r="J139" s="66"/>
+      <c r="K139" s="66"/>
+      <c r="L139" s="66"/>
+      <c r="M139" s="66"/>
+    </row>
+    <row r="140" spans="1:13" s="3" customFormat="1" ht="51.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A140" s="18"/>
+      <c r="B140" s="65" t="s">
         <v>240</v>
       </c>
-      <c r="C130" s="55"/>
-      <c r="D130" s="55"/>
-      <c r="E130" s="55"/>
-      <c r="F130" s="55"/>
-      <c r="G130" s="55"/>
-      <c r="H130" s="55"/>
-      <c r="I130" s="55"/>
-      <c r="J130" s="55"/>
-      <c r="K130" s="55"/>
-      <c r="L130" s="55"/>
-      <c r="M130" s="55"/>
-    </row>
-    <row r="131" spans="1:13" s="4" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A131" s="8" t="s">
+      <c r="C140" s="65"/>
+      <c r="D140" s="65"/>
+      <c r="E140" s="65"/>
+      <c r="F140" s="65"/>
+      <c r="G140" s="65"/>
+      <c r="H140" s="65"/>
+      <c r="I140" s="65"/>
+      <c r="J140" s="65"/>
+      <c r="K140" s="65"/>
+      <c r="L140" s="65"/>
+      <c r="M140" s="65"/>
+    </row>
+    <row r="141" spans="1:13" s="4" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A141" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B131" s="8" t="s">
+      <c r="B141" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C131" s="8" t="s">
+      <c r="C141" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D131" s="8" t="s">
+      <c r="D141" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="E131" s="8"/>
-      <c r="F131" s="8"/>
-      <c r="G131" s="8"/>
-      <c r="H131" s="8"/>
-      <c r="I131" s="8"/>
-      <c r="J131" s="8"/>
-      <c r="K131" s="8"/>
-      <c r="L131" s="8"/>
-      <c r="M131" s="8"/>
-    </row>
-    <row r="132" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="19" t="s">
+      <c r="E141" s="8"/>
+      <c r="F141" s="8"/>
+      <c r="G141" s="8"/>
+      <c r="H141" s="8"/>
+      <c r="I141" s="8"/>
+      <c r="J141" s="8"/>
+      <c r="K141" s="8"/>
+      <c r="L141" s="8"/>
+      <c r="M141" s="8"/>
+    </row>
+    <row r="142" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A142" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="B132" s="20" t="s">
+      <c r="B142" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="C132" s="21" t="s">
+      <c r="C142" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="D132" s="22" t="s">
+      <c r="D142" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="E132" s="22"/>
-      <c r="F132" s="22"/>
-      <c r="G132" s="22"/>
-      <c r="H132" s="22"/>
-      <c r="I132" s="22"/>
-      <c r="J132" s="22"/>
-      <c r="K132" s="22"/>
-      <c r="L132" s="22"/>
-      <c r="M132" s="22"/>
-    </row>
-    <row r="133" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="23" t="s">
+      <c r="E142" s="22"/>
+      <c r="F142" s="22"/>
+      <c r="G142" s="22"/>
+      <c r="H142" s="22"/>
+      <c r="I142" s="22"/>
+      <c r="J142" s="22"/>
+      <c r="K142" s="22"/>
+      <c r="L142" s="22"/>
+      <c r="M142" s="22"/>
+    </row>
+    <row r="143" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A143" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="B133" s="24" t="s">
+      <c r="B143" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="C133" s="25"/>
-      <c r="D133" s="26" t="s">
+      <c r="C143" s="25"/>
+      <c r="D143" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="E133" s="26"/>
-      <c r="F133" s="26"/>
-      <c r="G133" s="26"/>
-      <c r="H133" s="26"/>
-      <c r="I133" s="26"/>
-      <c r="J133" s="26"/>
-      <c r="K133" s="27"/>
-      <c r="L133" s="26"/>
-      <c r="M133" s="26"/>
+      <c r="E143" s="26"/>
+      <c r="F143" s="26"/>
+      <c r="G143" s="26"/>
+      <c r="H143" s="26"/>
+      <c r="I143" s="26"/>
+      <c r="J143" s="26"/>
+      <c r="K143" s="27"/>
+      <c r="L143" s="26"/>
+      <c r="M143" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="54">
-    <mergeCell ref="B107:M107"/>
-    <mergeCell ref="B118:M118"/>
-    <mergeCell ref="B130:M130"/>
-    <mergeCell ref="B124:M124"/>
+  <mergeCells count="56">
+    <mergeCell ref="B117:M117"/>
+    <mergeCell ref="B128:M128"/>
+    <mergeCell ref="B140:M140"/>
+    <mergeCell ref="B134:M134"/>
+    <mergeCell ref="A133:M133"/>
     <mergeCell ref="A123:M123"/>
-    <mergeCell ref="A113:M113"/>
-    <mergeCell ref="A117:M117"/>
-    <mergeCell ref="A129:M129"/>
-    <mergeCell ref="B55:M55"/>
+    <mergeCell ref="A127:M127"/>
+    <mergeCell ref="A139:M139"/>
     <mergeCell ref="B65:M65"/>
+    <mergeCell ref="B75:M75"/>
+    <mergeCell ref="A80:M80"/>
+    <mergeCell ref="B81:M81"/>
+    <mergeCell ref="B105:M105"/>
+    <mergeCell ref="A104:M104"/>
+    <mergeCell ref="A74:M74"/>
     <mergeCell ref="A70:M70"/>
-    <mergeCell ref="B71:M71"/>
-    <mergeCell ref="B95:M95"/>
-    <mergeCell ref="A94:M94"/>
-    <mergeCell ref="A64:M64"/>
-    <mergeCell ref="A60:M60"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="D91:E91"/>
     <mergeCell ref="B91:C91"/>
     <mergeCell ref="B92:C92"/>
-    <mergeCell ref="I72:J72"/>
-    <mergeCell ref="I73:J73"/>
-    <mergeCell ref="A90:M90"/>
+    <mergeCell ref="B101:C101"/>
+    <mergeCell ref="B102:C102"/>
+    <mergeCell ref="I82:J82"/>
+    <mergeCell ref="I83:J83"/>
+    <mergeCell ref="A100:M100"/>
     <mergeCell ref="N7:P7"/>
     <mergeCell ref="N8:P8"/>
     <mergeCell ref="A10:M10"/>
     <mergeCell ref="B6:M6"/>
     <mergeCell ref="A5:M5"/>
     <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A39:M39"/>
-    <mergeCell ref="A50:M50"/>
-    <mergeCell ref="A54:M54"/>
+    <mergeCell ref="A49:M49"/>
+    <mergeCell ref="A60:M60"/>
+    <mergeCell ref="A64:M64"/>
+    <mergeCell ref="A38:M38"/>
+    <mergeCell ref="B11:M11"/>
+    <mergeCell ref="B50:M50"/>
+    <mergeCell ref="B39:M39"/>
     <mergeCell ref="A28:M28"/>
-    <mergeCell ref="B11:M11"/>
-    <mergeCell ref="B40:M40"/>
     <mergeCell ref="B29:M29"/>
-    <mergeCell ref="A100:M100"/>
-    <mergeCell ref="A106:M106"/>
-    <mergeCell ref="D91:F91"/>
-    <mergeCell ref="C97:E97"/>
-    <mergeCell ref="C96:E96"/>
-    <mergeCell ref="C98:E98"/>
-    <mergeCell ref="B101:M101"/>
-    <mergeCell ref="A75:M75"/>
-    <mergeCell ref="A80:M80"/>
+    <mergeCell ref="A110:M110"/>
+    <mergeCell ref="A116:M116"/>
+    <mergeCell ref="D101:F101"/>
+    <mergeCell ref="C107:E107"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C108:E108"/>
+    <mergeCell ref="B111:M111"/>
     <mergeCell ref="A85:M85"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="G72:H72"/>
-    <mergeCell ref="G73:H73"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="E72:F72"/>
-    <mergeCell ref="E73:F73"/>
+    <mergeCell ref="A90:M90"/>
+    <mergeCell ref="A95:M95"/>
+    <mergeCell ref="B93:C93"/>
+    <mergeCell ref="G82:H82"/>
+    <mergeCell ref="G83:H83"/>
+    <mergeCell ref="D92:E92"/>
+    <mergeCell ref="D93:E93"/>
+    <mergeCell ref="E82:F82"/>
+    <mergeCell ref="E83:F83"/>
   </mergeCells>
-  <dataValidations count="59">
+  <conditionalFormatting sqref="F31:P31">
+    <cfRule type="expression" dxfId="11" priority="8">
+      <formula>A31="9504"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J31:P31">
+    <cfRule type="expression" dxfId="10" priority="7">
+      <formula>B31="9508"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F32:P32">
+    <cfRule type="expression" dxfId="9" priority="4">
+      <formula>F32="9504"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q31">
+    <cfRule type="expression" dxfId="8" priority="3">
+      <formula>L31="9504"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q31">
+    <cfRule type="expression" dxfId="7" priority="2">
+      <formula>I31="9508"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q32">
+    <cfRule type="expression" dxfId="6" priority="1">
+      <formula>Q32="9504"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="61">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"inband_vlan"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E13:E26" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"unspecified,remote-leaf-wan"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G31:G37 G13:G26" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G41:G47 G13:G26" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>switch_role</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H31:H37 H13:H26" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H41:H47 H13:H26" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>INDIRECT(G13)</formula1>
     </dataValidation>
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Inband VLAN" error="VLAN must be between 5 and 3097" sqref="B3" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>5</formula1>
       <formula2>3097</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Node ID" error="Valid Node ID is between 101 and 4000" sqref="D31:E37 C57:C58 D13:D26" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Node ID" error="Valid Node ID is between 101 and 4000" sqref="D41:E47 C67:C68 D13:D26" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>101</formula1>
       <formula2>4000</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A13:A26" xr:uid="{00000000-0002-0000-0000-000006000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A13:A26 A33:A36" xr:uid="{00000000-0002-0000-0000-000006000000}">
       <formula1>"switch"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A42:A48" xr:uid="{00000000-0002-0000-0000-000007000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A52:A58" xr:uid="{00000000-0002-0000-0000-000007000000}">
       <formula1>"apic_inb"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A52" xr:uid="{00000000-0002-0000-0000-000008000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A62" xr:uid="{00000000-0002-0000-0000-000008000000}">
       <formula1>"bgp_as"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BGP ASN" error="BGP ASN Must be between 1 and 4294967295" sqref="B52" xr:uid="{00000000-0002-0000-0000-000009000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BGP ASN" error="BGP ASN Must be between 1 and 4294967295" sqref="B62" xr:uid="{00000000-0002-0000-0000-000009000000}">
       <formula1>1</formula1>
       <formula2>4294967295</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Pod ID" error="Pod Id must be between 1 and 12!" sqref="D42:D48 F31:F37 F13:F26" xr:uid="{00000000-0002-0000-0000-00000A000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Pod ID" error="Pod Id must be between 1 and 12!" sqref="D52:D58 F41:F47 F13:F26" xr:uid="{00000000-0002-0000-0000-00000A000000}">
       <formula1>1</formula1>
       <formula2>12</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="APIC Node ID" error="APIC Node ID must be between 1 and 7" sqref="C42:C48" xr:uid="{00000000-0002-0000-0000-00000B000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="APIC Node ID" error="APIC Node ID must be between 1 and 7" sqref="C52:C58" xr:uid="{00000000-0002-0000-0000-00000B000000}">
       <formula1>1</formula1>
       <formula2>7</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A57:A58" xr:uid="{00000000-0002-0000-0000-00000C000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A67:A68" xr:uid="{00000000-0002-0000-0000-00000C000000}">
       <formula1>"bgp_rr"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B62 D77:D78 D87:D88 G103:G104 D115 I120:I121 I126:I127 D73 F8" xr:uid="{00000000-0002-0000-0000-00000D000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B72 D87:D88 D97:D98 G113:G114 D125 I130:I131 I136:I137 D83 F8" xr:uid="{00000000-0002-0000-0000-00000D000000}">
       <formula1>"inband,oob"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A62" xr:uid="{00000000-0002-0000-0000-00000E000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A72" xr:uid="{00000000-0002-0000-0000-00000E000000}">
       <formula1>"dns_mgmt"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A67:A68" xr:uid="{00000000-0002-0000-0000-00000F000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A77:A78" xr:uid="{00000000-0002-0000-0000-00000F000000}">
       <formula1>"dns"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C67:C68 D82:D83" xr:uid="{00000000-0002-0000-0000-000010000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C77:C78 D92:D93" xr:uid="{00000000-0002-0000-0000-000010000000}">
       <formula1>"no,yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A73" xr:uid="{00000000-0002-0000-0000-000011000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A83" xr:uid="{00000000-0002-0000-0000-000011000000}">
       <formula1>"smartcallhome"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C77:C78" xr:uid="{00000000-0002-0000-0000-000012000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C87:C88" xr:uid="{00000000-0002-0000-0000-000012000000}">
       <formula1>"false,true"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A82:A83" xr:uid="{00000000-0002-0000-0000-000013000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A92:A93" xr:uid="{00000000-0002-0000-0000-000013000000}">
       <formula1>"search_domain"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A77:A78" xr:uid="{00000000-0002-0000-0000-000014000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A87:A88" xr:uid="{00000000-0002-0000-0000-000014000000}">
       <formula1>"ntp"</formula1>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Community String" error="The SNMP Community can be 1 to 32 characters and contain letters, numbers, and [.\-]. No other special characters" sqref="B97:B98" xr:uid="{00000000-0002-0000-0000-000015000000}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Community String" error="The SNMP Community can be 1 to 32 characters and contain letters, numbers, and [.\-]. No other special characters" sqref="B107:B108" xr:uid="{00000000-0002-0000-0000-000015000000}">
       <formula1>1</formula1>
       <formula2>32</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A92" xr:uid="{00000000-0002-0000-0000-000016000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A102" xr:uid="{00000000-0002-0000-0000-000016000000}">
       <formula1>"snmp_info"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A97:A98" xr:uid="{00000000-0002-0000-0000-000017000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A107:A108" xr:uid="{00000000-0002-0000-0000-000017000000}">
       <formula1>"snmp_comm"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C109:C111" xr:uid="{00000000-0002-0000-0000-000018000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C119:C121" xr:uid="{00000000-0002-0000-0000-000018000000}">
       <formula1>"aes-128,des,none"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E109:E111" xr:uid="{00000000-0002-0000-0000-000019000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E119:E121" xr:uid="{00000000-0002-0000-0000-000019000000}">
       <formula1>"md5,sha1"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D103:D104" xr:uid="{00000000-0002-0000-0000-00001A000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D113:D114" xr:uid="{00000000-0002-0000-0000-00001A000000}">
       <formula1>"v1,v2c,v3"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A109:A111" xr:uid="{00000000-0002-0000-0000-00001B000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A119:A121" xr:uid="{00000000-0002-0000-0000-00001B000000}">
       <formula1>"snmp_user"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E115 H115" xr:uid="{00000000-0002-0000-0000-00001C000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E125 H125" xr:uid="{00000000-0002-0000-0000-00001C000000}">
       <formula1>"emergencies,alerts,critical,errors,warnings,notifications,information,debugging"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F115" xr:uid="{00000000-0002-0000-0000-00001D000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F125" xr:uid="{00000000-0002-0000-0000-00001D000000}">
       <formula1>"local0,local1,local2,local3,local4,local5,local6,local7"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G115 I115" xr:uid="{00000000-0002-0000-0000-00001E000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G125 I125" xr:uid="{00000000-0002-0000-0000-00001E000000}">
       <formula1>"enabled,disabled"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J115" xr:uid="{00000000-0002-0000-0000-00001F000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J125" xr:uid="{00000000-0002-0000-0000-00001F000000}">
       <formula1>"emergencies,alerts,critical"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A115" xr:uid="{00000000-0002-0000-0000-000020000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A125" xr:uid="{00000000-0002-0000-0000-000020000000}">
       <formula1>"syslog"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F120:F121 F126:F127" xr:uid="{00000000-0002-0000-0000-000021000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F130:F131 F136:F137" xr:uid="{00000000-0002-0000-0000-000021000000}">
       <formula1>"chap,mschap,pap"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="RADIUS Timeout" error="Timeout should be between 5 and 60 and be a Factor of 5.  Default is 5" sqref="G120:G121" xr:uid="{00000000-0002-0000-0000-000022000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="RADIUS Timeout" error="Timeout should be between 5 and 60 and be a Factor of 5.  Default is 5" sqref="G130:G131" xr:uid="{00000000-0002-0000-0000-000022000000}">
       <formula1>5</formula1>
       <formula2>60</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="RADIUS Retry" error="Retry should be a number between 1 and 5.  Default is 1" sqref="H120:H121" xr:uid="{00000000-0002-0000-0000-000023000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="RADIUS Retry" error="Retry should be a number between 1 and 5.  Default is 1" sqref="H130:H131" xr:uid="{00000000-0002-0000-0000-000023000000}">
       <formula1>1</formula1>
       <formula2>5</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="TACACS Timeout" error="Timeout should be between 5 and 60 and be a Factor of 5.  Default is 5" sqref="G126:G127" xr:uid="{00000000-0002-0000-0000-000024000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="TACACS Timeout" error="Timeout should be between 5 and 60 and be a Factor of 5.  Default is 5" sqref="G136:G137" xr:uid="{00000000-0002-0000-0000-000024000000}">
       <formula1>5</formula1>
       <formula2>60</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="TACACS Retry" error="Retry should be a number between 1 and 5.  Default is 1" sqref="H126:H127" xr:uid="{00000000-0002-0000-0000-000025000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="TACACS Retry" error="Retry should be a number between 1 and 5.  Default is 1" sqref="H136:H137" xr:uid="{00000000-0002-0000-0000-000025000000}">
       <formula1>1</formula1>
       <formula2>5</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Syslog Port" error="Valid Port Range is between 1 and 65535.  Default is 514" sqref="C115" xr:uid="{00000000-0002-0000-0000-000026000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Syslog Port" error="Valid Port Range is between 1 and 65535.  Default is 514" sqref="C125" xr:uid="{00000000-0002-0000-0000-000026000000}">
       <formula1>1</formula1>
       <formula2>65535</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="RADIUS Port" error="Valid Port Range is between 1 and 65535. Default is 1812" sqref="D120:D121" xr:uid="{00000000-0002-0000-0000-000027000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="RADIUS Port" error="Valid Port Range is between 1 and 65535. Default is 1812" sqref="D130:D131" xr:uid="{00000000-0002-0000-0000-000027000000}">
       <formula1>1</formula1>
       <formula2>65535</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="TACACS Port" error="Valid Port Range is between 1 and 65535. Default is 49" sqref="D126:D127" xr:uid="{00000000-0002-0000-0000-000028000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="TACACS Port" error="Valid Port Range is between 1 and 65535. Default is 49" sqref="D136:D137" xr:uid="{00000000-0002-0000-0000-000028000000}">
       <formula1>1</formula1>
       <formula2>65535</formula2>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Login Domain" error="Maximum length is 10 Alpha Numberic Characters or an underscore &quot;_&quot;.  But it must not begin with a underscore &quot;_&quot;." sqref="B126:B127" xr:uid="{00000000-0002-0000-0000-000029000000}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Login Domain" error="Maximum length is 10 Alpha Numberic Characters or an underscore &quot;_&quot;.  But it must not begin with a underscore &quot;_&quot;." sqref="B136:B137" xr:uid="{00000000-0002-0000-0000-000029000000}">
       <formula1>1</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A126:A127" xr:uid="{00000000-0002-0000-0000-00002A000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A136:A137" xr:uid="{00000000-0002-0000-0000-00002A000000}">
       <formula1>"tacacs"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A120:A121" xr:uid="{00000000-0002-0000-0000-00002B000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A130:A131" xr:uid="{00000000-0002-0000-0000-00002B000000}">
       <formula1>"radius"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SNMP Trap Port" error="Valid Port Range is between 1 and 65535.  Default is 162" sqref="C103:C104" xr:uid="{00000000-0002-0000-0000-00002C000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SNMP Trap Port" error="Valid Port Range is between 1 and 65535.  Default is 162" sqref="C113:C114" xr:uid="{00000000-0002-0000-0000-00002C000000}">
       <formula1>1</formula1>
       <formula2>65535</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A103:A104" xr:uid="{00000000-0002-0000-0000-00002D000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A113:A114" xr:uid="{00000000-0002-0000-0000-00002D000000}">
       <formula1>"snmp_trap"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SMTP Port" error="Valid Port Range is between 1 and 65535.  Default is 25" sqref="B73" xr:uid="{00000000-0002-0000-0000-00002E000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SMTP Port" error="Valid Port Range is between 1 and 65535.  Default is 25" sqref="B83" xr:uid="{00000000-0002-0000-0000-00002E000000}">
       <formula1>1</formula1>
       <formula2>65535</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Login Domain Type" error="The Login Domain Type can be [local|ldap|radius|tacacs|rsa|saml].  SAML is not supported for Console Authentication" sqref="D132:D133" xr:uid="{00000000-0002-0000-0000-00002F000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Login Domain Type" error="The Login Domain Type can be [local|ldap|radius|tacacs|rsa|saml].  SAML is not supported for Console Authentication" sqref="D142:D143" xr:uid="{00000000-0002-0000-0000-00002F000000}">
       <formula1>"local,ldap,radius,tacacs,rsa,saml"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B132:B133" xr:uid="{00000000-0002-0000-0000-000030000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B142:B143" xr:uid="{00000000-0002-0000-0000-000030000000}">
       <formula1>"console,default"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A132:A133" xr:uid="{00000000-0002-0000-0000-000031000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A142:A143" xr:uid="{00000000-0002-0000-0000-000031000000}">
       <formula1>"realm"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A31:A37" xr:uid="{A2F55667-432D-4009-90B0-3CBF96713B99}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A41:A47" xr:uid="{A2F55667-432D-4009-90B0-3CBF96713B99}">
       <formula1>"vpc_pair"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="VPC ID" error="The VPC ID must be a number between 1 and 1000" sqref="B31:B37" xr:uid="{2DB049D3-4D1F-4770-AA8C-B1564D6B004B}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="VPC ID" error="The VPC ID must be a number between 1 and 1000" sqref="B41:B47" xr:uid="{2DB049D3-4D1F-4770-AA8C-B1564D6B004B}">
       <formula1>1</formula1>
       <formula2>1000</formula2>
     </dataValidation>
@@ -5302,11 +5752,17 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J8" xr:uid="{EF451635-7AEA-41B7-80CF-916EDF399679}">
       <formula1>"password,ssh-key"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C31:Q32" xr:uid="{B9E1CD60-47CE-4C78-A5CF-1D8D26E4840D}">
+      <formula1>spine_modules</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A31:A32" xr:uid="{25454335-E68C-443E-9D9A-B6A17CD777C9}">
+      <formula1>spine_type</formula1>
+    </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E73" r:id="rId1" xr:uid="{47B0C783-B08F-4E70-8365-F66BC2D1DC4E}"/>
-    <hyperlink ref="G73" r:id="rId2" xr:uid="{ECB49B35-5BD8-4A7F-88FF-240597E5B135}"/>
-    <hyperlink ref="I73" r:id="rId3" xr:uid="{F5D689CB-3F4A-4EED-ADA0-F02A0EBD47A7}"/>
+    <hyperlink ref="E83" r:id="rId1" xr:uid="{47B0C783-B08F-4E70-8365-F66BC2D1DC4E}"/>
+    <hyperlink ref="G83" r:id="rId2" xr:uid="{ECB49B35-5BD8-4A7F-88FF-240597E5B135}"/>
+    <hyperlink ref="I83" r:id="rId3" xr:uid="{F5D689CB-3F4A-4EED-ADA0-F02A0EBD47A7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
@@ -5315,10 +5771,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5326,10 +5782,13 @@
     <col min="1" max="1" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="15" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>104</v>
       </c>
@@ -5339,8 +5798,14 @@
       <c r="C1" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="E1" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -5350,8 +5815,14 @@
       <c r="C2" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E2" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -5361,24 +5832,39 @@
       <c r="C3" s="1" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E3" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>88</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E4" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>89</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F5" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>90</v>
       </c>
@@ -5386,7 +5872,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>91</v>
       </c>
@@ -5394,7 +5880,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>92</v>
       </c>
@@ -5402,7 +5888,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>93</v>
       </c>
@@ -5410,7 +5896,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>94</v>
       </c>
@@ -5418,7 +5904,7 @@
         <v>9504</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>95</v>
       </c>
@@ -5426,7 +5912,7 @@
         <v>9508</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>96</v>
       </c>
@@ -5434,22 +5920,22 @@
         <v>9516</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>100</v>
       </c>

</xml_diff>